<commit_message>
soft constraints implemented testing needed
</commit_message>
<xml_diff>
--- a/src/FSEI_Mosta_EDT.xlsx
+++ b/src/FSEI_Mosta_EDT.xlsx
@@ -720,10 +720,14 @@
           <t>ANA2, TD/ G1, B1, Mme Bouabdelli</t>
         </is>
       </c>
-      <c r="E8" s="17" t="n"/>
+      <c r="E8" s="17" t="inlineStr">
+        <is>
+          <t>ANA2, TD/ G2, B1, Mme Bouabdelli</t>
+        </is>
+      </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G1, B4, Mme Diala.H</t>
+          <t>ALG2, TD/ G1, B2, Mme Diala.H</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
@@ -733,7 +737,7 @@
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G1, B3, DJAHAFI</t>
+          <t>ASD2, TD/ G2, B2, HABIB ZAHMANI M</t>
         </is>
       </c>
     </row>
@@ -743,23 +747,27 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G2, B4, Mme Diala.H</t>
-        </is>
-      </c>
-      <c r="E9" s="27" t="n"/>
+          <t>ANA2, TD/ G3, B2, Mlle FERRAOUN A.</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="inlineStr">
+        <is>
+          <t>ANA2, TD/ G4, B2, Mlle FERRAOUN A.</t>
+        </is>
+      </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G2, B1, Mme Bouabdelli</t>
+          <t>ALG2, TD/ G6, B3, Mme SAIDANI</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G2, C1, DJAHAFI</t>
+          <t>ALG2, TD/ G2, B1, Mme Diala.H</t>
         </is>
       </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G2, B2, HABIB ZAHMANI M</t>
+          <t>ALG2, TD/ G3, B1, Mme Diala.H</t>
         </is>
       </c>
     </row>
@@ -769,23 +777,27 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G3, B2, Mlle FERRAOUN A.</t>
-        </is>
-      </c>
-      <c r="E10" s="27" t="n"/>
+          <t>ANA2, TD/ G5, B3, M. Kaid</t>
+        </is>
+      </c>
+      <c r="E10" s="27" t="inlineStr">
+        <is>
+          <t>ANA2, TD/ G6, B3, M. Kaid</t>
+        </is>
+      </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G3, C2, MOUMEN</t>
+          <t>ANA2, TD/ G7, B1, M. Kaid</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G3, B2, Mme Diala.H</t>
+          <t>ALG2, TD/ G7, B2, Mme SAIDANI</t>
         </is>
       </c>
       <c r="H10" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G3, A1, MOUMEN</t>
+          <t>ASD2, TD/ G4, B3, BENAMEUR</t>
         </is>
       </c>
     </row>
@@ -793,105 +805,41 @@
       <c r="A11" s="30" t="n"/>
       <c r="B11" s="31" t="n"/>
       <c r="C11" s="31" t="n"/>
-      <c r="D11" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G4, C2, BENAMEUR</t>
-        </is>
-      </c>
+      <c r="D11" s="27" t="n"/>
       <c r="E11" s="27" t="n"/>
-      <c r="F11" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G4, B2, Mlle FERRAOUN A.</t>
-        </is>
-      </c>
-      <c r="G11" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G4, C2, HAMAMI</t>
-        </is>
-      </c>
-      <c r="H11" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G4, B1, Mme Diala.H</t>
-        </is>
-      </c>
+      <c r="F11" s="27" t="n"/>
+      <c r="G11" s="27" t="n"/>
+      <c r="H11" s="27" t="n"/>
     </row>
     <row r="12" ht="21.75" customHeight="1" s="24">
       <c r="A12" s="30" t="n"/>
       <c r="B12" s="31" t="n"/>
       <c r="C12" s="31" t="n"/>
-      <c r="D12" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G5, B3, M. Kaid</t>
-        </is>
-      </c>
+      <c r="D12" s="27" t="n"/>
       <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G5, S12, BENAMEUR</t>
-        </is>
-      </c>
-      <c r="G12" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G5, S12, M. Benzidane</t>
-        </is>
-      </c>
-      <c r="H12" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G5, A2, BENAMEUR</t>
-        </is>
-      </c>
+      <c r="F12" s="27" t="n"/>
+      <c r="G12" s="27" t="n"/>
+      <c r="H12" s="27" t="n"/>
     </row>
     <row r="13" ht="21.75" customHeight="1" s="24">
       <c r="A13" s="30" t="n"/>
       <c r="B13" s="31" t="n"/>
       <c r="C13" s="31" t="n"/>
-      <c r="D13" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G6, C1, Mme SAIDANI</t>
-        </is>
-      </c>
+      <c r="D13" s="27" t="n"/>
       <c r="E13" s="27" t="n"/>
-      <c r="F13" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G6, B3, M. Kaid</t>
-        </is>
-      </c>
-      <c r="G13" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G6, B4, BENAMEUR</t>
-        </is>
-      </c>
-      <c r="H13" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G6, B4, HAMAMI</t>
-        </is>
-      </c>
+      <c r="F13" s="27" t="n"/>
+      <c r="G13" s="27" t="n"/>
+      <c r="H13" s="27" t="n"/>
     </row>
     <row r="14" ht="21.75" customHeight="1" s="24">
       <c r="A14" s="30" t="n"/>
       <c r="B14" s="31" t="n"/>
       <c r="C14" s="31" t="n"/>
-      <c r="D14" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G7, S12, BENSALLOUA</t>
-        </is>
-      </c>
+      <c r="D14" s="27" t="n"/>
       <c r="E14" s="27" t="n"/>
-      <c r="F14" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G7, C1, Mme SAIDANI</t>
-        </is>
-      </c>
-      <c r="G14" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G7, B1, M. Kaid</t>
-        </is>
-      </c>
-      <c r="H14" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G7, A3, BENSALLOUA</t>
-        </is>
-      </c>
+      <c r="F14" s="27" t="n"/>
+      <c r="G14" s="27" t="n"/>
+      <c r="H14" s="27" t="n"/>
     </row>
     <row r="15" ht="21.75" customHeight="1" s="24">
       <c r="A15" s="30" t="n"/>
@@ -926,28 +874,32 @@
       </c>
       <c r="C17" s="17" t="inlineStr">
         <is>
+          <t>ASD2, TD/ G3, B2, MOUMEN</t>
+        </is>
+      </c>
+      <c r="D17" s="17" t="inlineStr">
+        <is>
+          <t>ALG2, TD/ G5, B1, Mme Diala.H</t>
+        </is>
+      </c>
+      <c r="E17" s="29" t="inlineStr">
+        <is>
+          <t>ASD2, COUR/ section 1, Amphi1, HENNI F</t>
+        </is>
+      </c>
+      <c r="F17" s="17" t="inlineStr">
+        <is>
           <t>ASD2, TP/ G1, A1, HABIB ZAHMANI M</t>
         </is>
       </c>
-      <c r="D17" s="29" t="inlineStr">
-        <is>
-          <t>ASD2, COUR/ section 1, Amphi1, HENNI F</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="n"/>
-      <c r="F17" s="17" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G1, B2, Mlle Zelmat Souhila</t>
-        </is>
-      </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G1, A1, Mlle Lakeb Ouda</t>
+          <t>ASD2, TP/ G2, A1, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G1, B1, Mekemmeche</t>
+          <t>SM2, TD/ G1, B1, DJAHAFI</t>
         </is>
       </c>
     </row>
@@ -956,24 +908,28 @@
       <c r="B18" s="31" t="n"/>
       <c r="C18" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G2, B4, Mlle Zelmat Souhila</t>
-        </is>
-      </c>
-      <c r="D18" s="31" t="n"/>
-      <c r="E18" s="27" t="n"/>
+          <t>ALG2, TD/ G4, B1, Mme Diala.H</t>
+        </is>
+      </c>
+      <c r="D18" s="27" t="inlineStr">
+        <is>
+          <t>ASD2, TD/ G6, B2, BENAMEUR</t>
+        </is>
+      </c>
+      <c r="E18" s="31" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G2, A1, HABIB ZAHMANI M</t>
+          <t>ASD2, TP/ G3, A2, MOUMEN</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G2, B2, Mekemmeche</t>
+          <t>ASD2, TP/ G5, A2, BENAMEUR</t>
         </is>
       </c>
       <c r="H18" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G2, A1, Mlle Lakeb Ouda</t>
+          <t>SM2, TD/ G4, B2, HAMAMI</t>
         </is>
       </c>
     </row>
@@ -982,116 +938,68 @@
       <c r="B19" s="31" t="n"/>
       <c r="C19" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G3, B2, DJAHAFI</t>
-        </is>
-      </c>
-      <c r="D19" s="31" t="n"/>
-      <c r="E19" s="27" t="n"/>
+          <t>ASD2, TD/ G5, B3, BENAMEUR</t>
+        </is>
+      </c>
+      <c r="D19" s="27" t="inlineStr">
+        <is>
+          <t>ASD2, TD/ G7, B3, BENSALLOUA</t>
+        </is>
+      </c>
+      <c r="E19" s="31" t="n"/>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G3, B3, Mlle Benaouad</t>
+          <t>ASD2, TP/ G4, A3, BENAMEUR</t>
         </is>
       </c>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G3, A2, Mlle Bouzid</t>
+          <t>ASD2, TP/ G7, A3, BENSALLOUA</t>
         </is>
       </c>
       <c r="H19" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G5, A2, Mlle Bouzid</t>
+          <t>ASD2, TP/ G6, A1, BENAMEUR</t>
         </is>
       </c>
     </row>
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
       <c r="B20" s="31" t="n"/>
-      <c r="C20" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G4, A2, BENAMEUR</t>
-        </is>
-      </c>
-      <c r="D20" s="31" t="n"/>
-      <c r="E20" s="27" t="n"/>
-      <c r="F20" s="27" t="inlineStr">
-        <is>
-          <t>OPM, TP/ G4, A3, Mlle Bouzid</t>
-        </is>
-      </c>
-      <c r="G20" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G4, B1, Mlle Benaouad</t>
-        </is>
-      </c>
-      <c r="H20" s="27" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G6, B2, Labdelli</t>
-        </is>
-      </c>
+      <c r="C20" s="27" t="n"/>
+      <c r="D20" s="27" t="n"/>
+      <c r="E20" s="31" t="n"/>
+      <c r="F20" s="27" t="n"/>
+      <c r="G20" s="27" t="n"/>
+      <c r="H20" s="27" t="n"/>
     </row>
     <row r="21" ht="21.75" customHeight="1" s="24">
       <c r="A21" s="30" t="n"/>
       <c r="B21" s="31" t="n"/>
-      <c r="C21" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G5, B1, Mme Diala.H</t>
-        </is>
-      </c>
-      <c r="D21" s="31" t="n"/>
-      <c r="E21" s="27" t="n"/>
-      <c r="F21" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G5, B1, HAMAMI</t>
-        </is>
-      </c>
-      <c r="G21" s="27" t="inlineStr">
-        <is>
-          <t>OPM, TP/ G6, A3, Mlle Hamou Maamar.M</t>
-        </is>
-      </c>
-      <c r="H21" s="27" t="inlineStr">
-        <is>
-          <t>OPM, TP/ G7, A3, Mlle Hamou Maamar.M</t>
-        </is>
-      </c>
+      <c r="C21" s="27" t="n"/>
+      <c r="D21" s="27" t="n"/>
+      <c r="E21" s="31" t="n"/>
+      <c r="F21" s="27" t="n"/>
+      <c r="G21" s="27" t="n"/>
+      <c r="H21" s="27" t="n"/>
     </row>
     <row r="22" ht="21.75" customHeight="1" s="24">
       <c r="A22" s="30" t="n"/>
       <c r="B22" s="31" t="n"/>
-      <c r="C22" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G6, C1, M. Benzidane</t>
-        </is>
-      </c>
-      <c r="D22" s="31" t="n"/>
-      <c r="E22" s="27" t="n"/>
-      <c r="F22" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G6, A2, BENAMEUR</t>
-        </is>
-      </c>
-      <c r="G22" s="27" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G7, B3, Labdelli</t>
-        </is>
-      </c>
+      <c r="C22" s="27" t="n"/>
+      <c r="D22" s="27" t="n"/>
+      <c r="E22" s="31" t="n"/>
+      <c r="F22" s="27" t="n"/>
+      <c r="G22" s="27" t="n"/>
       <c r="H22" s="27" t="n"/>
     </row>
     <row r="23" ht="21.75" customHeight="1" s="24">
       <c r="A23" s="30" t="n"/>
       <c r="B23" s="31" t="n"/>
-      <c r="C23" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G7, B3, HAMAMI</t>
-        </is>
-      </c>
-      <c r="D23" s="31" t="n"/>
-      <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G7, B4, Mme Kaisserli</t>
-        </is>
-      </c>
+      <c r="C23" s="27" t="n"/>
+      <c r="D23" s="27" t="n"/>
+      <c r="E23" s="31" t="n"/>
+      <c r="F23" s="27" t="n"/>
       <c r="G23" s="27" t="n"/>
       <c r="H23" s="27" t="n"/>
     </row>
@@ -1099,8 +1007,8 @@
       <c r="A24" s="30" t="n"/>
       <c r="B24" s="31" t="n"/>
       <c r="C24" s="27" t="n"/>
-      <c r="D24" s="31" t="n"/>
-      <c r="E24" s="27" t="n"/>
+      <c r="D24" s="27" t="n"/>
+      <c r="E24" s="31" t="n"/>
       <c r="F24" s="27" t="n"/>
       <c r="G24" s="27" t="n"/>
       <c r="H24" s="27" t="n"/>
@@ -1109,8 +1017,8 @@
       <c r="A25" s="32" t="n"/>
       <c r="B25" s="33" t="n"/>
       <c r="C25" s="16" t="n"/>
-      <c r="D25" s="33" t="n"/>
-      <c r="E25" s="16" t="n"/>
+      <c r="D25" s="16" t="n"/>
+      <c r="E25" s="33" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="16" t="n"/>
       <c r="H25" s="16" t="n"/>
@@ -1126,106 +1034,154 @@
           <t>SM2, COUR/ section 1, Amphi1, HASSAINE</t>
         </is>
       </c>
-      <c r="C26" s="29" t="inlineStr">
+      <c r="C26" s="17" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G1, B3, Mlle Zelmat Souhila</t>
+        </is>
+      </c>
+      <c r="D26" s="17" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G2, B3, Mlle Zelmat Souhila</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G3, B2, Mlle Benaouad</t>
+        </is>
+      </c>
+      <c r="F26" s="29" t="inlineStr">
         <is>
           <t>IPSD, COUR/ section 1, Amphi1, Mlle Dj. BENSIKADDOUR</t>
         </is>
       </c>
-      <c r="D26" s="17" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G3, B1, Mekemmeche</t>
-        </is>
-      </c>
-      <c r="E26" s="17" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G4, B1, Mekemmeche</t>
-        </is>
-      </c>
-      <c r="F26" s="17" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G5, B1, Mekemmeche</t>
-        </is>
-      </c>
-      <c r="G26" s="17" t="n"/>
-      <c r="H26" s="17" t="n"/>
+      <c r="G26" s="17" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G4, B1, Mlle Benaouad</t>
+        </is>
+      </c>
+      <c r="H26" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G1, A1, Mlle Lakeb Ouda</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
       <c r="B27" s="31" t="n"/>
-      <c r="C27" s="31" t="n"/>
-      <c r="D27" s="27" t="n"/>
-      <c r="E27" s="27" t="n"/>
-      <c r="F27" s="27" t="n"/>
-      <c r="G27" s="27" t="n"/>
-      <c r="H27" s="27" t="n"/>
+      <c r="C27" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G2, B1, DJAHAFI</t>
+        </is>
+      </c>
+      <c r="D27" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G3, B1, DJAHAFI</t>
+        </is>
+      </c>
+      <c r="E27" s="27" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G5, B3, M. Benzidane</t>
+        </is>
+      </c>
+      <c r="F27" s="31" t="n"/>
+      <c r="G27" s="27" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G6, B2, M. Benzidane</t>
+        </is>
+      </c>
+      <c r="H27" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G3, A2, Mlle Bouzid</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
       <c r="B28" s="31" t="n"/>
-      <c r="C28" s="31" t="n"/>
-      <c r="D28" s="27" t="n"/>
-      <c r="E28" s="27" t="n"/>
-      <c r="F28" s="27" t="n"/>
-      <c r="G28" s="27" t="n"/>
-      <c r="H28" s="27" t="n"/>
+      <c r="C28" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G5, B2, HAMAMI</t>
+        </is>
+      </c>
+      <c r="D28" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G6, B2, HAMAMI</t>
+        </is>
+      </c>
+      <c r="E28" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G7, B1, HAMAMI</t>
+        </is>
+      </c>
+      <c r="F28" s="31" t="n"/>
+      <c r="G28" s="27" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G7, B3, Mme Kaisserli</t>
+        </is>
+      </c>
+      <c r="H28" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G6, A3, Mlle Hamou Maamar.M</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
       <c r="B29" s="31" t="n"/>
-      <c r="C29" s="31" t="n"/>
+      <c r="C29" s="27" t="n"/>
       <c r="D29" s="27" t="n"/>
       <c r="E29" s="27" t="n"/>
-      <c r="F29" s="27" t="n"/>
+      <c r="F29" s="31" t="n"/>
       <c r="G29" s="27" t="n"/>
       <c r="H29" s="27" t="n"/>
     </row>
     <row r="30" ht="21.75" customHeight="1" s="24">
       <c r="A30" s="30" t="n"/>
       <c r="B30" s="31" t="n"/>
-      <c r="C30" s="31" t="n"/>
+      <c r="C30" s="27" t="n"/>
       <c r="D30" s="27" t="n"/>
       <c r="E30" s="27" t="n"/>
-      <c r="F30" s="27" t="n"/>
+      <c r="F30" s="31" t="n"/>
       <c r="G30" s="27" t="n"/>
       <c r="H30" s="27" t="n"/>
     </row>
     <row r="31" ht="21.75" customHeight="1" s="24">
       <c r="A31" s="30" t="n"/>
       <c r="B31" s="31" t="n"/>
-      <c r="C31" s="31" t="n"/>
+      <c r="C31" s="27" t="n"/>
       <c r="D31" s="27" t="n"/>
       <c r="E31" s="27" t="n"/>
-      <c r="F31" s="27" t="n"/>
+      <c r="F31" s="31" t="n"/>
       <c r="G31" s="27" t="n"/>
       <c r="H31" s="27" t="n"/>
     </row>
     <row r="32" ht="21.75" customHeight="1" s="24">
       <c r="A32" s="30" t="n"/>
       <c r="B32" s="31" t="n"/>
-      <c r="C32" s="31" t="n"/>
+      <c r="C32" s="27" t="n"/>
       <c r="D32" s="27" t="n"/>
       <c r="E32" s="27" t="n"/>
-      <c r="F32" s="27" t="n"/>
+      <c r="F32" s="31" t="n"/>
       <c r="G32" s="27" t="n"/>
       <c r="H32" s="27" t="n"/>
     </row>
     <row r="33" ht="21.75" customHeight="1" s="24">
       <c r="A33" s="30" t="n"/>
       <c r="B33" s="31" t="n"/>
-      <c r="C33" s="31" t="n"/>
+      <c r="C33" s="27" t="n"/>
       <c r="D33" s="27" t="n"/>
       <c r="E33" s="27" t="n"/>
-      <c r="F33" s="27" t="n"/>
+      <c r="F33" s="31" t="n"/>
       <c r="G33" s="27" t="n"/>
       <c r="H33" s="27" t="n"/>
     </row>
     <row r="34" ht="21.75" customHeight="1" s="24">
       <c r="A34" s="32" t="n"/>
       <c r="B34" s="33" t="n"/>
-      <c r="C34" s="33" t="n"/>
+      <c r="C34" s="16" t="n"/>
       <c r="D34" s="16" t="n"/>
       <c r="E34" s="16" t="n"/>
-      <c r="F34" s="16" t="n"/>
+      <c r="F34" s="33" t="n"/>
       <c r="G34" s="16" t="n"/>
       <c r="H34" s="16" t="n"/>
     </row>
@@ -1245,19 +1201,47 @@
           <t>OPM, COUR/ section 1, Amphi1, Mlle Ali Merina.H</t>
         </is>
       </c>
-      <c r="D35" s="17" t="n"/>
-      <c r="E35" s="17" t="n"/>
-      <c r="F35" s="17" t="n"/>
-      <c r="G35" s="17" t="n"/>
+      <c r="D35" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G2, A1, Mlle Lakeb Ouda</t>
+        </is>
+      </c>
+      <c r="E35" s="17" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G1, B1, Mekemmeche</t>
+        </is>
+      </c>
+      <c r="F35" s="17" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G2, B1, Mekemmeche</t>
+        </is>
+      </c>
+      <c r="G35" s="17" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G3, B1, Mekemmeche</t>
+        </is>
+      </c>
       <c r="H35" s="17" t="n"/>
     </row>
     <row r="36" ht="21.75" customHeight="1" s="24">
       <c r="A36" s="30" t="n"/>
       <c r="B36" s="31" t="n"/>
       <c r="C36" s="31" t="n"/>
-      <c r="D36" s="27" t="n"/>
-      <c r="E36" s="27" t="n"/>
-      <c r="F36" s="27" t="n"/>
+      <c r="D36" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G4, A2, Mlle Bouzid</t>
+        </is>
+      </c>
+      <c r="E36" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G5, A1, Mlle Bouzid</t>
+        </is>
+      </c>
+      <c r="F36" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G7, B2, Labdelli</t>
+        </is>
+      </c>
       <c r="G36" s="27" t="n"/>
       <c r="H36" s="27" t="n"/>
     </row>
@@ -1265,8 +1249,16 @@
       <c r="A37" s="30" t="n"/>
       <c r="B37" s="31" t="n"/>
       <c r="C37" s="31" t="n"/>
-      <c r="D37" s="27" t="n"/>
-      <c r="E37" s="27" t="n"/>
+      <c r="D37" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G7, A3, Mlle Hamou Maamar.M</t>
+        </is>
+      </c>
+      <c r="E37" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G6, B2, Labdelli</t>
+        </is>
+      </c>
       <c r="F37" s="27" t="n"/>
       <c r="G37" s="27" t="n"/>
       <c r="H37" s="27" t="n"/>
@@ -1342,8 +1334,16 @@
           <t>PHY2, COUR/ section 1, Amphi1, M. Benchehida</t>
         </is>
       </c>
-      <c r="C44" s="17" t="n"/>
-      <c r="D44" s="17" t="n"/>
+      <c r="C44" s="17" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G4, B1, Mekemmeche</t>
+        </is>
+      </c>
+      <c r="D44" s="17" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G5, B1, Mekemmeche</t>
+        </is>
+      </c>
       <c r="E44" s="17" t="n"/>
       <c r="F44" s="17" t="n"/>
       <c r="G44" s="17" t="n"/>
@@ -2412,9 +2412,9 @@
     <mergeCell ref="B8:B16"/>
     <mergeCell ref="C8:C16"/>
     <mergeCell ref="B17:B25"/>
-    <mergeCell ref="D17:D25"/>
+    <mergeCell ref="E17:E25"/>
     <mergeCell ref="B26:B34"/>
-    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="F26:F34"/>
     <mergeCell ref="B35:B43"/>
     <mergeCell ref="C35:C43"/>
     <mergeCell ref="B44:B52"/>
@@ -2552,19 +2552,23 @@
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>TG, TP/ G1, C3, Mr Ablaoui H.</t>
+          <t>Mod2, TD/ G1, S16, Mlle Bouzid Leila</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>PROGQUAD, TP/ G1, C3, M. AMIR A.</t>
-        </is>
-      </c>
-      <c r="G8" s="17" t="n"/>
+          <t>OAF 2, TD/ G1, S8, Mr S. M. Bahri</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>TCONTROL, TD/ G1, S9, Mr. BOUAGADA</t>
+        </is>
+      </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>Mod2, TD/ G1, Amphi4, Mlle Bouzid Leila</t>
+          <t>CFRAC, TD/ G1, S8, M. Zoubir DAHMANI</t>
         </is>
       </c>
     </row>
@@ -2661,28 +2665,24 @@
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>TCONTROL, COUR/ section 1, S13, Mr. BOUAGADA</t>
+          <t>TCONTROL, COUR/ section 1, C2, Mr. BOUAGADA</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>OAF 2, TD/ G1, S8, Mr S. M. Bahri</t>
+          <t>TG, TD/ G1, S16, Mr Ablaoui H.</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>TCONTROL, TD/ G1, S8, Mr. BOUAGADA</t>
-        </is>
-      </c>
-      <c r="G17" s="17" t="inlineStr">
-        <is>
-          <t>CFRAC, TD/ G1, S7, M. Zoubir DAHMANI</t>
-        </is>
-      </c>
+          <t>PROGQUAD, TD/ G1, S7, M. AMIR A.</t>
+        </is>
+      </c>
+      <c r="G17" s="17" t="n"/>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>TG, TD/ G1, S15, Mr Ablaoui H.</t>
+          <t>TG, TP/ G1, M3, Mr Ablaoui H.</t>
         </is>
       </c>
     </row>
@@ -2779,12 +2779,12 @@
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>TG, COUR/ section 1, B3, Mr Ablaoui H.</t>
+          <t>TG, COUR/ section 1, C2, Mr Ablaoui H.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>PROGQUAD, TD/ G1, B4, M. AMIR A.</t>
+          <t>PROGQUAD, TP/ G1, M1, M. AMIR A.</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
@@ -4203,13 +4203,21 @@
           <t>Chim2, COUR/ section 1, Amphi2, Belhachemi</t>
         </is>
       </c>
-      <c r="F8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>Maths2, TD/ G3, S16, Mme.Bechaoui</t>
+        </is>
+      </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>Info2, TP/ G1, M2, Adda</t>
-        </is>
-      </c>
-      <c r="H8" s="17" t="n"/>
+          <t>Chim2, TD/ G1, S16, Hamiani</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
+          <t>Chim2, TD/ G1, S2, Hamiani</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
@@ -4225,22 +4233,26 @@
       </c>
       <c r="D9" s="31" t="n"/>
       <c r="E9" s="31" t="n"/>
-      <c r="F9" s="27" t="n"/>
-      <c r="G9" s="27" t="n"/>
-      <c r="H9" s="27" t="n"/>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>Chim2, TD/ G4, S2, Belhachemi</t>
+        </is>
+      </c>
+      <c r="G9" s="27" t="inlineStr">
+        <is>
+          <t>Maths2, TD/ G2, S8, Mme.Bechaoui</t>
+        </is>
+      </c>
+      <c r="H9" s="27" t="inlineStr">
+        <is>
+          <t>Maths2, TD/ G2, S16, Mme.Bechaoui</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="21.75" customHeight="1" s="24">
       <c r="A10" s="30" t="n"/>
-      <c r="B10" s="27" t="inlineStr">
-        <is>
-          <t>Phys2, TD/ G3, S13, Benguettat</t>
-        </is>
-      </c>
-      <c r="C10" s="27" t="inlineStr">
-        <is>
-          <t>Phys2, TD/ G3, S13, Benguettat</t>
-        </is>
-      </c>
+      <c r="B10" s="27" t="n"/>
+      <c r="C10" s="27" t="n"/>
       <c r="D10" s="31" t="n"/>
       <c r="E10" s="31" t="n"/>
       <c r="F10" s="27" t="n"/>
@@ -4249,11 +4261,7 @@
     </row>
     <row r="11" ht="21.75" customHeight="1" s="24">
       <c r="A11" s="30" t="n"/>
-      <c r="B11" s="27" t="inlineStr">
-        <is>
-          <t>Info2, TP/ G4, A3, Adda</t>
-        </is>
-      </c>
+      <c r="B11" s="27" t="n"/>
       <c r="C11" s="27" t="n"/>
       <c r="D11" s="31" t="n"/>
       <c r="E11" s="31" t="n"/>
@@ -4319,33 +4327,37 @@
       </c>
       <c r="B17" s="17" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G1, C1, Hamiani</t>
+          <t>Maths2, TD/ G3, B4, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="C17" s="17" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G1, S15, Hamiani</t>
+          <t>Chim2, TD/ G3, S13, Belhachemi</t>
         </is>
       </c>
       <c r="D17" s="29" t="inlineStr">
         <is>
-          <t>Maths2, COUR/ section 1, Amphi3, Mme.Bechaoui</t>
+          <t>Maths2, COUR/ section 1, Amphi2, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="E17" s="29" t="inlineStr">
         <is>
-          <t>Chim2, COUR/ section 1, Amphi1, Belhachemi</t>
-        </is>
-      </c>
-      <c r="F17" s="17" t="n"/>
+          <t>Chim2, COUR/ section 1, Amphi2, Belhachemi</t>
+        </is>
+      </c>
+      <c r="F17" s="17" t="inlineStr">
+        <is>
+          <t>Phys2, TD/ G1, S11, Benguettat</t>
+        </is>
+      </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G1, S9, Benguettat</t>
+          <t>Phys2, TD/ G3, S13, Benguettat</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G1, S6, Benguettat</t>
+          <t>Phys2, TD/ G2, S14, Benguettat</t>
         </is>
       </c>
     </row>
@@ -4353,66 +4365,38 @@
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G2, B4, Mme.Bechaoui</t>
+          <t>Chim2, TD/ G4, C1, Belhachemi</t>
         </is>
       </c>
       <c r="C18" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G2, S14, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G4, S12, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="D18" s="31" t="n"/>
       <c r="E18" s="31" t="n"/>
-      <c r="F18" s="27" t="n"/>
-      <c r="G18" s="27" t="inlineStr">
-        <is>
-          <t>Maths2, TD/ G3, S11, Mme.Bechaoui</t>
-        </is>
-      </c>
-      <c r="H18" s="27" t="inlineStr">
-        <is>
-          <t>Maths2, TD/ G3, S4, Mme.Bechaoui</t>
-        </is>
-      </c>
+      <c r="F18" s="27" t="inlineStr">
+        <is>
+          <t>Info2, TP/ G2, M3, Adda</t>
+        </is>
+      </c>
+      <c r="G18" s="27" t="n"/>
+      <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
-      <c r="B19" s="27" t="inlineStr">
-        <is>
-          <t>Chim2, TD/ G3, C2, Belhachemi</t>
-        </is>
-      </c>
-      <c r="C19" s="27" t="inlineStr">
-        <is>
-          <t>Chim2, TD/ G3, S4, Belhachemi</t>
-        </is>
-      </c>
+      <c r="B19" s="27" t="n"/>
+      <c r="C19" s="27" t="n"/>
       <c r="D19" s="31" t="n"/>
       <c r="E19" s="31" t="n"/>
       <c r="F19" s="27" t="n"/>
-      <c r="G19" s="27" t="inlineStr">
-        <is>
-          <t>Chim2, TD/ G4, S10, Belhachemi</t>
-        </is>
-      </c>
-      <c r="H19" s="27" t="inlineStr">
-        <is>
-          <t>Chim2, TD/ G4, S5, Belhachemi</t>
-        </is>
-      </c>
+      <c r="G19" s="27" t="n"/>
+      <c r="H19" s="27" t="n"/>
     </row>
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
-      <c r="B20" s="27" t="inlineStr">
-        <is>
-          <t>Phys2, TD/ G4, S12, Benguettat</t>
-        </is>
-      </c>
-      <c r="C20" s="27" t="inlineStr">
-        <is>
-          <t>Phys2, TD/ G4, S5, Benguettat</t>
-        </is>
-      </c>
+      <c r="B20" s="27" t="n"/>
+      <c r="C20" s="27" t="n"/>
       <c r="D20" s="31" t="n"/>
       <c r="E20" s="31" t="n"/>
       <c r="F20" s="27" t="n"/>
@@ -4477,60 +4461,64 @@
       </c>
       <c r="B26" s="17" t="inlineStr">
         <is>
+          <t>Chim2, TD/ G3, C1, Belhachemi</t>
+        </is>
+      </c>
+      <c r="C26" s="29" t="inlineStr">
+        <is>
+          <t>Phys2, COUR/ section 1, Amphi4, Mr.Senouci</t>
+        </is>
+      </c>
+      <c r="D26" s="29" t="inlineStr">
+        <is>
+          <t>Phys2, COUR/ section 1, Amphi2, Mr.Senouci</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="inlineStr">
+        <is>
+          <t>Phys2, TD/ G1, S12, Benguettat</t>
+        </is>
+      </c>
+      <c r="F26" s="17" t="inlineStr">
+        <is>
           <t>Phys2, TD/ G2, C1, Benguettat</t>
         </is>
       </c>
-      <c r="C26" s="17" t="inlineStr">
-        <is>
-          <t>Phys2, TD/ G2, C1, Benguettat</t>
-        </is>
-      </c>
-      <c r="D26" s="29" t="inlineStr">
-        <is>
-          <t>Phys2, COUR/ section 1, Amphi2, Mr.Senouci</t>
-        </is>
-      </c>
-      <c r="E26" s="29" t="inlineStr">
-        <is>
-          <t>Phys2, COUR/ section 1, Amphi1, Mr.Senouci</t>
-        </is>
-      </c>
-      <c r="F26" s="17" t="n"/>
-      <c r="G26" s="17" t="n"/>
-      <c r="H26" s="17" t="inlineStr">
-        <is>
-          <t>Info2, TP/ G2, M3, Adda</t>
-        </is>
-      </c>
+      <c r="G26" s="17" t="inlineStr">
+        <is>
+          <t>Info2, TP/ G1, M2, Adda</t>
+        </is>
+      </c>
+      <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
       <c r="B27" s="27" t="inlineStr">
         <is>
+          <t>Maths2, TD/ G4, B4, Mme.Bechaoui</t>
+        </is>
+      </c>
+      <c r="C27" s="31" t="n"/>
+      <c r="D27" s="31" t="n"/>
+      <c r="E27" s="27" t="n"/>
+      <c r="F27" s="27" t="inlineStr">
+        <is>
           <t>Info2, TP/ G3, C3, Adda</t>
         </is>
       </c>
-      <c r="C27" s="27" t="inlineStr">
-        <is>
-          <t>Maths2, TD/ G4, B4, Mme.Bechaoui</t>
-        </is>
-      </c>
-      <c r="D27" s="31" t="n"/>
-      <c r="E27" s="31" t="n"/>
-      <c r="F27" s="27" t="n"/>
-      <c r="G27" s="27" t="n"/>
+      <c r="G27" s="27" t="inlineStr">
+        <is>
+          <t>Phys2, TD/ G3, S12, Benguettat</t>
+        </is>
+      </c>
       <c r="H27" s="27" t="n"/>
     </row>
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
-      <c r="B28" s="27" t="inlineStr">
-        <is>
-          <t>Maths2, TD/ G4, B4, Mme.Bechaoui</t>
-        </is>
-      </c>
-      <c r="C28" s="27" t="n"/>
+      <c r="B28" s="27" t="n"/>
+      <c r="C28" s="31" t="n"/>
       <c r="D28" s="31" t="n"/>
-      <c r="E28" s="31" t="n"/>
+      <c r="E28" s="27" t="n"/>
       <c r="F28" s="27" t="n"/>
       <c r="G28" s="27" t="n"/>
       <c r="H28" s="27" t="n"/>
@@ -4538,9 +4526,9 @@
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
       <c r="B29" s="27" t="n"/>
-      <c r="C29" s="27" t="n"/>
+      <c r="C29" s="31" t="n"/>
       <c r="D29" s="31" t="n"/>
-      <c r="E29" s="31" t="n"/>
+      <c r="E29" s="27" t="n"/>
       <c r="F29" s="27" t="n"/>
       <c r="G29" s="27" t="n"/>
       <c r="H29" s="27" t="n"/>
@@ -4548,9 +4536,9 @@
     <row r="30" ht="21.75" customHeight="1" s="24">
       <c r="A30" s="30" t="n"/>
       <c r="B30" s="27" t="n"/>
-      <c r="C30" s="27" t="n"/>
+      <c r="C30" s="31" t="n"/>
       <c r="D30" s="31" t="n"/>
-      <c r="E30" s="31" t="n"/>
+      <c r="E30" s="27" t="n"/>
       <c r="F30" s="27" t="n"/>
       <c r="G30" s="27" t="n"/>
       <c r="H30" s="27" t="n"/>
@@ -4558,9 +4546,9 @@
     <row r="31" ht="21.75" customHeight="1" s="24">
       <c r="A31" s="30" t="n"/>
       <c r="B31" s="27" t="n"/>
-      <c r="C31" s="27" t="n"/>
+      <c r="C31" s="31" t="n"/>
       <c r="D31" s="31" t="n"/>
-      <c r="E31" s="31" t="n"/>
+      <c r="E31" s="27" t="n"/>
       <c r="F31" s="27" t="n"/>
       <c r="G31" s="27" t="n"/>
       <c r="H31" s="27" t="n"/>
@@ -4568,9 +4556,9 @@
     <row r="32" ht="21.75" customHeight="1" s="24">
       <c r="A32" s="30" t="n"/>
       <c r="B32" s="27" t="n"/>
-      <c r="C32" s="27" t="n"/>
+      <c r="C32" s="31" t="n"/>
       <c r="D32" s="31" t="n"/>
-      <c r="E32" s="31" t="n"/>
+      <c r="E32" s="27" t="n"/>
       <c r="F32" s="27" t="n"/>
       <c r="G32" s="27" t="n"/>
       <c r="H32" s="27" t="n"/>
@@ -4578,9 +4566,9 @@
     <row r="33" ht="21.75" customHeight="1" s="24">
       <c r="A33" s="30" t="n"/>
       <c r="B33" s="27" t="n"/>
-      <c r="C33" s="27" t="n"/>
+      <c r="C33" s="31" t="n"/>
       <c r="D33" s="31" t="n"/>
-      <c r="E33" s="31" t="n"/>
+      <c r="E33" s="27" t="n"/>
       <c r="F33" s="27" t="n"/>
       <c r="G33" s="27" t="n"/>
       <c r="H33" s="27" t="n"/>
@@ -4588,9 +4576,9 @@
     <row r="34" ht="21.75" customHeight="1" s="24">
       <c r="A34" s="32" t="n"/>
       <c r="B34" s="16" t="n"/>
-      <c r="C34" s="16" t="n"/>
+      <c r="C34" s="33" t="n"/>
       <c r="D34" s="33" t="n"/>
-      <c r="E34" s="33" t="n"/>
+      <c r="E34" s="16" t="n"/>
       <c r="F34" s="16" t="n"/>
       <c r="G34" s="16" t="n"/>
       <c r="H34" s="16" t="n"/>
@@ -4611,9 +4599,17 @@
           <t>HisSci, COUR/ section 1, Amphi4, Benguettat</t>
         </is>
       </c>
-      <c r="D35" s="17" t="n"/>
+      <c r="D35" s="17" t="inlineStr">
+        <is>
+          <t>Phys2, TD/ G4, B2, Benguettat</t>
+        </is>
+      </c>
       <c r="E35" s="17" t="n"/>
-      <c r="F35" s="17" t="n"/>
+      <c r="F35" s="17" t="inlineStr">
+        <is>
+          <t>Info2, TP/ G4, M2, Adda</t>
+        </is>
+      </c>
       <c r="G35" s="17" t="n"/>
       <c r="H35" s="17" t="n"/>
     </row>
@@ -4703,7 +4699,11 @@
           <t>Jeudi</t>
         </is>
       </c>
-      <c r="B44" s="17" t="n"/>
+      <c r="B44" s="17" t="inlineStr">
+        <is>
+          <t>Phys2, TD/ G4, B2, Benguettat</t>
+        </is>
+      </c>
       <c r="C44" s="17" t="n"/>
       <c r="D44" s="17" t="n"/>
       <c r="E44" s="17" t="n"/>
@@ -5775,8 +5775,8 @@
     <mergeCell ref="E8:E16"/>
     <mergeCell ref="D17:D25"/>
     <mergeCell ref="E17:E25"/>
+    <mergeCell ref="C26:C34"/>
     <mergeCell ref="D26:D34"/>
-    <mergeCell ref="E26:E34"/>
     <mergeCell ref="B35:B43"/>
     <mergeCell ref="C35:C43"/>
   </mergeCells>
@@ -5903,23 +5903,35 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>Thdyna, COUR/ section 1, S14, Hentit H</t>
+          <t>Thdyna, COUR/ section 1, S13, Hentit H</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>Thdyna, COUR/ section 1, S14, Hentit H</t>
-        </is>
-      </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>Thdyna, TD/ G1, S13, Hentit H</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
-      <c r="H8" s="17" t="n"/>
+          <t>Thdyna, COUR/ section 1, S13, Hentit H</t>
+        </is>
+      </c>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>Thdyna, TD/ G1, S2, Hentit H</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>FVC, TD/ G1, S3, Latreuch</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>FVC, TD/ G1, S2, Latreuch</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
+          <t>MQ, TD/ G1, S3, Meghoufel</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
@@ -6009,33 +6021,33 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>FVC, COUR/ section 1, S13, Latreuch</t>
+          <t>FVC, COUR/ section 1, C2, Latreuch</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>FVC, COUR/ section 1, S6, Latreuch</t>
+          <t>FVC, COUR/ section 1, S14, Latreuch</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>Thdyna, TD/ G1, S16, Hentit H</t>
+          <t>Thdyna, TD/ G1, S2, Hentit H</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>FVC, TD/ G1, S16, Latreuch</t>
+          <t>MQ, TD/ G1, S10, Meghoufel</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>FVC, TD/ G1, S8, Latreuch</t>
+          <t>elecmag, TD/ G1, S14, Abbes</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>MQ, TD/ G1, S7, Meghoufel</t>
+          <t>elecmag, TD/ G1, S15, Abbes</t>
         </is>
       </c>
     </row>
@@ -6132,25 +6144,13 @@
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>MQ, COUR/ section 1, C2, Meghoufel</t>
-        </is>
-      </c>
-      <c r="D26" s="17" t="inlineStr">
-        <is>
-          <t>MQ, TD/ G1, C1, Meghoufel</t>
-        </is>
-      </c>
+          <t>MQ, COUR/ section 1, S12, Meghoufel</t>
+        </is>
+      </c>
+      <c r="D26" s="17" t="n"/>
       <c r="E26" s="17" t="n"/>
-      <c r="F26" s="17" t="inlineStr">
-        <is>
-          <t>elecmag, TD/ G1, B3, Abbes</t>
-        </is>
-      </c>
-      <c r="G26" s="17" t="inlineStr">
-        <is>
-          <t>elecmag, TD/ G1, B2, Abbes</t>
-        </is>
-      </c>
+      <c r="F26" s="17" t="n"/>
+      <c r="G26" s="17" t="n"/>
       <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
@@ -6343,12 +6343,12 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
+          <t>elecgen, COUR/ section 1, B3, Melati</t>
+        </is>
+      </c>
+      <c r="C44" s="29" t="inlineStr">
+        <is>
           <t>elecgen, COUR/ section 1, B2, Melati</t>
-        </is>
-      </c>
-      <c r="C44" s="29" t="inlineStr">
-        <is>
-          <t>elecgen, COUR/ section 1, B1, Melati</t>
         </is>
       </c>
       <c r="D44" s="17" t="n"/>
@@ -7551,23 +7551,35 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>PhysSol, COUR/ section 1, S15, Bouattou</t>
+          <t>PhysSol, COUR/ section 1, S14, Bouattou</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>PhysSol, COUR/ section 1, S15, Bouattou</t>
-        </is>
-      </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>PhysSol, TD/ G1, S14, Bouattou</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
-      <c r="H8" s="17" t="n"/>
+          <t>PhysSol, COUR/ section 1, S14, Bouattou</t>
+        </is>
+      </c>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>PhysSol, TD/ G1, S3, Bouattou</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>PhysNuc, TD/ G1, S1, Abbassa</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>PhysNuc, TD/ G1, S3, Abbassa</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
+          <t>TransCha, TD/ G1, S1, Boukra</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
@@ -7657,33 +7669,33 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>PhysNuc, COUR/ section 1, S14, Abbassa</t>
+          <t>PhysNuc, COUR/ section 1, S12, Abbassa</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>PhysNuc, COUR/ section 1, S7, Abbassa</t>
+          <t>PhysNuc, COUR/ section 1, S15, Abbassa</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>PhysSol, TD/ G1, S2, Bouattou</t>
+          <t>PhysSol, TD/ G1, S3, Bouattou</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>PhysNuc, TD/ G1, S2, Abbassa</t>
+          <t>TransCha, TD/ G1, S9, Boukra</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>PhysNuc, TD/ G1, S16, Abbassa</t>
+          <t>PhysAto, TD/ G1, S15, Beghdad</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>TransCha, TD/ G1, S11, Boukra</t>
+          <t>PhysAto, TD/ G1, S4, Beghdad</t>
         </is>
       </c>
     </row>
@@ -7780,25 +7792,13 @@
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>TransCha, COUR/ section 1, S12, Boukra</t>
-        </is>
-      </c>
-      <c r="D26" s="17" t="inlineStr">
-        <is>
-          <t>TransCha, TD/ G1, C2, Boukra</t>
-        </is>
-      </c>
+          <t>TransCha, COUR/ section 1, S13, Boukra</t>
+        </is>
+      </c>
+      <c r="D26" s="17" t="n"/>
       <c r="E26" s="17" t="n"/>
-      <c r="F26" s="17" t="inlineStr">
-        <is>
-          <t>PhysAto, TD/ G1, B4, Beghdad</t>
-        </is>
-      </c>
-      <c r="G26" s="17" t="inlineStr">
-        <is>
-          <t>PhysAto, TD/ G1, B3, Beghdad</t>
-        </is>
-      </c>
+      <c r="F26" s="17" t="n"/>
+      <c r="G26" s="17" t="n"/>
       <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
@@ -9197,29 +9197,53 @@
           <t>ChiOrg2, COUR/ section 1, S3, Kadi</t>
         </is>
       </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>ChiOrg2, TD/ G1, S15, Kadi</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
-      <c r="H8" s="17" t="n"/>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>ChiOrg2, TD/ G1, S1, Kadi</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>ThermoCin, TD/ G1, Amphi4, Belayachi</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>ChimAna, TD/ G1, S1, Bourada</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
+          <t>ChiQuan, TD/ G1, Amphi4, Boulenouar</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
       <c r="B9" s="31" t="n"/>
       <c r="C9" s="31" t="n"/>
-      <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>ThermoCin, TD/ G2, S4, Belayachi</t>
-        </is>
-      </c>
-      <c r="F9" s="27" t="n"/>
-      <c r="G9" s="27" t="n"/>
-      <c r="H9" s="27" t="n"/>
+      <c r="D9" s="27" t="inlineStr">
+        <is>
+          <t>ThermoCin, TD/ G2, Amphi3, Belayachi</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="n"/>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>ChiOrg2, TD/ G2, Amphi3, Kadi</t>
+        </is>
+      </c>
+      <c r="G9" s="27" t="inlineStr">
+        <is>
+          <t>ChiQuan, TD/ G2, Amphi3, Boulenouar</t>
+        </is>
+      </c>
+      <c r="H9" s="27" t="inlineStr">
+        <is>
+          <t>ChimAna, TD/ G2, Amphi3, Bourada</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="21.75" customHeight="1" s="24">
       <c r="A10" s="30" t="n"/>
@@ -9309,46 +9333,26 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>ThermoCin, TD/ G1, S1, Belayachi</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="n"/>
-      <c r="F17" s="17" t="inlineStr">
-        <is>
-          <t>ChimAna, TD/ G1, S3, Bourada</t>
-        </is>
-      </c>
-      <c r="G17" s="17" t="inlineStr">
-        <is>
-          <t>ChiQuan, TD/ G1, S3, Boulenouar</t>
-        </is>
-      </c>
-      <c r="H17" s="17" t="inlineStr">
-        <is>
-          <t>ChimInorg, TD/ G1, S10, Messaoudi</t>
-        </is>
-      </c>
+          <t>ChimInorg, TD/ G1, S1, Messaoudi</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="inlineStr">
+        <is>
+          <t>ChimInorg, TD/ G2, S15, Messaoudi</t>
+        </is>
+      </c>
+      <c r="F17" s="17" t="n"/>
+      <c r="G17" s="17" t="n"/>
+      <c r="H17" s="17" t="n"/>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="31" t="n"/>
       <c r="C18" s="31" t="n"/>
-      <c r="D18" s="27" t="inlineStr">
-        <is>
-          <t>ChiOrg2, TD/ G2, S3, Kadi</t>
-        </is>
-      </c>
+      <c r="D18" s="27" t="n"/>
       <c r="E18" s="27" t="n"/>
-      <c r="F18" s="27" t="inlineStr">
-        <is>
-          <t>ChiQuan, TD/ G2, S1, Boulenouar</t>
-        </is>
-      </c>
-      <c r="G18" s="27" t="inlineStr">
-        <is>
-          <t>ChimAna, TD/ G2, S2, Bourada</t>
-        </is>
-      </c>
+      <c r="F18" s="27" t="n"/>
+      <c r="G18" s="27" t="n"/>
       <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
@@ -9437,11 +9441,7 @@
           <t>ChiQuan, COUR/ section 1, S3, Benmalti</t>
         </is>
       </c>
-      <c r="D26" s="17" t="inlineStr">
-        <is>
-          <t>ChimInorg, TD/ G2, S12, Messaoudi</t>
-        </is>
-      </c>
+      <c r="D26" s="17" t="n"/>
       <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="17" t="n"/>
@@ -10848,14 +10848,22 @@
           <t>TS, COUR/ section 1, S1, Belhakem</t>
         </is>
       </c>
-      <c r="D8" s="17" t="n"/>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>TS, TD/ G1, Amphi4, Belhakem</t>
+        </is>
+      </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>TS, TD/ G1, S5, Belhakem</t>
+          <t>ElecChemi, TD/ G2, S6, Belayachi</t>
         </is>
       </c>
       <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>TS, TD/ G2, Amphi4, Belhakem</t>
+        </is>
+      </c>
       <c r="H8" s="17" t="n"/>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
@@ -10863,11 +10871,7 @@
       <c r="B9" s="31" t="n"/>
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>SpecMol, TD/ G2, S6, Belouatek</t>
-        </is>
-      </c>
+      <c r="E9" s="27" t="n"/>
       <c r="F9" s="27" t="n"/>
       <c r="G9" s="27" t="n"/>
       <c r="H9" s="27" t="n"/>
@@ -10960,22 +10964,18 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>TS, TD/ G2, Amphi4, Belhakem</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="inlineStr">
-        <is>
-          <t>SpecMol, TD/ G1, B2, Belouatek</t>
-        </is>
-      </c>
+          <t>ElecChemi, TD/ G1, Amphi3, Belayachi</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>ElecChemi, TD/ G1, Amphi3, Belayachi</t>
+          <t>SpecMol, TD/ G1, S8, Belouatek</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>CSC, TD/ G1, Amphi3, Bourahla</t>
+          <t>CSC, TD/ G1, S4, Bourahla</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -10984,18 +10984,18 @@
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="31" t="n"/>
       <c r="C18" s="31" t="n"/>
-      <c r="D18" s="27" t="n"/>
+      <c r="D18" s="27" t="inlineStr">
+        <is>
+          <t>SpecMol, TD/ G2, Amphi4, Belouatek</t>
+        </is>
+      </c>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>CSC, TD/ G2, Amphi4, Bourahla</t>
-        </is>
-      </c>
-      <c r="G18" s="27" t="inlineStr">
-        <is>
-          <t>ElecChemi, TD/ G2, S1, Belayachi</t>
-        </is>
-      </c>
+          <t>CSC, TD/ G2, S16, Bourahla</t>
+        </is>
+      </c>
+      <c r="G18" s="27" t="n"/>
       <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
@@ -12498,23 +12498,27 @@
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G1, S7, HAMAMI</t>
-        </is>
-      </c>
-      <c r="E8" s="17" t="n"/>
+          <t>ANA2, TD/ G2, B4, Mme Bendehmane H</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="inlineStr">
+        <is>
+          <t>ALG2, TD/ G1, C2, Mme SAIDANI</t>
+        </is>
+      </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G1, S5, BENSALLOUA</t>
+          <t>ASD2, TD/ G1, C2, BENSALLOUA</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G1, S13, Mme SAIDANI</t>
+          <t>ASD2, TD/ G2, C1, BENSALLOUA</t>
         </is>
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G1, C1, M. Kaid</t>
+          <t>ANA2, TD/ G1, B4, M. Kaid</t>
         </is>
       </c>
     </row>
@@ -12524,23 +12528,27 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G2, S13, Mme Bendehmane H</t>
-        </is>
-      </c>
-      <c r="E9" s="27" t="n"/>
+          <t>ANA2, TD/ G4, C1, Mme Ablaoui</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="inlineStr">
+        <is>
+          <t>ANA2, TD/ G3, B4, Mme Bendehmane H</t>
+        </is>
+      </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G2, S7, HAMAMI</t>
+          <t>ALG2, TD/ G3, C1, Mme TABHARIT</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G2, S15, BENSALLOUA</t>
+          <t>ALG2, TD/ G4, B4, Mme TABHARIT</t>
         </is>
       </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G2, C2, Mme SAIDANI</t>
+          <t>ASD2, TD/ G3, C2, BENSALLOUA</t>
         </is>
       </c>
     </row>
@@ -12550,23 +12558,27 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G3, S4, Mme TABHARIT</t>
-        </is>
-      </c>
-      <c r="E10" s="27" t="n"/>
+          <t>ANA2, TD/ G6, C2, M. Ould Ali M</t>
+        </is>
+      </c>
+      <c r="E10" s="27" t="inlineStr">
+        <is>
+          <t>ANA2, TD/ G7, C1, M. Ould Ali M</t>
+        </is>
+      </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G3, S13, Mme Bendehmane H</t>
+          <t>ANA2, TD/ G5, B4, Mme Ablaoui</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G3, S6, Mme Kaisserli</t>
+          <t>ASD2, TD/ G5, C2, KAID SLIMANE</t>
         </is>
       </c>
       <c r="H10" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G3, S15, Labdelli</t>
+          <t>ALG2, TD/ G5, C1, Mme TABHARIT</t>
         </is>
       </c>
     </row>
@@ -12574,105 +12586,41 @@
       <c r="A11" s="30" t="n"/>
       <c r="B11" s="31" t="n"/>
       <c r="C11" s="31" t="n"/>
-      <c r="D11" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G4, S14, Mme Ablaoui</t>
-        </is>
-      </c>
+      <c r="D11" s="27" t="n"/>
       <c r="E11" s="27" t="n"/>
-      <c r="F11" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G4, S4, Mme TABHARIT</t>
-        </is>
-      </c>
-      <c r="G11" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G4, S4, KAID SLIMANE</t>
-        </is>
-      </c>
-      <c r="H11" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G4, S14, Mme Kaisserli</t>
-        </is>
-      </c>
+      <c r="F11" s="27" t="n"/>
+      <c r="G11" s="27" t="n"/>
+      <c r="H11" s="27" t="n"/>
     </row>
     <row r="12" ht="21.75" customHeight="1" s="24">
       <c r="A12" s="30" t="n"/>
       <c r="B12" s="31" t="n"/>
       <c r="C12" s="31" t="n"/>
-      <c r="D12" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G5, S5, KAID SLIMANE</t>
-        </is>
-      </c>
+      <c r="D12" s="27" t="n"/>
       <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G5, S14, Mme Ablaoui</t>
-        </is>
-      </c>
-      <c r="G12" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G5, S14, Mme TABHARIT</t>
-        </is>
-      </c>
-      <c r="H12" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G5, S13, HASSAINE</t>
-        </is>
-      </c>
+      <c r="F12" s="27" t="n"/>
+      <c r="G12" s="27" t="n"/>
+      <c r="H12" s="27" t="n"/>
     </row>
     <row r="13" ht="21.75" customHeight="1" s="24">
       <c r="A13" s="30" t="n"/>
       <c r="B13" s="31" t="n"/>
       <c r="C13" s="31" t="n"/>
-      <c r="D13" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G6, S15, M. Ould Ali M</t>
-        </is>
-      </c>
+      <c r="D13" s="27" t="n"/>
       <c r="E13" s="27" t="n"/>
-      <c r="F13" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G6, S6, KAID SLIMANE</t>
-        </is>
-      </c>
-      <c r="G13" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G6, S5, HASSAINE</t>
-        </is>
-      </c>
-      <c r="H13" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G6, S12, Mme TABHARIT</t>
-        </is>
-      </c>
+      <c r="F13" s="27" t="n"/>
+      <c r="G13" s="27" t="n"/>
+      <c r="H13" s="27" t="n"/>
     </row>
     <row r="14" ht="21.75" customHeight="1" s="24">
       <c r="A14" s="30" t="n"/>
       <c r="B14" s="31" t="n"/>
       <c r="C14" s="31" t="n"/>
-      <c r="D14" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TD/ G7, S6, HENNI F</t>
-        </is>
-      </c>
+      <c r="D14" s="27" t="n"/>
       <c r="E14" s="27" t="n"/>
-      <c r="F14" s="27" t="inlineStr">
-        <is>
-          <t>ANA2, TD/ G7, S15, M. Ould Ali M</t>
-        </is>
-      </c>
-      <c r="G14" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G7, S7, Mlle Dj. BENSIKADDOUR</t>
-        </is>
-      </c>
-      <c r="H14" s="27" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G7, S4, M. Benchehida</t>
-        </is>
-      </c>
+      <c r="F14" s="27" t="n"/>
+      <c r="G14" s="27" t="n"/>
+      <c r="H14" s="27" t="n"/>
     </row>
     <row r="15" ht="21.75" customHeight="1" s="24">
       <c r="A15" s="30" t="n"/>
@@ -12712,23 +12660,27 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G1, B4, Mme Kaisserli</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="n"/>
+          <t>ALG2, TD/ G2, B4, Mme SAIDANI</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G1, B2, HAMAMI</t>
+        </is>
+      </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G1, S12, Labdelli</t>
+          <t>SM2, TD/ G2, B3, HAMAMI</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G1, A4, BENSALLOUA</t>
+          <t>IPSD, TD/ G1, B3, Mme Kaisserli</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G3, A4, BENSALLOUA</t>
+          <t>IPSD, TD/ G2, B4, Mme Kaisserli</t>
         </is>
       </c>
     </row>
@@ -12738,23 +12690,27 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G2, C2, Labdelli</t>
-        </is>
-      </c>
-      <c r="E18" s="27" t="n"/>
+          <t>ASD2, TD/ G4, C2, KAID SLIMANE</t>
+        </is>
+      </c>
+      <c r="E18" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G5, B3, HASSAINE</t>
+        </is>
+      </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G2, A4, BENSALLOUA</t>
+          <t>ASD2, TD/ G6, B1, KAID SLIMANE</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G2, C1, Mme Kaisserli</t>
+          <t>SM2, TD/ G3, B1, HAMAMI</t>
         </is>
       </c>
       <c r="H18" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G4, C4, Mlle Ali Merina.H</t>
+          <t>IPSD, TD/ G5, C1, M. Benyatou Kamel</t>
         </is>
       </c>
     </row>
@@ -12764,23 +12720,27 @@
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G3, B2, BENSALLOUA</t>
-        </is>
-      </c>
-      <c r="E19" s="27" t="n"/>
+          <t>ALG2, TD/ G6, C1, Mme TABHARIT</t>
+        </is>
+      </c>
+      <c r="E19" s="27" t="inlineStr">
+        <is>
+          <t>ALG2, TD/ G7, B1, Mme TABHARIT</t>
+        </is>
+      </c>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G3, C4, Mlle Hamou Maamar.M</t>
+          <t>ASD2, TD/ G7, B2, HENNI F</t>
         </is>
       </c>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G3, B4, HAMAMI</t>
+          <t>SM2, TD/ G6, B2, HASSAINE</t>
         </is>
       </c>
       <c r="H19" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G6, C3, KAID SLIMANE</t>
+          <t>SM2, TD/ G7, B3, HASSAINE</t>
         </is>
       </c>
     </row>
@@ -12788,88 +12748,40 @@
       <c r="A20" s="30" t="n"/>
       <c r="B20" s="31" t="n"/>
       <c r="C20" s="31" t="n"/>
-      <c r="D20" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G4, B3, HAMAMI</t>
-        </is>
-      </c>
+      <c r="D20" s="27" t="n"/>
       <c r="E20" s="27" t="n"/>
-      <c r="F20" s="27" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G4, S13, M. Benchehida</t>
-        </is>
-      </c>
-      <c r="G20" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G4, C3, KAID SLIMANE</t>
-        </is>
-      </c>
+      <c r="F20" s="27" t="n"/>
+      <c r="G20" s="27" t="n"/>
       <c r="H20" s="27" t="n"/>
     </row>
     <row r="21" ht="21.75" customHeight="1" s="24">
       <c r="A21" s="30" t="n"/>
       <c r="B21" s="31" t="n"/>
       <c r="C21" s="31" t="n"/>
-      <c r="D21" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G5, C1, M. Benyatou Kamel</t>
-        </is>
-      </c>
+      <c r="D21" s="27" t="n"/>
       <c r="E21" s="27" t="n"/>
-      <c r="F21" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G5, C3, KAID SLIMANE</t>
-        </is>
-      </c>
-      <c r="G21" s="27" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G5, C2, M. Benchehida</t>
-        </is>
-      </c>
+      <c r="F21" s="27" t="n"/>
+      <c r="G21" s="27" t="n"/>
       <c r="H21" s="27" t="n"/>
     </row>
     <row r="22" ht="21.75" customHeight="1" s="24">
       <c r="A22" s="30" t="n"/>
       <c r="B22" s="31" t="n"/>
       <c r="C22" s="31" t="n"/>
-      <c r="D22" s="27" t="inlineStr">
-        <is>
-          <t>PHY2, TD/ G6, S12, M. Benchehida</t>
-        </is>
-      </c>
+      <c r="D22" s="27" t="n"/>
       <c r="E22" s="27" t="n"/>
-      <c r="F22" s="27" t="inlineStr">
-        <is>
-          <t>IPSD, TD/ G6, C2, M. Benyatou Kamel</t>
-        </is>
-      </c>
-      <c r="G22" s="27" t="inlineStr">
-        <is>
-          <t>OPM, TP/ G6, M1, Mlle Ali Merina.H</t>
-        </is>
-      </c>
+      <c r="F22" s="27" t="n"/>
+      <c r="G22" s="27" t="n"/>
       <c r="H22" s="27" t="n"/>
     </row>
     <row r="23" ht="21.75" customHeight="1" s="24">
       <c r="A23" s="30" t="n"/>
       <c r="B23" s="31" t="n"/>
       <c r="C23" s="31" t="n"/>
-      <c r="D23" s="27" t="inlineStr">
-        <is>
-          <t>ALG2, TD/ G7, B1, Mme TABHARIT</t>
-        </is>
-      </c>
+      <c r="D23" s="27" t="n"/>
       <c r="E23" s="27" t="n"/>
-      <c r="F23" s="27" t="inlineStr">
-        <is>
-          <t>SM2, TD/ G7, C1, HASSAINE</t>
-        </is>
-      </c>
-      <c r="G23" s="27" t="inlineStr">
-        <is>
-          <t>ASD2, TP/ G7, C4, HENNI F</t>
-        </is>
-      </c>
+      <c r="F23" s="27" t="n"/>
+      <c r="G23" s="27" t="n"/>
       <c r="H23" s="27" t="n"/>
     </row>
     <row r="24" ht="21.75" customHeight="1" s="24">
@@ -12905,22 +12817,34 @@
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>SM2, COUR/ section 2, Amphi2, HASSAINE</t>
+          <t>SM2, COUR/ section 2, Amphi1, HASSAINE</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G1, A1, Mlle Hamou Maamar.M</t>
+          <t>IPSD, TD/ G3, B4, Mme Kaisserli</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G2, A1, Mlle Hamou Maamar.M</t>
-        </is>
-      </c>
-      <c r="F26" s="17" t="n"/>
-      <c r="G26" s="17" t="n"/>
-      <c r="H26" s="17" t="n"/>
+          <t>PHY2, TD/ G1, C1, Labdelli</t>
+        </is>
+      </c>
+      <c r="F26" s="17" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G1, A1, BENSALLOUA</t>
+        </is>
+      </c>
+      <c r="G26" s="17" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G3, C1, Labdelli</t>
+        </is>
+      </c>
+      <c r="H26" s="17" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G2, A4, BENSALLOUA</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
@@ -12928,27 +12852,59 @@
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G5, A2, Mlle Ali Merina.H</t>
+          <t>IPSD, TD/ G6, C1, M. Benyatou Kamel</t>
         </is>
       </c>
       <c r="E27" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G7, A2, Mlle Ali Merina.H</t>
-        </is>
-      </c>
-      <c r="F27" s="27" t="n"/>
-      <c r="G27" s="27" t="n"/>
-      <c r="H27" s="27" t="n"/>
+          <t>IPSD, TD/ G4, B4, Mme Kaisserli</t>
+        </is>
+      </c>
+      <c r="F27" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G2, B1, Labdelli</t>
+        </is>
+      </c>
+      <c r="G27" s="27" t="inlineStr">
+        <is>
+          <t>SM2, TD/ G4, B4, HAMAMI</t>
+        </is>
+      </c>
+      <c r="H27" s="27" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G5, C3, KAID SLIMANE</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
       <c r="B28" s="31" t="n"/>
       <c r="C28" s="31" t="n"/>
-      <c r="D28" s="27" t="n"/>
-      <c r="E28" s="27" t="n"/>
-      <c r="F28" s="27" t="n"/>
-      <c r="G28" s="27" t="n"/>
-      <c r="H28" s="27" t="n"/>
+      <c r="D28" s="27" t="inlineStr">
+        <is>
+          <t>IPSD, TD/ G7, C2, Mlle Dj. BENSIKADDOUR</t>
+        </is>
+      </c>
+      <c r="E28" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G5, C2, M. Benchehida</t>
+        </is>
+      </c>
+      <c r="F28" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G4, B2, M. Benchehida</t>
+        </is>
+      </c>
+      <c r="G28" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G6, C2, M. Benchehida</t>
+        </is>
+      </c>
+      <c r="H28" s="27" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G7, C4, HENNI F</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
@@ -13026,19 +12982,51 @@
           <t>TIC, COUR/ section 2, Amphi2, HENNI K.</t>
         </is>
       </c>
-      <c r="D35" s="17" t="n"/>
-      <c r="E35" s="17" t="n"/>
-      <c r="F35" s="17" t="n"/>
-      <c r="G35" s="17" t="n"/>
-      <c r="H35" s="17" t="n"/>
+      <c r="D35" s="17" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G3, A4, BENSALLOUA</t>
+        </is>
+      </c>
+      <c r="E35" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G1, A3, Mlle Hamou Maamar.M</t>
+        </is>
+      </c>
+      <c r="F35" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G2, A1, Mlle Hamou Maamar.M</t>
+        </is>
+      </c>
+      <c r="G35" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G6, A1, Mlle Ali Merina.H</t>
+        </is>
+      </c>
+      <c r="H35" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G3, A1, Mlle Hamou Maamar.M</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="21.75" customHeight="1" s="24">
       <c r="A36" s="30" t="n"/>
       <c r="B36" s="31" t="n"/>
       <c r="C36" s="31" t="n"/>
-      <c r="D36" s="27" t="n"/>
-      <c r="E36" s="27" t="n"/>
-      <c r="F36" s="27" t="n"/>
+      <c r="D36" s="27" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G4, C3, KAID SLIMANE</t>
+        </is>
+      </c>
+      <c r="E36" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G5, A4, Mlle Ali Merina.H</t>
+        </is>
+      </c>
+      <c r="F36" s="27" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G4, A2, Mlle Ali Merina.H</t>
+        </is>
+      </c>
       <c r="G36" s="27" t="n"/>
       <c r="H36" s="27" t="n"/>
     </row>
@@ -13046,8 +13034,16 @@
       <c r="A37" s="30" t="n"/>
       <c r="B37" s="31" t="n"/>
       <c r="C37" s="31" t="n"/>
-      <c r="D37" s="27" t="n"/>
-      <c r="E37" s="27" t="n"/>
+      <c r="D37" s="27" t="inlineStr">
+        <is>
+          <t>PHY2, TD/ G7, B1, M. Benchehida</t>
+        </is>
+      </c>
+      <c r="E37" s="27" t="inlineStr">
+        <is>
+          <t>ASD2, TP/ G6, A2, KAID SLIMANE</t>
+        </is>
+      </c>
       <c r="F37" s="27" t="n"/>
       <c r="G37" s="27" t="n"/>
       <c r="H37" s="27" t="n"/>
@@ -13118,7 +13114,11 @@
           <t>Jeudi</t>
         </is>
       </c>
-      <c r="B44" s="17" t="n"/>
+      <c r="B44" s="17" t="inlineStr">
+        <is>
+          <t>OPM, TP/ G7, A1, Mlle Ali Merina.H</t>
+        </is>
+      </c>
       <c r="C44" s="29" t="inlineStr">
         <is>
           <t>PHY2, COUR/ section 2, Amphi1, M. Benchehida</t>
@@ -14333,23 +14333,27 @@
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>TL, TD/ G1, S11, MIDOUN M.</t>
-        </is>
-      </c>
-      <c r="E8" s="17" t="n"/>
+          <t>TL, TD/ G1, S12, MIDOUN M.</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="inlineStr">
+        <is>
+          <t>TL, TD/ G3, S12, MIDOUN M.</t>
+        </is>
+      </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>SE1, TD/ G1, S8, BOUZEBIBA</t>
+          <t>SE1, TD/ G1, S15, BOUZEBIBA</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>BDD, TD/ G1, S8, MIROUD</t>
+          <t>BDD, TD/ G1, S15, MIROUD</t>
         </is>
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G1, S11, BOUZEBIBA</t>
+          <t>BDD, TD/ G2, S14, MENAD</t>
         </is>
       </c>
     </row>
@@ -14359,23 +14363,27 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G2, S8, BOUZEBIBA</t>
-        </is>
-      </c>
-      <c r="E9" s="27" t="n"/>
+          <t>SE1, TD/ G2, S15, BOUZEBIBA</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="inlineStr">
+        <is>
+          <t>TL, TD/ G5, S13, BESNASSI</t>
+        </is>
+      </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G2, S11, MIDOUN M.</t>
+          <t>TL, TD/ G2, S12, MIDOUN M.</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G2, S16, MENAD</t>
+          <t>SE1, TD/ G3, S12, DJAHAFI</t>
         </is>
       </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G2, A4, MIDOUN M.</t>
+          <t>SE1, TD/ G4, S12, DJAHAFI</t>
         </is>
       </c>
     </row>
@@ -14385,23 +14393,27 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G3, S16, DJAHAFI</t>
-        </is>
-      </c>
-      <c r="E10" s="27" t="n"/>
+          <t>TL, TD/ G4, S13, BESNASSI</t>
+        </is>
+      </c>
+      <c r="E10" s="27" t="inlineStr">
+        <is>
+          <t>SE1, TD/ G6, S15, KHIAT</t>
+        </is>
+      </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G3, S1, MENAD</t>
+          <t>TL, TD/ G6, S13, BESNASSI</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G3, S11, MIDOUN M.</t>
+          <t>SE1, TD/ G5, S13, KHIAT</t>
         </is>
       </c>
       <c r="H10" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G3, C4, HENNI K</t>
+          <t>BDD, TD/ G5, S15, MAGHNI SANDID Z.</t>
         </is>
       </c>
     </row>
@@ -14411,23 +14423,27 @@
       <c r="C11" s="31" t="n"/>
       <c r="D11" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G4, S10, BESNASSI</t>
-        </is>
-      </c>
-      <c r="E11" s="27" t="n"/>
+          <t>TL, TD/ G7, S14, BESSAOUD K.</t>
+        </is>
+      </c>
+      <c r="E11" s="27" t="inlineStr">
+        <is>
+          <t>TL, TD/ G8, S14, BESSAOUD K.</t>
+        </is>
+      </c>
       <c r="F11" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G4, S16, DJAHAFI</t>
+          <t>TL, TD/ G9, S14, BESSAOUD K.</t>
         </is>
       </c>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G4, S3, BOUZEBIBA</t>
+          <t>SE1, TD/ G7, S14, KENNICHE A.</t>
         </is>
       </c>
       <c r="H11" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G4, S6, MENAD</t>
+          <t>SE1, TD/ G8, S13, KENNICHE A.</t>
         </is>
       </c>
     </row>
@@ -14435,131 +14451,51 @@
       <c r="A12" s="30" t="n"/>
       <c r="B12" s="31" t="n"/>
       <c r="C12" s="31" t="n"/>
-      <c r="D12" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TD/ G5, S2, KHIAT</t>
-        </is>
-      </c>
+      <c r="D12" s="27" t="n"/>
       <c r="E12" s="27" t="n"/>
-      <c r="F12" s="27" t="inlineStr">
-        <is>
-          <t>TL, TD/ G5, S10, BESNASSI</t>
-        </is>
-      </c>
-      <c r="G12" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TD/ G5, S2, MAGHNI SANDID Z.</t>
-        </is>
-      </c>
-      <c r="H12" s="27" t="inlineStr">
-        <is>
-          <t>TL, TP/ G5, C3, BESNASSI</t>
-        </is>
-      </c>
+      <c r="F12" s="27" t="n"/>
+      <c r="G12" s="27" t="n"/>
+      <c r="H12" s="27" t="n"/>
     </row>
     <row r="13" ht="21.75" customHeight="1" s="24">
       <c r="A13" s="30" t="n"/>
       <c r="B13" s="31" t="n"/>
       <c r="C13" s="31" t="n"/>
-      <c r="D13" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TD/ G6, S1, MAGHNI SANDID Z.</t>
-        </is>
-      </c>
+      <c r="D13" s="27" t="n"/>
       <c r="E13" s="27" t="n"/>
-      <c r="F13" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TD/ G6, S2, KHIAT</t>
-        </is>
-      </c>
-      <c r="G13" s="27" t="inlineStr">
-        <is>
-          <t>TL, TD/ G6, S10, BESNASSI</t>
-        </is>
-      </c>
-      <c r="H13" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TP/ G6, M1, BETOUATI</t>
-        </is>
-      </c>
+      <c r="F13" s="27" t="n"/>
+      <c r="G13" s="27" t="n"/>
+      <c r="H13" s="27" t="n"/>
     </row>
     <row r="14" ht="21.75" customHeight="1" s="24">
       <c r="A14" s="30" t="n"/>
       <c r="B14" s="31" t="n"/>
       <c r="C14" s="31" t="n"/>
-      <c r="D14" s="27" t="inlineStr">
-        <is>
-          <t>TL, TD/ G7, S9, BESSAOUD K.</t>
-        </is>
-      </c>
+      <c r="D14" s="27" t="n"/>
       <c r="E14" s="27" t="n"/>
-      <c r="F14" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TD/ G7, S3, KENNICHE A.</t>
-        </is>
-      </c>
-      <c r="G14" s="27" t="inlineStr">
-        <is>
-          <t>RÉS, TD/ G7, S1, LAREDJ A. M</t>
-        </is>
-      </c>
-      <c r="H14" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TD/ G7, S7, MAGHNI SANDID Z.</t>
-        </is>
-      </c>
+      <c r="F14" s="27" t="n"/>
+      <c r="G14" s="27" t="n"/>
+      <c r="H14" s="27" t="n"/>
     </row>
     <row r="15" ht="21.75" customHeight="1" s="24">
       <c r="A15" s="30" t="n"/>
       <c r="B15" s="31" t="n"/>
       <c r="C15" s="31" t="n"/>
-      <c r="D15" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TD/ G8, S3, KENNICHE A.</t>
-        </is>
-      </c>
+      <c r="D15" s="27" t="n"/>
       <c r="E15" s="27" t="n"/>
-      <c r="F15" s="27" t="inlineStr">
-        <is>
-          <t>TL, TD/ G8, S9, BESSAOUD K.</t>
-        </is>
-      </c>
-      <c r="G15" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TP/ G8, A1, KENNICHE A.</t>
-        </is>
-      </c>
-      <c r="H15" s="27" t="inlineStr">
-        <is>
-          <t>RÉS, TD/ G8, S10, LAREDJ A. M</t>
-        </is>
-      </c>
+      <c r="F15" s="27" t="n"/>
+      <c r="G15" s="27" t="n"/>
+      <c r="H15" s="27" t="n"/>
     </row>
     <row r="16" ht="21.75" customHeight="1" s="24">
       <c r="A16" s="32" t="n"/>
       <c r="B16" s="33" t="n"/>
       <c r="C16" s="33" t="n"/>
-      <c r="D16" s="16" t="inlineStr">
-        <is>
-          <t>RÉS, TD/ G9, Amphi3, LAREDJ A. M</t>
-        </is>
-      </c>
+      <c r="D16" s="16" t="n"/>
       <c r="E16" s="16" t="n"/>
-      <c r="F16" s="16" t="inlineStr">
-        <is>
-          <t>BDD, TD/ G9, Amphi3, MAGHNI SANDID Z.</t>
-        </is>
-      </c>
-      <c r="G16" s="16" t="inlineStr">
-        <is>
-          <t>TL, TD/ G9, S9, BESSAOUD K.</t>
-        </is>
-      </c>
-      <c r="H16" s="16" t="inlineStr">
-        <is>
-          <t>SE1, TD/ G9, S5, KENNICHE A.</t>
-        </is>
-      </c>
+      <c r="F16" s="16" t="n"/>
+      <c r="G16" s="16" t="n"/>
+      <c r="H16" s="16" t="n"/>
     </row>
     <row r="17" ht="21.75" customHeight="1" s="24">
       <c r="A17" s="28" t="inlineStr">
@@ -14579,23 +14515,27 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>TL, TP/ G1, A1, MIDOUN M.</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="n"/>
+          <t>RÉS, TD/ G1, S15, BOUZEBIBA</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="inlineStr">
+        <is>
+          <t>RÉS, TD/ G2, C2, BOUZEBIBA</t>
+        </is>
+      </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>SE1, TP/ G1, M3, HENNI K</t>
+          <t>TL, TP/ G1, A4, MIDOUN M.</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>TL, TP/ G3, M2, MIDOUN M.</t>
+          <t>TL, TP/ G2, A4, MIDOUN M.</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>SE1, TP/ G2, M1, HENNI K</t>
+          <t>TL, TP/ G3, A2, MIDOUN M.</t>
         </is>
       </c>
     </row>
@@ -14605,23 +14545,27 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G2, S14, BOUZEBIBA</t>
-        </is>
-      </c>
-      <c r="E18" s="27" t="n"/>
+          <t>BDD, TD/ G3, S13, MENAD</t>
+        </is>
+      </c>
+      <c r="E18" s="27" t="inlineStr">
+        <is>
+          <t>BDD, TD/ G4, B4, MENAD</t>
+        </is>
+      </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G3, S14, BOUZEBIBA</t>
+          <t>RÉS, TD/ G3, C1, BOUZEBIBA</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G5, S12, BOUZEBIBA</t>
+          <t>TL, TP/ G4, C3, BESNASSI</t>
         </is>
       </c>
       <c r="H18" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G4, M2, DJAHAFI</t>
+          <t>RÉS, TD/ G4, S12, BOUZEBIBA</t>
         </is>
       </c>
     </row>
@@ -14631,23 +14575,27 @@
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G3, C4, BETOUATI</t>
-        </is>
-      </c>
-      <c r="E19" s="27" t="n"/>
+          <t>BDD, TD/ G6, S14, MAGHNI SANDID Z.</t>
+        </is>
+      </c>
+      <c r="E19" s="27" t="inlineStr">
+        <is>
+          <t>BDD, TD/ G7, C1, MAGHNI SANDID Z.</t>
+        </is>
+      </c>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G6, M1, BESNASSI</t>
+          <t>RÉS, TD/ G7, C2, LAREDJ A. M</t>
         </is>
       </c>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G9, M3, BESSAOUD K.</t>
+          <t>TL, TP/ G7, C4, BESSAOUD K.</t>
         </is>
       </c>
       <c r="H19" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G6, B3, BOUZEBIBA</t>
+          <t>TL, TP/ G5, A3, BESNASSI</t>
         </is>
       </c>
     </row>
@@ -14657,19 +14605,27 @@
       <c r="C20" s="31" t="n"/>
       <c r="D20" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G4, A2, BESNASSI</t>
-        </is>
-      </c>
-      <c r="E20" s="27" t="n"/>
+          <t>SE1, TD/ G9, S12, KENNICHE A.</t>
+        </is>
+      </c>
+      <c r="E20" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TD/ G8, S12, LAREDJ A. M</t>
+        </is>
+      </c>
       <c r="F20" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G8, M2, BESSAOUD K.</t>
-        </is>
-      </c>
-      <c r="G20" s="27" t="n"/>
+          <t>BDD, TD/ G8, B4, MAGHNI SANDID Z.</t>
+        </is>
+      </c>
+      <c r="G20" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TD/ G9, B4, LAREDJ A. M</t>
+        </is>
+      </c>
       <c r="H20" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G7, M3, KENNICHE A.</t>
+          <t>BDD, TD/ G9, C2, MAGHNI SANDID Z.</t>
         </is>
       </c>
     </row>
@@ -14677,11 +14633,7 @@
       <c r="A21" s="30" t="n"/>
       <c r="B21" s="31" t="n"/>
       <c r="C21" s="31" t="n"/>
-      <c r="D21" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TP/ G5, A4, DJAHAFI</t>
-        </is>
-      </c>
+      <c r="D21" s="27" t="n"/>
       <c r="E21" s="27" t="n"/>
       <c r="F21" s="27" t="n"/>
       <c r="G21" s="27" t="n"/>
@@ -14691,11 +14643,7 @@
       <c r="A22" s="30" t="n"/>
       <c r="B22" s="31" t="n"/>
       <c r="C22" s="31" t="n"/>
-      <c r="D22" s="27" t="inlineStr">
-        <is>
-          <t>RÉS, TP/ G6, M1, BENHAMED</t>
-        </is>
-      </c>
+      <c r="D22" s="27" t="n"/>
       <c r="E22" s="27" t="n"/>
       <c r="F22" s="27" t="n"/>
       <c r="G22" s="27" t="n"/>
@@ -14705,11 +14653,7 @@
       <c r="A23" s="30" t="n"/>
       <c r="B23" s="31" t="n"/>
       <c r="C23" s="31" t="n"/>
-      <c r="D23" s="27" t="inlineStr">
-        <is>
-          <t>TL, TP/ G7, A3, BESSAOUD K.</t>
-        </is>
-      </c>
+      <c r="D23" s="27" t="n"/>
       <c r="E23" s="27" t="n"/>
       <c r="F23" s="27" t="n"/>
       <c r="G23" s="27" t="n"/>
@@ -14719,11 +14663,7 @@
       <c r="A24" s="30" t="n"/>
       <c r="B24" s="31" t="n"/>
       <c r="C24" s="31" t="n"/>
-      <c r="D24" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TD/ G8, S13, MAGHNI SANDID Z.</t>
-        </is>
-      </c>
+      <c r="D24" s="27" t="n"/>
       <c r="E24" s="27" t="n"/>
       <c r="F24" s="27" t="n"/>
       <c r="G24" s="27" t="n"/>
@@ -14733,11 +14673,7 @@
       <c r="A25" s="32" t="n"/>
       <c r="B25" s="33" t="n"/>
       <c r="C25" s="33" t="n"/>
-      <c r="D25" s="16" t="inlineStr">
-        <is>
-          <t>SE1, TP/ G9, C3, KENNICHE A.</t>
-        </is>
-      </c>
+      <c r="D25" s="16" t="n"/>
       <c r="E25" s="16" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="16" t="n"/>
@@ -14756,32 +14692,32 @@
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>DAW, COUR/ section 1, Amphi3, SEHABA K.</t>
+          <t>DAW, COUR/ section 1, Amphi2, SEHABA K.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
+          <t>SE1, TP/ G1, A3, HENNI K</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="inlineStr">
+        <is>
+          <t>SE1, TP/ G2, A2, HENNI K</t>
+        </is>
+      </c>
+      <c r="F26" s="17" t="inlineStr">
+        <is>
           <t>BDD, TP/ G1, A4, MEROUFEL B.</t>
         </is>
       </c>
-      <c r="E26" s="17" t="inlineStr">
-        <is>
-          <t>BDD, TP/ G8, A3, MIROUD</t>
-        </is>
-      </c>
-      <c r="F26" s="17" t="inlineStr">
-        <is>
-          <t>RÉS, TP/ G1, A4,  MOUSSA M.</t>
-        </is>
-      </c>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>POO, TP/ G1, A1, BETOUATI</t>
+          <t>BDD, TP/ G2, A3, MEROUFEL B.</t>
         </is>
       </c>
       <c r="H26" s="17" t="inlineStr">
         <is>
-          <t>DAW, TP/ G1, A4, HENNI K</t>
+          <t>BDD, TP/ G4, M2, BETOUATI</t>
         </is>
       </c>
     </row>
@@ -14791,27 +14727,27 @@
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G2, M1,  MOUSSA M.</t>
+          <t>RÉS, TD/ G5, S12, BOUZEBIBA</t>
         </is>
       </c>
       <c r="E27" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G9, A4, BENHAMED</t>
+          <t>SE1, TP/ G4, A3, DJAHAFI</t>
         </is>
       </c>
       <c r="F27" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G2, A1, MEROUFEL B.</t>
+          <t>SE1, TP/ G3, A2, HENNI K</t>
         </is>
       </c>
       <c r="G27" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G2, A3, HENNI K</t>
+          <t>BDD, TP/ G3, A4, BETOUATI</t>
         </is>
       </c>
       <c r="H27" s="27" t="inlineStr">
         <is>
-          <t>POO, TP/ G2, A2, BETOUATI</t>
+          <t>SE1, TP/ G6, M1, DJAHAFI</t>
         </is>
       </c>
     </row>
@@ -14821,23 +14757,27 @@
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G3, M2, BENHAMED</t>
-        </is>
-      </c>
-      <c r="E28" s="27" t="n"/>
+          <t>TL, TP/ G6, A1, BESNASSI</t>
+        </is>
+      </c>
+      <c r="E28" s="27" t="inlineStr">
+        <is>
+          <t>SE1, TP/ G7, A4, KENNICHE A.</t>
+        </is>
+      </c>
       <c r="F28" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G3, M1, HENNI K</t>
+          <t>RÉS, TD/ G6, B3, BOUZEBIBA</t>
         </is>
       </c>
       <c r="G28" s="27" t="inlineStr">
         <is>
-          <t>POO, TP/ G4, A2, ABID M.</t>
+          <t>SE1, TP/ G5, A1, DJAHAFI</t>
         </is>
       </c>
       <c r="H28" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G5, A1, BENHAMED</t>
+          <t>BDD, TP/ G7, M3, MIROUD</t>
         </is>
       </c>
     </row>
@@ -14847,63 +14787,43 @@
       <c r="C29" s="31" t="n"/>
       <c r="D29" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G4, C3, BETOUATI</t>
-        </is>
-      </c>
-      <c r="E29" s="27" t="n"/>
+          <t>TL, TP/ G8, A2, BESSAOUD K.</t>
+        </is>
+      </c>
+      <c r="E29" s="27" t="inlineStr">
+        <is>
+          <t>TL, TP/ G9, A1, BESSAOUD K.</t>
+        </is>
+      </c>
       <c r="F29" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G4, C3, BENHAMED</t>
+          <t>SE1, TP/ G8, A3, KENNICHE A.</t>
         </is>
       </c>
       <c r="G29" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G5, A4, SEHABA K.</t>
-        </is>
-      </c>
-      <c r="H29" s="27" t="inlineStr">
-        <is>
-          <t>DAW, TP/ G6, C3, SEHABA K.</t>
-        </is>
-      </c>
+          <t>SE1, TP/ G9, A2, KENNICHE A.</t>
+        </is>
+      </c>
+      <c r="H29" s="27" t="n"/>
     </row>
     <row r="30" ht="21.75" customHeight="1" s="24">
       <c r="A30" s="30" t="n"/>
       <c r="B30" s="31" t="n"/>
       <c r="C30" s="31" t="n"/>
-      <c r="D30" s="27" t="inlineStr">
-        <is>
-          <t>POO, TP/ G5, M3, ABID M.</t>
-        </is>
-      </c>
+      <c r="D30" s="27" t="n"/>
       <c r="E30" s="27" t="n"/>
-      <c r="F30" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TP/ G5, A2, BETOUATI</t>
-        </is>
-      </c>
+      <c r="F30" s="27" t="n"/>
       <c r="G30" s="27" t="n"/>
-      <c r="H30" s="27" t="inlineStr">
-        <is>
-          <t>POO, TP/ G7, A3, ABID M.</t>
-        </is>
-      </c>
+      <c r="H30" s="27" t="n"/>
     </row>
     <row r="31" ht="21.75" customHeight="1" s="24">
       <c r="A31" s="30" t="n"/>
       <c r="B31" s="31" t="n"/>
       <c r="C31" s="31" t="n"/>
-      <c r="D31" s="27" t="inlineStr">
-        <is>
-          <t>SE1, TP/ G6, A3, DJAHAFI</t>
-        </is>
-      </c>
+      <c r="D31" s="27" t="n"/>
       <c r="E31" s="27" t="n"/>
-      <c r="F31" s="27" t="inlineStr">
-        <is>
-          <t>POO, TP/ G6, C4, ABID M.</t>
-        </is>
-      </c>
+      <c r="F31" s="27" t="n"/>
       <c r="G31" s="27" t="n"/>
       <c r="H31" s="27" t="n"/>
     </row>
@@ -14911,17 +14831,9 @@
       <c r="A32" s="30" t="n"/>
       <c r="B32" s="31" t="n"/>
       <c r="C32" s="31" t="n"/>
-      <c r="D32" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TP/ G7, C4, MIROUD</t>
-        </is>
-      </c>
+      <c r="D32" s="27" t="n"/>
       <c r="E32" s="27" t="n"/>
-      <c r="F32" s="27" t="inlineStr">
-        <is>
-          <t>DAW, TP/ G7, M2, SEHABA K.</t>
-        </is>
-      </c>
+      <c r="F32" s="27" t="n"/>
       <c r="G32" s="27" t="n"/>
       <c r="H32" s="27" t="n"/>
     </row>
@@ -14931,11 +14843,7 @@
       <c r="C33" s="31" t="n"/>
       <c r="D33" s="27" t="n"/>
       <c r="E33" s="27" t="n"/>
-      <c r="F33" s="27" t="inlineStr">
-        <is>
-          <t>BDD, TP/ G9, A3, MIROUD</t>
-        </is>
-      </c>
+      <c r="F33" s="27" t="n"/>
       <c r="G33" s="27" t="n"/>
       <c r="H33" s="27" t="n"/>
     </row>
@@ -14957,77 +14865,149 @@
       </c>
       <c r="B35" s="17" t="inlineStr">
         <is>
-          <t>POO, TP/ G3, A2, BETOUATI</t>
+          <t>RÉS, TP/ G1, A3,  MOUSSA M.</t>
         </is>
       </c>
       <c r="C35" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G8, A1, BENHAMED</t>
+          <t>RÉS, TP/ G2, A3,  MOUSSA M.</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>DAW, TP/ G8, A1, SEHABA K.</t>
-        </is>
-      </c>
-      <c r="E35" s="17" t="n"/>
-      <c r="F35" s="17" t="n"/>
-      <c r="G35" s="17" t="n"/>
-      <c r="H35" s="17" t="n"/>
+          <t>POO, TP/ G1, M1, BETOUATI</t>
+        </is>
+      </c>
+      <c r="E35" s="17" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G1, C4, HENNI K</t>
+        </is>
+      </c>
+      <c r="F35" s="17" t="inlineStr">
+        <is>
+          <t>POO, TP/ G2, A4, BETOUATI</t>
+        </is>
+      </c>
+      <c r="G35" s="17" t="inlineStr">
+        <is>
+          <t>POO, TP/ G3, A3, BETOUATI</t>
+        </is>
+      </c>
+      <c r="H35" s="17" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G4, A4, HENNI K</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="21.75" customHeight="1" s="24">
       <c r="A36" s="30" t="n"/>
       <c r="B36" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G4, A4, HENNI K</t>
+          <t>RÉS, TP/ G3, A4, BENHAMED</t>
         </is>
       </c>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>POO, TP/ G9, A2, ABID M.</t>
-        </is>
-      </c>
-      <c r="D36" s="27" t="n"/>
-      <c r="E36" s="27" t="n"/>
-      <c r="F36" s="27" t="n"/>
-      <c r="G36" s="27" t="n"/>
-      <c r="H36" s="27" t="n"/>
+          <t>RÉS, TP/ G4, A4, BENHAMED</t>
+        </is>
+      </c>
+      <c r="D36" s="27" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G2, M3, HENNI K</t>
+        </is>
+      </c>
+      <c r="E36" s="27" t="inlineStr">
+        <is>
+          <t>POO, TP/ G5, C3, ABID M.</t>
+        </is>
+      </c>
+      <c r="F36" s="27" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G3, C4, HENNI K</t>
+        </is>
+      </c>
+      <c r="G36" s="27" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G5, A4, SEHABA K.</t>
+        </is>
+      </c>
+      <c r="H36" s="27" t="inlineStr">
+        <is>
+          <t>POO, TP/ G6, A3, ABID M.</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="21.75" customHeight="1" s="24">
       <c r="A37" s="30" t="n"/>
       <c r="B37" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G7, A1, BENHAMED</t>
-        </is>
-      </c>
-      <c r="C37" s="27" t="n"/>
-      <c r="D37" s="27" t="n"/>
-      <c r="E37" s="27" t="n"/>
-      <c r="F37" s="27" t="n"/>
-      <c r="G37" s="27" t="n"/>
-      <c r="H37" s="27" t="n"/>
+          <t>BDD, TP/ G5, A1, BETOUATI</t>
+        </is>
+      </c>
+      <c r="C37" s="27" t="inlineStr">
+        <is>
+          <t>BDD, TP/ G6, A1, BETOUATI</t>
+        </is>
+      </c>
+      <c r="D37" s="27" t="inlineStr">
+        <is>
+          <t>POO, TP/ G4, M2, ABID M.</t>
+        </is>
+      </c>
+      <c r="E37" s="27" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G6, M1, SEHABA K.</t>
+        </is>
+      </c>
+      <c r="F37" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TP/ G6, A3, BENHAMED</t>
+        </is>
+      </c>
+      <c r="G37" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TP/ G7, A2, BENHAMED</t>
+        </is>
+      </c>
+      <c r="H37" s="27" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G7, C3, SEHABA K.</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="21.75" customHeight="1" s="24">
       <c r="A38" s="30" t="n"/>
       <c r="B38" s="27" t="inlineStr">
         <is>
-          <t>POO, TP/ G8, A3, ABID M.</t>
-        </is>
-      </c>
-      <c r="C38" s="27" t="n"/>
-      <c r="D38" s="27" t="n"/>
+          <t>BDD, TP/ G8, A2, MIROUD</t>
+        </is>
+      </c>
+      <c r="C38" s="27" t="inlineStr">
+        <is>
+          <t>BDD, TP/ G9, A2, MIROUD</t>
+        </is>
+      </c>
+      <c r="D38" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TP/ G5, C4, BENHAMED</t>
+        </is>
+      </c>
       <c r="E38" s="27" t="n"/>
-      <c r="F38" s="27" t="n"/>
+      <c r="F38" s="27" t="inlineStr">
+        <is>
+          <t>POO, TP/ G7, C3, ABID M.</t>
+        </is>
+      </c>
       <c r="G38" s="27" t="n"/>
-      <c r="H38" s="27" t="n"/>
+      <c r="H38" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TP/ G8, A2, BENHAMED</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="21.75" customHeight="1" s="24">
       <c r="A39" s="30" t="n"/>
-      <c r="B39" s="27" t="inlineStr">
-        <is>
-          <t>DAW, TP/ G9, C3, SEHABA K.</t>
-        </is>
-      </c>
+      <c r="B39" s="27" t="n"/>
       <c r="C39" s="27" t="n"/>
       <c r="D39" s="27" t="n"/>
       <c r="E39" s="27" t="n"/>
@@ -15081,9 +15061,21 @@
           <t>Jeudi</t>
         </is>
       </c>
-      <c r="B44" s="17" t="n"/>
-      <c r="C44" s="17" t="n"/>
-      <c r="D44" s="17" t="n"/>
+      <c r="B44" s="17" t="inlineStr">
+        <is>
+          <t>POO, TP/ G8, A3, ABID M.</t>
+        </is>
+      </c>
+      <c r="C44" s="17" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G8, A2, SEHABA K.</t>
+        </is>
+      </c>
+      <c r="D44" s="17" t="inlineStr">
+        <is>
+          <t>DAW, TP/ G9, A1, SEHABA K.</t>
+        </is>
+      </c>
       <c r="E44" s="17" t="n"/>
       <c r="F44" s="17" t="n"/>
       <c r="G44" s="17" t="n"/>
@@ -15091,8 +15083,16 @@
     </row>
     <row r="45" ht="21.75" customHeight="1" s="24">
       <c r="A45" s="30" t="n"/>
-      <c r="B45" s="27" t="n"/>
-      <c r="C45" s="27" t="n"/>
+      <c r="B45" s="27" t="inlineStr">
+        <is>
+          <t>RÉS, TP/ G9, A2, BENHAMED</t>
+        </is>
+      </c>
+      <c r="C45" s="27" t="inlineStr">
+        <is>
+          <t>POO, TP/ G9, A1, ABID M.</t>
+        </is>
+      </c>
       <c r="D45" s="27" t="n"/>
       <c r="E45" s="27" t="n"/>
       <c r="F45" s="27" t="n"/>
@@ -16289,27 +16289,27 @@
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>SI, TD/ G1, Amphi4, BENIDRIS F.Z</t>
+          <t>SI, TD/ G1, S4, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>SI, TD/ G5, B1, BENIDRIS F.Z</t>
+          <t>SI, TD/ G4, S4, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G1, Amphi4, HOCINE N.</t>
+          <t>RS, TD/ G1, S4, HOCINE N.</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G1, A2, HOCINE</t>
+          <t>IA, TP/ G1, A1, HOCINE</t>
         </is>
       </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>AP, TP/ G1, M2, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G1, A1, MECHAOUI M. D.G</t>
         </is>
       </c>
     </row>
@@ -16319,27 +16319,27 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
+          <t>RS, TD/ G2, S5, HOCINE N.</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="inlineStr">
+        <is>
+          <t>RS, TD/ G5, S5, HOCINE N.</t>
+        </is>
+      </c>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
           <t>AP, TP/ G2, A1, MECHAOUI M. D.G</t>
         </is>
       </c>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>RS, TD/ G6, B2, HOCINE N.</t>
-        </is>
-      </c>
-      <c r="F9" s="27" t="inlineStr">
-        <is>
-          <t>IA, TP/ G2, A2, HOCINE</t>
-        </is>
-      </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G2, Amphi3, BENIDRIS F.Z</t>
+          <t>SI, TD/ G2, S4, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G3, S9, BENIDRIS F.Z</t>
+          <t>SI, TD/ G3, S4, BENIDRIS F.Z</t>
         </is>
       </c>
     </row>
@@ -16349,27 +16349,27 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
+          <t>AP, TP/ G3, A1, MECHAOUI M. D.G</t>
+        </is>
+      </c>
+      <c r="E10" s="27" t="inlineStr">
+        <is>
+          <t>AP, TP/ G6, A1, MECHAOUI M. D.G</t>
+        </is>
+      </c>
+      <c r="F10" s="27" t="inlineStr">
+        <is>
           <t>IA, TP/ G3, A2, HOCINE</t>
         </is>
       </c>
-      <c r="E10" s="27" t="inlineStr">
-        <is>
-          <t>AP, TP/ G7, A1, MECHAOUI M. D.G</t>
-        </is>
-      </c>
-      <c r="F10" s="27" t="inlineStr">
-        <is>
-          <t>AP, TP/ G3, A1, MECHAOUI M. D.G</t>
-        </is>
-      </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>RS, TD/ G3, Amphi4, HOCINE N.</t>
+          <t>DSS, TP/ G3, A2, DELALI A.</t>
         </is>
       </c>
       <c r="H10" s="27" t="inlineStr">
         <is>
-          <t>IA, TP/ G4, M3, HOCINE</t>
+          <t>RS, TD/ G4, S5, HOCINE N.</t>
         </is>
       </c>
     </row>
@@ -16377,22 +16377,10 @@
       <c r="A11" s="30" t="n"/>
       <c r="B11" s="31" t="n"/>
       <c r="C11" s="31" t="n"/>
-      <c r="D11" s="27" t="inlineStr">
-        <is>
-          <t>DSS, TP/ G4, A3, DELALI A.</t>
-        </is>
-      </c>
+      <c r="D11" s="27" t="n"/>
       <c r="E11" s="27" t="n"/>
-      <c r="F11" s="27" t="inlineStr">
-        <is>
-          <t>DSS, TP/ G5, A3, DELALI A.</t>
-        </is>
-      </c>
-      <c r="G11" s="27" t="inlineStr">
-        <is>
-          <t>DSS, TP/ G6, A3, DELALI A.</t>
-        </is>
-      </c>
+      <c r="F11" s="27" t="n"/>
+      <c r="G11" s="27" t="n"/>
       <c r="H11" s="27" t="n"/>
     </row>
     <row r="12" ht="21.75" customHeight="1" s="24">
@@ -16463,27 +16451,27 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G2, S4, HOCINE N.</t>
+          <t>RS, TD/ G3, S5, HOCINE N.</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G1, A1, DELALI A.</t>
+          <t>IA, TP/ G2, A1, HOCINE</t>
         </is>
       </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G4, S4, HOCINE N.</t>
+          <t>AP, TP/ G5, C3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G5, S13, HOCINE N.</t>
+          <t>DSS, TP/ G1, M3, DELALI A.</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G7, B4, HOCINE N.</t>
+          <t>DSS, TP/ G2, C3, DELALI A.</t>
         </is>
       </c>
     </row>
@@ -16493,21 +16481,29 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G4, S15, BENIDRIS F.Z</t>
+          <t>AP, TP/ G4, A1, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="E18" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G7, B1, BENIDRIS F.Z</t>
+          <t>SI, TD/ G6, S13, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G6, S15, BENIDRIS F.Z</t>
-        </is>
-      </c>
-      <c r="G18" s="27" t="n"/>
-      <c r="H18" s="27" t="n"/>
+          <t>RS, TD/ G6, S13, HOCINE N.</t>
+        </is>
+      </c>
+      <c r="G18" s="27" t="inlineStr">
+        <is>
+          <t>IA, TP/ G4, M2, HOCINE</t>
+        </is>
+      </c>
+      <c r="H18" s="27" t="inlineStr">
+        <is>
+          <t>IA, TP/ G5, A4, HOCINE</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
@@ -16515,23 +16511,31 @@
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G5, M2, MECHAOUI M. D.G</t>
-        </is>
-      </c>
-      <c r="E19" s="27" t="n"/>
-      <c r="F19" s="27" t="n"/>
-      <c r="G19" s="27" t="n"/>
+          <t>SI, TD/ G5, S4, BENIDRIS F.Z</t>
+        </is>
+      </c>
+      <c r="E19" s="27" t="inlineStr">
+        <is>
+          <t>RS, TD/ G7, S14, HOCINE N.</t>
+        </is>
+      </c>
+      <c r="F19" s="27" t="inlineStr">
+        <is>
+          <t>SI, TD/ G7, S12, BENIDRIS F.Z</t>
+        </is>
+      </c>
+      <c r="G19" s="27" t="inlineStr">
+        <is>
+          <t>AP, TP/ G7, M1, MECHAOUI M. D.G</t>
+        </is>
+      </c>
       <c r="H19" s="27" t="n"/>
     </row>
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
       <c r="B20" s="31" t="n"/>
       <c r="C20" s="31" t="n"/>
-      <c r="D20" s="27" t="inlineStr">
-        <is>
-          <t>IA, TP/ G6, M3, HOCINE</t>
-        </is>
-      </c>
+      <c r="D20" s="27" t="n"/>
       <c r="E20" s="27" t="n"/>
       <c r="F20" s="27" t="n"/>
       <c r="G20" s="27" t="n"/>
@@ -16600,21 +16604,25 @@
       </c>
       <c r="C26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G2, A3, DELALI A.</t>
-        </is>
-      </c>
-      <c r="D26" s="17" t="n"/>
+          <t>DSS, TP/ G4, A2, DELALI A.</t>
+        </is>
+      </c>
+      <c r="D26" s="17" t="inlineStr">
+        <is>
+          <t>DSS, TP/ G5, C3, DELALI A.</t>
+        </is>
+      </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G3, M1, DELALI A.</t>
-        </is>
-      </c>
-      <c r="F26" s="17" t="inlineStr">
-        <is>
-          <t>DSS, TP/ G7, M3, DELALI A.</t>
-        </is>
-      </c>
-      <c r="G26" s="17" t="n"/>
+          <t>DSS, TP/ G6, C3, DELALI A.</t>
+        </is>
+      </c>
+      <c r="F26" s="17" t="n"/>
+      <c r="G26" s="17" t="inlineStr">
+        <is>
+          <t>DSS, TP/ G7, C3, DELALI A.</t>
+        </is>
+      </c>
       <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
@@ -16622,15 +16630,15 @@
       <c r="B27" s="31" t="n"/>
       <c r="C27" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G4, A1, MECHAOUI M. D.G</t>
-        </is>
-      </c>
-      <c r="D27" s="27" t="n"/>
-      <c r="E27" s="27" t="inlineStr">
-        <is>
-          <t>AP, TP/ G6, C3, MECHAOUI M. D.G</t>
-        </is>
-      </c>
+          <t>IA, TP/ G6, A1, HOCINE</t>
+        </is>
+      </c>
+      <c r="D27" s="27" t="inlineStr">
+        <is>
+          <t>IA, TP/ G7, A4, HOCINE</t>
+        </is>
+      </c>
+      <c r="E27" s="27" t="n"/>
       <c r="F27" s="27" t="n"/>
       <c r="G27" s="27" t="n"/>
       <c r="H27" s="27" t="n"/>
@@ -16638,17 +16646,9 @@
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
       <c r="B28" s="31" t="n"/>
-      <c r="C28" s="27" t="inlineStr">
-        <is>
-          <t>IA, TP/ G5, A2, HOCINE</t>
-        </is>
-      </c>
+      <c r="C28" s="27" t="n"/>
       <c r="D28" s="27" t="n"/>
-      <c r="E28" s="27" t="inlineStr">
-        <is>
-          <t>IA, TP/ G7, C4, HOCINE</t>
-        </is>
-      </c>
+      <c r="E28" s="27" t="n"/>
       <c r="F28" s="27" t="n"/>
       <c r="G28" s="27" t="n"/>
       <c r="H28" s="27" t="n"/>
@@ -18018,17 +18018,25 @@
           <t>ANA4, COUR/ section 1, S16, Mme Limam</t>
         </is>
       </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>ANA4, TD/ G1, B3, Mme Limam</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>ANA4, TD/ G1, S6, Mme Limam</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>ALG4, TD/ G1, S6, M.Ould ali</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>AC, TD/ G1, S6, Mlle Amina FERRAOUN</t>
+        </is>
+      </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>ALG4, TD/ G1, S16, M.Ould ali</t>
+          <t>ANUM2, TD/ G1, S7, M. Belhamiti Omar</t>
         </is>
       </c>
     </row>
@@ -18036,17 +18044,25 @@
       <c r="A9" s="30" t="n"/>
       <c r="B9" s="31" t="n"/>
       <c r="C9" s="31" t="n"/>
-      <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>ALG4, TD/ G2, B4, M.Ould ali</t>
-        </is>
-      </c>
-      <c r="F9" s="27" t="n"/>
-      <c r="G9" s="27" t="n"/>
+      <c r="D9" s="27" t="inlineStr">
+        <is>
+          <t>ALG4, TD/ G2, S7, M.Ould ali</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="n"/>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>ANA4, TD/ G2, S5, Mme Limam</t>
+        </is>
+      </c>
+      <c r="G9" s="27" t="inlineStr">
+        <is>
+          <t>ANA4, TD/ G2, S5, Mme Limam</t>
+        </is>
+      </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G2, S8, Mme Limam</t>
+          <t>AC, TD/ G2, S6, Mlle Amina FERRAOUN</t>
         </is>
       </c>
     </row>
@@ -18138,25 +18154,21 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G1, S5, Mme Limam</t>
+          <t>ANA4, TD/ G1, S6, Mme Limam</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>AC, TD/ G1, S6, Mlle Amina FERRAOUN</t>
+          <t>PROBA, TD/ G1, S14, M. Mohammedi Mustapha</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>ANUM2, TD/ G1, S14, M. Belhamiti Omar</t>
-        </is>
-      </c>
-      <c r="H17" s="17" t="inlineStr">
-        <is>
-          <t>PROBA, TD/ G1, C2, M. Mohammedi Mustapha</t>
-        </is>
-      </c>
+          <t>GÉOMÉ, TD/ G1, C2, Mme Bendahmane Hafida</t>
+        </is>
+      </c>
+      <c r="H17" s="17" t="n"/>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
@@ -18164,25 +18176,21 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>AC, TD/ G2, S6, Mlle Amina FERRAOUN</t>
+          <t>ANUM2, TD/ G2, S7, M. Belhamiti Omar</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G2, S5, Mme Limam</t>
+          <t>GÉOMÉ, TD/ G2, S15, Mme Bendahmane Hafida</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>PROBA, TD/ G2, S15, M. Mohammedi Mustapha</t>
-        </is>
-      </c>
-      <c r="H18" s="27" t="inlineStr">
-        <is>
-          <t>ANUM2, TD/ G2, C1, M. Belhamiti Omar</t>
-        </is>
-      </c>
+          <t>PROBA, TD/ G2, C1, M. Mohammedi Mustapha</t>
+        </is>
+      </c>
+      <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
@@ -18270,16 +18278,8 @@
           <t>ANUM2, COUR/ section 1, S16, M. Belhamiti Omar</t>
         </is>
       </c>
-      <c r="D26" s="17" t="inlineStr">
-        <is>
-          <t>GÉOMÉ, TD/ G1, B2, Mme Bendahmane Hafida</t>
-        </is>
-      </c>
-      <c r="E26" s="17" t="inlineStr">
-        <is>
-          <t>GÉOMÉ, TD/ G2, B2, Mme Bendahmane Hafida</t>
-        </is>
-      </c>
+      <c r="D26" s="17" t="n"/>
+      <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="17" t="n"/>
       <c r="H26" s="17" t="n"/>
@@ -19685,17 +19685,25 @@
           <t>TOL, COUR/ section 1, S2, M. Menad Abdallah</t>
         </is>
       </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>TOL, TD/ G1, C1, M. Menad Abdallah</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>TOL, TD/ G1, S11, M. Menad Abdallah</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>EDP, TD/ G1, S11, Mme Belmouhoub-Ould ali</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>EDP, TD/ G1, S11, Mme Belmouhoub-Ould ali</t>
+        </is>
+      </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>EDP, TD/ G1, S3, Mme Belmouhoub-Ould ali</t>
+          <t>TRAL, TD/ G1, S11, M. Andasmas M</t>
         </is>
       </c>
     </row>
@@ -19703,17 +19711,25 @@
       <c r="A9" s="30" t="n"/>
       <c r="B9" s="31" t="n"/>
       <c r="C9" s="31" t="n"/>
-      <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>EDP, TD/ G2, C2, Mme Belmouhoub-Ould ali</t>
-        </is>
-      </c>
-      <c r="F9" s="27" t="n"/>
-      <c r="G9" s="27" t="n"/>
+      <c r="D9" s="27" t="inlineStr">
+        <is>
+          <t>EDP, TD/ G2, S10, Mme Belmouhoub-Ould ali</t>
+        </is>
+      </c>
+      <c r="E9" s="27" t="n"/>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>TOL, TD/ G2, S7, M. Menad Abdallah</t>
+        </is>
+      </c>
+      <c r="G9" s="27" t="inlineStr">
+        <is>
+          <t>TOL, TD/ G2, S7, M. Menad Abdallah</t>
+        </is>
+      </c>
       <c r="H9" s="27" t="inlineStr">
         <is>
-          <t>TOL, TD/ G2, S2, M. Menad Abdallah</t>
+          <t>Géo. Diff, TD/ G2, S10, M. Fettouch Houari</t>
         </is>
       </c>
     </row>
@@ -19805,25 +19821,17 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>TOL, TD/ G1, S7, M. Menad Abdallah</t>
+          <t>TOL, TD/ G1, S11, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>EDP, TD/ G1, S11, Mme Belmouhoub-Ould ali</t>
-        </is>
-      </c>
-      <c r="G17" s="17" t="inlineStr">
-        <is>
-          <t>TRAL, TD/ G1, S4, M. Andasmas M</t>
-        </is>
-      </c>
-      <c r="H17" s="17" t="inlineStr">
-        <is>
-          <t>Géo. Diff, TD/ G1, S13, M. Fettouch Houari</t>
-        </is>
-      </c>
+          <t>Géo. Diff, TD/ G1, S5, M. Fettouch Houari</t>
+        </is>
+      </c>
+      <c r="G17" s="17" t="n"/>
+      <c r="H17" s="17" t="n"/>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
@@ -19831,25 +19839,17 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>EDP, TD/ G2, S11, Mme Belmouhoub-Ould ali</t>
+          <t>EDP, TD/ G2, S10, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>TOL, TD/ G2, S7, M. Menad Abdallah</t>
-        </is>
-      </c>
-      <c r="G18" s="27" t="inlineStr">
-        <is>
-          <t>Géo. Diff, TD/ G2, S5, M. Fettouch Houari</t>
-        </is>
-      </c>
-      <c r="H18" s="27" t="inlineStr">
-        <is>
-          <t>TRAL, TD/ G2, S12, M. Andasmas M</t>
-        </is>
-      </c>
+          <t>TRAL, TD/ G2, S4, M. Andasmas M</t>
+        </is>
+      </c>
+      <c r="G18" s="27" t="n"/>
+      <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
@@ -21341,7 +21341,7 @@
       </c>
       <c r="C8" s="17" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G1, A1, MOUSSA M.</t>
+          <t>AOSI, TD/ G2, B1, KHIAT</t>
         </is>
       </c>
       <c r="D8" s="29" t="inlineStr">
@@ -21354,78 +21354,70 @@
           <t>ALOS, COUR/ section 1, Amphi1, MOUSSA M.</t>
         </is>
       </c>
-      <c r="F8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>AOSI, TP/ G1, A3, KHIAT</t>
+        </is>
+      </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G1, A4, KHIAT</t>
-        </is>
-      </c>
-      <c r="H8" s="17" t="n"/>
+          <t>ALOS, TP/ G2, A4, MOUSSA M.</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
+          <t>ALOS, TP/ G1, A2, MOUSSA M.</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
       <c r="B9" s="27" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G2, A1, MOUSSA M.</t>
+          <t>AOSI, TD/ G3, B2, KHELIFA N.</t>
         </is>
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G2, B1, KHIAT</t>
+          <t>AOSI, TD/ G4, B2, KHELIFA N.</t>
         </is>
       </c>
       <c r="D9" s="31" t="n"/>
       <c r="E9" s="31" t="n"/>
-      <c r="F9" s="27" t="n"/>
+      <c r="F9" s="27" t="inlineStr">
+        <is>
+          <t>AOSI, TP/ G3, A4, KHELIFA N.</t>
+        </is>
+      </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>SSI, TP/ G2, M1, BENTAOUZA C</t>
-        </is>
-      </c>
-      <c r="H9" s="27" t="n"/>
+          <t>AOSI, TP/ G4, A3, KHELIFA N.</t>
+        </is>
+      </c>
+      <c r="H9" s="27" t="inlineStr">
+        <is>
+          <t>SSI, TP/ G2, A3, BENTAOUZA C</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="21.75" customHeight="1" s="24">
       <c r="A10" s="30" t="n"/>
-      <c r="B10" s="27" t="inlineStr">
-        <is>
-          <t>AOSI, TD/ G3, B2, KHELIFA N.</t>
-        </is>
-      </c>
-      <c r="C10" s="27" t="inlineStr">
-        <is>
-          <t>SSI, TP/ G3, A2, BENTAOUZA C</t>
-        </is>
-      </c>
+      <c r="B10" s="27" t="n"/>
+      <c r="C10" s="27" t="n"/>
       <c r="D10" s="31" t="n"/>
       <c r="E10" s="31" t="n"/>
       <c r="F10" s="27" t="n"/>
-      <c r="G10" s="27" t="inlineStr">
-        <is>
-          <t>AOSI, TP/ G3, C3, KHELIFA N.</t>
-        </is>
-      </c>
+      <c r="G10" s="27" t="n"/>
       <c r="H10" s="27" t="n"/>
     </row>
     <row r="11" ht="21.75" customHeight="1" s="24">
       <c r="A11" s="30" t="n"/>
-      <c r="B11" s="27" t="inlineStr">
-        <is>
-          <t>SSI, TP/ G4, A2, BENTAOUZA C</t>
-        </is>
-      </c>
-      <c r="C11" s="27" t="inlineStr">
-        <is>
-          <t>AOSI, TD/ G4, B2, KHELIFA N.</t>
-        </is>
-      </c>
+      <c r="B11" s="27" t="n"/>
+      <c r="C11" s="27" t="n"/>
       <c r="D11" s="31" t="n"/>
       <c r="E11" s="31" t="n"/>
       <c r="F11" s="27" t="n"/>
-      <c r="G11" s="27" t="inlineStr">
-        <is>
-          <t>ALOS, TP/ G4, C4, MOUSSA M.</t>
-        </is>
-      </c>
+      <c r="G11" s="27" t="n"/>
       <c r="H11" s="27" t="n"/>
     </row>
     <row r="12" ht="21.75" customHeight="1" s="24">
@@ -21486,7 +21478,7 @@
       </c>
       <c r="B17" s="17" t="inlineStr">
         <is>
-          <t>SSI, TP/ G1, A4, BENTAOUZA C</t>
+          <t>AOSI, TP/ G2, A1, KHIAT</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
@@ -21496,35 +21488,55 @@
       </c>
       <c r="D17" s="29" t="inlineStr">
         <is>
-          <t>OWS, COUR/ section 1, Amphi2, DJEBBARA R.</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="n"/>
-      <c r="F17" s="17" t="n"/>
+          <t>OWS, COUR/ section 1, Amphi1, DJEBBARA R.</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="inlineStr">
+        <is>
+          <t>SSI, TP/ G1, A3, BENTAOUZA C</t>
+        </is>
+      </c>
+      <c r="F17" s="17" t="inlineStr">
+        <is>
+          <t>RO, TP/ G2, M1,  MIROUD</t>
+        </is>
+      </c>
       <c r="G17" s="17" t="n"/>
-      <c r="H17" s="17" t="n"/>
+      <c r="H17" s="17" t="inlineStr">
+        <is>
+          <t>FDD, TP/ G1, M1, HABIB ZAHMANI M</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G2, A1, KHIAT</t>
+          <t>ALOS, TP/ G3, A2, MOUSSA M.</t>
         </is>
       </c>
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="31" t="n"/>
-      <c r="E18" s="27" t="n"/>
-      <c r="F18" s="27" t="n"/>
+      <c r="E18" s="27" t="inlineStr">
+        <is>
+          <t>ALOS, TP/ G4, A2, MOUSSA M.</t>
+        </is>
+      </c>
+      <c r="F18" s="27" t="inlineStr">
+        <is>
+          <t>SSI, TP/ G3, C4, BENTAOUZA C</t>
+        </is>
+      </c>
       <c r="G18" s="27" t="n"/>
-      <c r="H18" s="27" t="n"/>
+      <c r="H18" s="27" t="inlineStr">
+        <is>
+          <t>SSI, TP/ G4, C4, BENTAOUZA C</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
-      <c r="B19" s="27" t="inlineStr">
-        <is>
-          <t>ALOS, TP/ G3, A3, MOUSSA M.</t>
-        </is>
-      </c>
+      <c r="B19" s="27" t="n"/>
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="31" t="n"/>
       <c r="E19" s="27" t="n"/>
@@ -21534,11 +21546,7 @@
     </row>
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
-      <c r="B20" s="27" t="inlineStr">
-        <is>
-          <t>AOSI, TP/ G4, A2, KHELIFA N.</t>
-        </is>
-      </c>
+      <c r="B20" s="27" t="n"/>
       <c r="C20" s="31" t="n"/>
       <c r="D20" s="31" t="n"/>
       <c r="E20" s="27" t="n"/>
@@ -21604,12 +21612,12 @@
       </c>
       <c r="B26" s="17" t="inlineStr">
         <is>
-          <t>FDD, TP/ G1, A1, HABIB ZAHMANI M</t>
+          <t>RO, TP/ G1, A2,  MIROUD</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>FDD, COUR/ section 1, Amphi4, MOUMEN M.</t>
+          <t>FDD, COUR/ section 1, Amphi3, MOUMEN M.</t>
         </is>
       </c>
       <c r="D26" s="29" t="inlineStr">
@@ -21617,75 +21625,59 @@
           <t>RO, COUR/ section 1, Amphi1, BAHNES N.</t>
         </is>
       </c>
-      <c r="E26" s="17" t="n"/>
+      <c r="E26" s="17" t="inlineStr">
+        <is>
+          <t>FDD, TP/ G3, C4, HABIB ZAHMANI M</t>
+        </is>
+      </c>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>RO, TP/ G1, C4,  MIROUD</t>
-        </is>
-      </c>
-      <c r="H26" s="17" t="inlineStr">
-        <is>
-          <t>SMA, TP/ G1, M1, MEROUFEL B.</t>
-        </is>
-      </c>
+          <t>RO, TP/ G3, M1, BAHNES N.</t>
+        </is>
+      </c>
+      <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
       <c r="B27" s="27" t="inlineStr">
         <is>
-          <t>RO, TP/ G2, A2,  MIROUD</t>
+          <t>FDD, TP/ G2, A1, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="31" t="n"/>
-      <c r="E27" s="27" t="n"/>
+      <c r="E27" s="27" t="inlineStr">
+        <is>
+          <t>RO, TP/ G4, M1, BAHNES N.</t>
+        </is>
+      </c>
       <c r="F27" s="27" t="n"/>
       <c r="G27" s="27" t="inlineStr">
         <is>
-          <t>FDD, TP/ G2, C3, HABIB ZAHMANI M</t>
-        </is>
-      </c>
-      <c r="H27" s="27" t="inlineStr">
-        <is>
-          <t>FDD, TP/ G3, C4, HABIB ZAHMANI M</t>
-        </is>
-      </c>
+          <t>FDD, TP/ G4, C4, HABIB ZAHMANI M</t>
+        </is>
+      </c>
+      <c r="H27" s="27" t="n"/>
     </row>
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
-      <c r="B28" s="27" t="inlineStr">
-        <is>
-          <t>RO, TP/ G3, A3, BAHNES N.</t>
-        </is>
-      </c>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="31" t="n"/>
       <c r="E28" s="27" t="n"/>
       <c r="F28" s="27" t="n"/>
-      <c r="G28" s="27" t="inlineStr">
-        <is>
-          <t>SMA, TP/ G3, M2, MEROUFEL B.</t>
-        </is>
-      </c>
+      <c r="G28" s="27" t="n"/>
       <c r="H28" s="27" t="n"/>
     </row>
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
-      <c r="B29" s="27" t="inlineStr">
-        <is>
-          <t>SMA, TP/ G4, A4, MEROUFEL B.</t>
-        </is>
-      </c>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="31" t="n"/>
       <c r="D29" s="31" t="n"/>
       <c r="E29" s="27" t="n"/>
       <c r="F29" s="27" t="n"/>
-      <c r="G29" s="27" t="inlineStr">
-        <is>
-          <t>RO, TP/ G4, M1, BAHNES N.</t>
-        </is>
-      </c>
+      <c r="G29" s="27" t="n"/>
       <c r="H29" s="27" t="n"/>
     </row>
     <row r="30" ht="21.75" customHeight="1" s="24">
@@ -21754,25 +21746,29 @@
           <t>SMA, COUR/ section 1, Amphi3, MEROUFEL B.</t>
         </is>
       </c>
-      <c r="D35" s="17" t="inlineStr">
-        <is>
-          <t>SMA, TP/ G2, A3, MEROUFEL B.</t>
-        </is>
-      </c>
-      <c r="E35" s="17" t="n"/>
-      <c r="F35" s="17" t="n"/>
-      <c r="G35" s="17" t="n"/>
+      <c r="D35" s="17" t="n"/>
+      <c r="E35" s="17" t="inlineStr">
+        <is>
+          <t>SMA, TP/ G1, M2, MEROUFEL B.</t>
+        </is>
+      </c>
+      <c r="F35" s="17" t="inlineStr">
+        <is>
+          <t>SMA, TP/ G2, M1, MEROUFEL B.</t>
+        </is>
+      </c>
+      <c r="G35" s="17" t="inlineStr">
+        <is>
+          <t>SMA, TP/ G3, C3, MEROUFEL B.</t>
+        </is>
+      </c>
       <c r="H35" s="17" t="n"/>
     </row>
     <row r="36" ht="21.75" customHeight="1" s="24">
       <c r="A36" s="30" t="n"/>
       <c r="B36" s="31" t="n"/>
       <c r="C36" s="31" t="n"/>
-      <c r="D36" s="27" t="inlineStr">
-        <is>
-          <t>FDD, TP/ G4, A2, HABIB ZAHMANI M</t>
-        </is>
-      </c>
+      <c r="D36" s="27" t="n"/>
       <c r="E36" s="27" t="n"/>
       <c r="F36" s="27" t="n"/>
       <c r="G36" s="27" t="n"/>
@@ -21854,7 +21850,11 @@
           <t>Jeudi</t>
         </is>
       </c>
-      <c r="B44" s="17" t="n"/>
+      <c r="B44" s="17" t="inlineStr">
+        <is>
+          <t>SMA, TP/ G4, A4, MEROUFEL B.</t>
+        </is>
+      </c>
       <c r="C44" s="17" t="n"/>
       <c r="D44" s="17" t="n"/>
       <c r="E44" s="17" t="n"/>
@@ -23064,19 +23064,23 @@
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>GSR, TP/ G1, A4, LAREDJ A.</t>
+          <t>GSR, TD/ G1, S9, LAREDJ A.</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
+          <t>RO, TD/ G1, S10, BAHNES N.</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>GSR, TP/ G1, C3, LAREDJ A.</t>
+        </is>
+      </c>
+      <c r="H8" s="17" t="inlineStr">
+        <is>
           <t>VS, TP/ G1, A4, FILALI F.</t>
-        </is>
-      </c>
-      <c r="G8" s="17" t="n"/>
-      <c r="H8" s="17" t="inlineStr">
-        <is>
-          <t>GSR, TD/ G1, S1, LAREDJ A.</t>
         </is>
       </c>
     </row>
@@ -23168,27 +23172,31 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ASBDA, COUR/ section 1, B1, HABIB ZAHMANI M</t>
+          <t>SRI, COUR/ section 1, B1, BENTAOUZA C</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>PR, COUR/ section 1, C2, HOCINE N.</t>
+          <t>ASBDA, COUR/ section 1, B4, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G1, S10, KHIAT</t>
+          <t>AOSI, TD/ G1, S9, KHIAT</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>RO, TD/ G1, S10, BAHNES N.</t>
+          <t>AOSI, TP/ G1, M2, KHIAT</t>
         </is>
       </c>
       <c r="G17" s="17" t="n"/>
-      <c r="H17" s="17" t="n"/>
+      <c r="H17" s="17" t="inlineStr">
+        <is>
+          <t>PR, TP/ G1, M2, HOCINE N.</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
@@ -23278,31 +23286,23 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>SRI, COUR/ section 1, B1, BENTAOUZA C</t>
+          <t>PR, COUR/ section 1, B1, HOCINE N.</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>AOSI, COUR/ section 1, B1, KHELIFA N.</t>
-        </is>
-      </c>
-      <c r="D26" s="17" t="n"/>
-      <c r="E26" s="17" t="inlineStr">
-        <is>
-          <t>SRI, TP/ G1, M2, BENTAOUZA C</t>
-        </is>
-      </c>
+          <t>AOSI, COUR/ section 1, B4, KHELIFA N.</t>
+        </is>
+      </c>
+      <c r="D26" s="17" t="inlineStr">
+        <is>
+          <t>SRI, TP/ G1, C4, BENTAOUZA C</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="n"/>
-      <c r="G26" s="17" t="inlineStr">
-        <is>
-          <t>PR, TP/ G1, M3, HOCINE N.</t>
-        </is>
-      </c>
-      <c r="H26" s="17" t="inlineStr">
-        <is>
-          <t>AOSI, TP/ G1, M2, KHIAT</t>
-        </is>
-      </c>
+      <c r="G26" s="17" t="n"/>
+      <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
@@ -24700,17 +24700,25 @@
           <t>TO2, COUR/ section 1, B4, M. B. BENDOUKHA</t>
         </is>
       </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>AC2, TD/ G1, S12, M. BELAIDI Benharrat</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
+      <c r="D8" s="17" t="inlineStr">
+        <is>
+          <t>AC2, TD/ G1, S8, M. BELAIDI Benharrat</t>
+        </is>
+      </c>
+      <c r="E8" s="17" t="n"/>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>TO2, TD/ G1, S9, M. B. BENDOUKHA</t>
+        </is>
+      </c>
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>GéoDiff2, TD/ G1, S10, M. BELARBI Lakehal</t>
+        </is>
+      </c>
       <c r="H8" s="17" t="inlineStr">
         <is>
-          <t>TO2, TD/ G1, Amphi3, M. B. BENDOUKHA</t>
+          <t>GéoDiff2, TD/ G1, S9, M. BELARBI Lakehal</t>
         </is>
       </c>
     </row>
@@ -24807,28 +24815,28 @@
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>Dis2, COUR/ section 1, S12, M. BOUZIT Hamid</t>
+          <t>Dis2, COUR/ section 1, C1, M. BOUZIT Hamid</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>AC2, TD/ G1, S9, M. BELAIDI Benharrat</t>
+          <t>AC2, TD/ G1, S8, M. BELAIDI Benharrat</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>GéoDiff2, TD/ G1, S9, M. BELARBI Lakehal</t>
+          <t>Dis2, TD/ G1, S6, M. BOUZIT Hamid</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>GéoDiff2, TD/ G1, S6, M. BELARBI Lakehal</t>
+          <t>EDP2, TD/ G1, S12, M. Andasmas M</t>
         </is>
       </c>
       <c r="H17" s="17" t="inlineStr">
         <is>
-          <t>Dis2, TD/ G1, S14, M. BOUZIT Hamid</t>
+          <t>EDP2, TD/ G1, S13, M. Andasmas M</t>
         </is>
       </c>
     </row>
@@ -24925,25 +24933,21 @@
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>STAT2, COUR/ section 1, B2, Mlle Dj.BENSIKADDOUR</t>
+          <t>STAT2, COUR/ section 1, C1, Mlle Dj.BENSIKADDOUR</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>EDP2, TD/ G1, B3, M. Andasmas M</t>
+          <t>STAT2, TD/ G1, S13, Mlle Dj.BENSIKADDOUR</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>STAT2, TD/ G1, B2, Mlle Dj.BENSIKADDOUR</t>
-        </is>
-      </c>
-      <c r="G26" s="17" t="inlineStr">
-        <is>
-          <t>SEMIGROUP, TD/ G1, B1, Mlle Medeghri Ahmed</t>
-        </is>
-      </c>
+          <t>SEMIGROUP, TD/ G1, B4, Mlle Medeghri Ahmed</t>
+        </is>
+      </c>
+      <c r="G26" s="17" t="n"/>
       <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
@@ -25042,11 +25046,7 @@
           <t>Anglais2, COUR/ section 1, B2, M. Dahmani Z.</t>
         </is>
       </c>
-      <c r="D35" s="17" t="inlineStr">
-        <is>
-          <t>EDP2, TD/ G1, B1, M. Andasmas M</t>
-        </is>
-      </c>
+      <c r="D35" s="17" t="n"/>
       <c r="E35" s="17" t="n"/>
       <c r="F35" s="17" t="n"/>
       <c r="G35" s="17" t="n"/>

</xml_diff>

<commit_message>
solver code refactoring,runtime assertions, comments
</commit_message>
<xml_diff>
--- a/src/FSEI_Mosta_EDT.xlsx
+++ b/src/FSEI_Mosta_EDT.xlsx
@@ -2779,12 +2779,12 @@
           <t>TG, COUR/ section 1, B4, Mr Ablaoui H.</t>
         </is>
       </c>
-      <c r="D26" s="17" t="n"/>
-      <c r="E26" s="17" t="inlineStr">
-        <is>
-          <t>TG, TP/ G1, M2, Mr Ablaoui H.</t>
-        </is>
-      </c>
+      <c r="D26" s="17" t="inlineStr">
+        <is>
+          <t>TG, TP/ G1, M3, Mr Ablaoui H.</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="inlineStr">
         <is>
           <t>PROGQUAD, TP/ G1, M2, M. AMIR A.</t>
@@ -4229,7 +4229,7 @@
       <c r="F9" s="27" t="n"/>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>Info2, TP/ G2, M2, Adda</t>
+          <t>Info2, TP/ G2, M1, Adda</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="C26" s="17" t="inlineStr">
         <is>
-          <t>Info2, TP/ G3, A4, Adda</t>
+          <t>Info2, TP/ G3, A3, Adda</t>
         </is>
       </c>
       <c r="D26" s="29" t="inlineStr">
@@ -17927,7 +17927,7 @@
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G1, A1, HOCINE</t>
+          <t>DSS, TP/ G1, A1, DELALI A.</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -17974,14 +17974,10 @@
       </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>IA, TP/ G3, A2, HOCINE</t>
-        </is>
-      </c>
-      <c r="G10" s="27" t="inlineStr">
-        <is>
           <t>DSS, TP/ G3, A2, DELALI A.</t>
         </is>
       </c>
+      <c r="G10" s="27" t="n"/>
       <c r="H10" s="27" t="n"/>
     </row>
     <row r="11" ht="21.75" customHeight="1" s="24">
@@ -17990,15 +17986,11 @@
       <c r="C11" s="31" t="n"/>
       <c r="D11" s="27" t="inlineStr">
         <is>
-          <t>IA, TP/ G4, A2, HOCINE</t>
+          <t>DSS, TP/ G4, A2, DELALI A.</t>
         </is>
       </c>
       <c r="E11" s="27" t="n"/>
-      <c r="F11" s="27" t="inlineStr">
-        <is>
-          <t>DSS, TP/ G4, A3, DELALI A.</t>
-        </is>
-      </c>
+      <c r="F11" s="27" t="n"/>
       <c r="G11" s="27" t="n"/>
       <c r="H11" s="27" t="n"/>
     </row>
@@ -18085,7 +18077,7 @@
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G1, M1, DELALI A.</t>
+          <t>AP, TP/ G4, C4, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -18096,7 +18088,7 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>IA, TP/ G2, A2, HOCINE</t>
+          <t>DSS, TP/ G2, A2, DELALI A.</t>
         </is>
       </c>
       <c r="E18" s="27" t="inlineStr">
@@ -18111,7 +18103,7 @@
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G4, C4, MECHAOUI M. D.G</t>
+          <t>DSS, TP/ G5, M1, DELALI A.</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -18127,7 +18119,7 @@
       </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t>IA, TP/ G7, A3, HOCINE</t>
+          <t>DSS, TP/ G7, A3, DELALI A.</t>
         </is>
       </c>
       <c r="F19" s="27" t="inlineStr">
@@ -18148,11 +18140,7 @@
         </is>
       </c>
       <c r="E20" s="27" t="n"/>
-      <c r="F20" s="27" t="inlineStr">
-        <is>
-          <t>IA, TP/ G6, M2, HOCINE</t>
-        </is>
-      </c>
+      <c r="F20" s="27" t="n"/>
       <c r="G20" s="27" t="n"/>
       <c r="H20" s="27" t="n"/>
     </row>
@@ -18219,23 +18207,23 @@
       </c>
       <c r="C26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G2, A3, DELALI A.</t>
+          <t>IA, TP/ G1, A2, HOCINE N.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G5, A4, DELALI A.</t>
+          <t>DSS, TP/ G6, A4, DELALI A.</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G6, M1, DELALI A.</t>
+          <t>IA, TP/ G2, M1, HOCINE N.</t>
         </is>
       </c>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G7, M3, DELALI A.</t>
+          <t>IA, TP/ G3, M3, HOCINE N.</t>
         </is>
       </c>
       <c r="H26" s="17" t="n"/>
@@ -18245,7 +18233,7 @@
       <c r="B27" s="31" t="n"/>
       <c r="C27" s="27" t="inlineStr">
         <is>
-          <t>IA, TP/ G5, A2, HOCINE</t>
+          <t>AP, TP/ G6, A1, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="D27" s="27" t="inlineStr">
@@ -18263,7 +18251,7 @@
       <c r="B28" s="31" t="n"/>
       <c r="C28" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G6, A1, MECHAOUI M. D.G</t>
+          <t>SI, TD/ G7, B1, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="D28" s="27" t="n"/>
@@ -18275,11 +18263,7 @@
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
       <c r="B29" s="31" t="n"/>
-      <c r="C29" s="27" t="inlineStr">
-        <is>
-          <t>SI, TD/ G7, B1, BENIDRIS F.Z</t>
-        </is>
-      </c>
+      <c r="C29" s="27" t="n"/>
       <c r="D29" s="27" t="n"/>
       <c r="E29" s="27" t="n"/>
       <c r="F29" s="27" t="n"/>
@@ -18342,11 +18326,27 @@
           <t>Mercredi</t>
         </is>
       </c>
-      <c r="B35" s="17" t="n"/>
-      <c r="C35" s="17" t="n"/>
+      <c r="B35" s="17" t="inlineStr">
+        <is>
+          <t>IA, TP/ G4, C4, HOCINE N.</t>
+        </is>
+      </c>
+      <c r="C35" s="17" t="inlineStr">
+        <is>
+          <t>IA, TP/ G5, C4, HOCINE N.</t>
+        </is>
+      </c>
       <c r="D35" s="17" t="n"/>
-      <c r="E35" s="17" t="n"/>
-      <c r="F35" s="17" t="n"/>
+      <c r="E35" s="17" t="inlineStr">
+        <is>
+          <t>IA, TP/ G6, C3, HOCINE N.</t>
+        </is>
+      </c>
+      <c r="F35" s="17" t="inlineStr">
+        <is>
+          <t>IA, TP/ G7, M2, HOCINE N.</t>
+        </is>
+      </c>
       <c r="G35" s="17" t="n"/>
       <c r="H35" s="17" t="n"/>
     </row>
@@ -22975,12 +22975,12 @@
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G1, A4, MOUSSA M.</t>
+          <t>ALOS, TP/ G1, A3, MOUSSA M.</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>SSI, TP/ G1, C3, BENTAOUZA C</t>
+          <t>SSI, TP/ G1, A4, BENTAOUZA C</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -23002,7 +23002,7 @@
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>RO, TP/ G2, C4,  MIROUD</t>
+          <t>RO, TP/ G2, C3,  MIROUD</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -23019,12 +23019,12 @@
       <c r="E10" s="27" t="n"/>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>SSI, TP/ G3, C3, BENTAOUZA C</t>
+          <t>SSI, TP/ G3, A4, BENTAOUZA C</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G3, A3, KHELIFA N.</t>
+          <t>AOSI, TP/ G3, A2, KHELIFA N.</t>
         </is>
       </c>
       <c r="H10" s="27" t="n"/>
@@ -23046,7 +23046,7 @@
       </c>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G4, A4, MOUSSA M.</t>
+          <t>ALOS, TP/ G4, A3, MOUSSA M.</t>
         </is>
       </c>
       <c r="H11" s="27" t="n"/>
@@ -23125,7 +23125,7 @@
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G2, M3, KHIAT</t>
+          <t>RO, TP/ G1, M3,  MIROUD</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
@@ -23145,7 +23145,11 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="31" t="n"/>
       <c r="E18" s="27" t="n"/>
-      <c r="F18" s="27" t="n"/>
+      <c r="F18" s="27" t="inlineStr">
+        <is>
+          <t>AOSI, TP/ G2, M2, KHIAT</t>
+        </is>
+      </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
           <t>RO, TP/ G3, M3, BAHNES N.</t>
@@ -23249,13 +23253,17 @@
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>RO, TP/ G1, C4,  MIROUD</t>
-        </is>
-      </c>
-      <c r="E26" s="17" t="n"/>
+          <t>SMA, TP/ G1, M1, MEROUFEL B.</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="inlineStr">
+        <is>
+          <t>FDD, TP/ G3, M2, HABIB ZAHMANI M</t>
+        </is>
+      </c>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G1, C4, MEROUFEL B.</t>
+          <t>SMA, TP/ G2, C4, MEROUFEL B.</t>
         </is>
       </c>
       <c r="G26" s="17" t="n"/>
@@ -23273,7 +23281,7 @@
       <c r="E27" s="27" t="n"/>
       <c r="F27" s="27" t="inlineStr">
         <is>
-          <t>FDD, TP/ G3, C3, HABIB ZAHMANI M</t>
+          <t>FDD, TP/ G4, C3, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="G27" s="27" t="n"/>
@@ -23285,7 +23293,7 @@
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="27" t="inlineStr">
         <is>
-          <t>SMA, TP/ G3, M2, MEROUFEL B.</t>
+          <t>RO, TP/ G4, C4, BAHNES N.</t>
         </is>
       </c>
       <c r="E28" s="27" t="n"/>
@@ -23297,11 +23305,7 @@
       <c r="A29" s="30" t="n"/>
       <c r="B29" s="31" t="n"/>
       <c r="C29" s="31" t="n"/>
-      <c r="D29" s="27" t="inlineStr">
-        <is>
-          <t>RO, TP/ G4, M1, BAHNES N.</t>
-        </is>
-      </c>
+      <c r="D29" s="27" t="n"/>
       <c r="E29" s="27" t="n"/>
       <c r="F29" s="27" t="n"/>
       <c r="G29" s="27" t="n"/>
@@ -23376,12 +23380,12 @@
       <c r="D35" s="17" t="n"/>
       <c r="E35" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G2, C4, MEROUFEL B.</t>
+          <t>SMA, TP/ G3, C4, MEROUFEL B.</t>
         </is>
       </c>
       <c r="F35" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G4, M2, MEROUFEL B.</t>
+          <t>SMA, TP/ G4, M3, MEROUFEL B.</t>
         </is>
       </c>
       <c r="G35" s="17" t="n"/>
@@ -23392,11 +23396,7 @@
       <c r="B36" s="31" t="n"/>
       <c r="C36" s="31" t="n"/>
       <c r="D36" s="27" t="n"/>
-      <c r="E36" s="27" t="inlineStr">
-        <is>
-          <t>FDD, TP/ G4, C3, HABIB ZAHMANI M</t>
-        </is>
-      </c>
+      <c r="E36" s="27" t="n"/>
       <c r="F36" s="27" t="n"/>
       <c r="G36" s="27" t="n"/>
       <c r="H36" s="27" t="n"/>
@@ -24698,7 +24698,7 @@
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>GSR, TP/ G1, M1, LAREDJ A.</t>
+          <t>GSR, TP/ G1, C4, LAREDJ A.</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -24907,7 +24907,7 @@
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>VS, TP/ G1, M3, FILALI F.</t>
+          <t>VS, TP/ G1, M2, FILALI F.</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
@@ -25018,15 +25018,15 @@
       <c r="D35" s="17" t="n"/>
       <c r="E35" s="17" t="inlineStr">
         <is>
+          <t>AOSI, TP/ G1, M1, KHIAT</t>
+        </is>
+      </c>
+      <c r="F35" s="17" t="n"/>
+      <c r="G35" s="17" t="inlineStr">
+        <is>
           <t>PR, TP/ G1, M1, HOCINE N.</t>
         </is>
       </c>
-      <c r="F35" s="17" t="inlineStr">
-        <is>
-          <t>AOSI, TP/ G1, M3, KHIAT</t>
-        </is>
-      </c>
-      <c r="G35" s="17" t="n"/>
       <c r="H35" s="17" t="n"/>
     </row>
     <row r="36" ht="21.75" customHeight="1" s="24">

</xml_diff>

<commit_message>
relational (prof,mod,multiplicity)* add in gui bindings 50%
</commit_message>
<xml_diff>
--- a/src/FSEI_Mosta_EDT.xlsx
+++ b/src/FSEI_Mosta_EDT.xlsx
@@ -708,32 +708,32 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>ANA2, COUR/ section 1, Amphi1, Mr Bouzit H</t>
+          <t>ANA2, COUR/ section 1, Amphi4, Mr Bouzit H</t>
         </is>
       </c>
       <c r="C8" s="17" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G1, B1, Mme Bouabdelli</t>
+          <t>ANA2, TD/ G1, S1, Mme Bouabdelli</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G1, B4, Mme Diala.H</t>
+          <t>ALG2, TD/ G1, S10, Mme Diala.H</t>
         </is>
       </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G3, B2, Mme Diala.H</t>
+          <t>ALG2, TD/ G3, S8, Mme Diala.H</t>
         </is>
       </c>
       <c r="F8" s="29" t="inlineStr">
         <is>
-          <t>ALG2, COUR/ section 1, Amphi1, M. Medeghri Ahmed</t>
+          <t>ALG2, COUR/ section 1, Amphi4, M. Medeghri Ahmed</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G1, B3, HABIB ZAHMANI M</t>
+          <t>ASD2, TD/ G1, S9, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -743,23 +743,23 @@
       <c r="B9" s="31" t="n"/>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G2, B4, Mme Diala.H</t>
+          <t>ALG2, TD/ G2, S10, Mme Diala.H</t>
         </is>
       </c>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G2, B1, Mme Bouabdelli</t>
+          <t>ANA2, TD/ G2, S1, Mme Bouabdelli</t>
         </is>
       </c>
       <c r="E9" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G4, B4, BENAMEUR</t>
+          <t>ASD2, TD/ G4, S10, BENAMEUR</t>
         </is>
       </c>
       <c r="F9" s="31" t="n"/>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G3, B4, MOUMEN</t>
+          <t>ASD2, TD/ G3, S10, MOUMEN</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -769,23 +769,23 @@
       <c r="B10" s="31" t="n"/>
       <c r="C10" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G3, B2, Mlle FERRAOUN A.</t>
+          <t>ANA2, TD/ G3, S8, Mlle FERRAOUN A.</t>
         </is>
       </c>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G4, B2, Mlle FERRAOUN A.</t>
+          <t>ANA2, TD/ G4, S8, Mlle FERRAOUN A.</t>
         </is>
       </c>
       <c r="E10" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G6, B3, Mme SAIDANI</t>
+          <t>ALG2, TD/ G6, S9, Mme SAIDANI</t>
         </is>
       </c>
       <c r="F10" s="31" t="n"/>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G5, B1, Mme Diala.H</t>
+          <t>ALG2, TD/ G5, S1, Mme Diala.H</t>
         </is>
       </c>
       <c r="H10" s="27" t="n"/>
@@ -795,23 +795,23 @@
       <c r="B11" s="31" t="n"/>
       <c r="C11" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G5, B3, M. Kaid</t>
+          <t>ANA2, TD/ G5, S9, M. Kaid</t>
         </is>
       </c>
       <c r="D11" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G6, B3, M. Kaid</t>
+          <t>ANA2, TD/ G6, S9, M. Kaid</t>
         </is>
       </c>
       <c r="E11" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G7, B1, M. Kaid</t>
+          <t>ANA2, TD/ G7, S1, M. Kaid</t>
         </is>
       </c>
       <c r="F11" s="31" t="n"/>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G7, B2, Mme SAIDANI</t>
+          <t>ALG2, TD/ G7, S8, Mme SAIDANI</t>
         </is>
       </c>
       <c r="H11" s="27" t="n"/>
@@ -874,32 +874,32 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ANA2, COUR/ section 1, Amphi1, Mr Bouzit H</t>
+          <t>ANA2, COUR/ section 1, Amphi4, Mr Bouzit H</t>
         </is>
       </c>
       <c r="C17" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G2, B2, HABIB ZAHMANI M</t>
+          <t>ASD2, TD/ G2, S8, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="D17" s="29" t="inlineStr">
         <is>
-          <t>ASD2, COUR/ section 1, Amphi1, HENNI F</t>
+          <t>ASD2, COUR/ section 1, Amphi4, HENNI F</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G1, A1, HABIB ZAHMANI M</t>
+          <t>ASD2, TP/ G1, M3, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G1, B1, DJAHAFI</t>
+          <t>SM2, TD/ G1, S1, DJAHAFI</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G2, B1, DJAHAFI</t>
+          <t>SM2, TD/ G2, S1, DJAHAFI</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -909,23 +909,23 @@
       <c r="B18" s="31" t="n"/>
       <c r="C18" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G4, B1, Mme Diala.H</t>
+          <t>ALG2, TD/ G4, S1, Mme Diala.H</t>
         </is>
       </c>
       <c r="D18" s="31" t="n"/>
       <c r="E18" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G3, A2, MOUMEN</t>
+          <t>ASD2, TP/ G3, M2, MOUMEN</t>
         </is>
       </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G2, A1, HABIB ZAHMANI M</t>
+          <t>ASD2, TP/ G2, M3, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G3, B3, Mlle Benaouad</t>
+          <t>IPSD, TD/ G3, S9, Mlle Benaouad</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -935,23 +935,23 @@
       <c r="B19" s="31" t="n"/>
       <c r="C19" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G5, B3, BENAMEUR</t>
+          <t>ASD2, TD/ G5, S9, BENAMEUR</t>
         </is>
       </c>
       <c r="D19" s="31" t="n"/>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G6, B1, BENAMEUR</t>
+          <t>ASD2, TD/ G6, S1, BENAMEUR</t>
         </is>
       </c>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G4, A2, BENAMEUR</t>
+          <t>ASD2, TP/ G4, M2, BENAMEUR</t>
         </is>
       </c>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G4, B2, HAMAMI</t>
+          <t>SM2, TD/ G4, S8, HAMAMI</t>
         </is>
       </c>
       <c r="H19" s="27" t="n"/>
@@ -961,19 +961,19 @@
       <c r="B20" s="31" t="n"/>
       <c r="C20" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G7, B4, BENSALLOUA</t>
+          <t>ASD2, TD/ G7, S10, BENSALLOUA</t>
         </is>
       </c>
       <c r="D20" s="31" t="n"/>
       <c r="E20" s="27" t="n"/>
       <c r="F20" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G7, A3, BENSALLOUA</t>
+          <t>ASD2, TP/ G7, M1, BENSALLOUA</t>
         </is>
       </c>
       <c r="G20" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G5, A1, BENAMEUR</t>
+          <t>ASD2, TP/ G5, M3, BENAMEUR</t>
         </is>
       </c>
       <c r="H20" s="27" t="n"/>
@@ -1036,32 +1036,32 @@
       </c>
       <c r="B26" s="17" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G1, B3, Mlle Zelmat Souhila</t>
+          <t>IPSD, TD/ G1, S9, Mlle Zelmat Souhila</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>SM2, COUR/ section 1, Amphi1, HASSAINE</t>
+          <t>SM2, COUR/ section 1, Amphi4, HASSAINE</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G2, B2, Mlle Zelmat Souhila</t>
+          <t>IPSD, TD/ G2, S8, Mlle Zelmat Souhila</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G1, A1, Mlle Lakeb Ouda</t>
+          <t>OPM, TP/ G1, M3, Mlle Lakeb Ouda</t>
         </is>
       </c>
       <c r="F26" s="29" t="inlineStr">
         <is>
-          <t>IPSD, COUR/ section 1, Amphi1, Mlle Dj. BENSIKADDOUR</t>
+          <t>IPSD, COUR/ section 1, Amphi4, Mlle Dj. BENSIKADDOUR</t>
         </is>
       </c>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G1, B3, Mekemmeche</t>
+          <t>PHY2, TD/ G1, S9, Mekemmeche</t>
         </is>
       </c>
       <c r="H26" s="17" t="n"/>
@@ -1070,24 +1070,24 @@
       <c r="A27" s="30" t="n"/>
       <c r="B27" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G3, B1, DJAHAFI</t>
+          <t>SM2, TD/ G3, S1, DJAHAFI</t>
         </is>
       </c>
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G4, B3, Mlle Benaouad</t>
+          <t>IPSD, TD/ G4, S9, Mlle Benaouad</t>
         </is>
       </c>
       <c r="E27" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G2, B2, Mekemmeche</t>
+          <t>PHY2, TD/ G2, S8, Mekemmeche</t>
         </is>
       </c>
       <c r="F27" s="31" t="n"/>
       <c r="G27" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G4, A1, Mlle Bouzid</t>
+          <t>OPM, TP/ G4, M3, Mlle Bouzid</t>
         </is>
       </c>
       <c r="H27" s="27" t="n"/>
@@ -1096,24 +1096,24 @@
       <c r="A28" s="30" t="n"/>
       <c r="B28" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G5, B2, HAMAMI</t>
+          <t>SM2, TD/ G5, S8, HAMAMI</t>
         </is>
       </c>
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G5, B4, M. Benzidane</t>
+          <t>IPSD, TD/ G5, S10, M. Benzidane</t>
         </is>
       </c>
       <c r="E28" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G3, A2, Mlle Bouzid</t>
+          <t>OPM, TP/ G3, M2, Mlle Bouzid</t>
         </is>
       </c>
       <c r="F28" s="31" t="n"/>
       <c r="G28" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G6, B1, M. Benzidane</t>
+          <t>IPSD, TD/ G6, S1, M. Benzidane</t>
         </is>
       </c>
       <c r="H28" s="27" t="n"/>
@@ -1122,24 +1122,24 @@
       <c r="A29" s="30" t="n"/>
       <c r="B29" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G6, A1, BENAMEUR</t>
+          <t>ASD2, TP/ G6, M3, BENAMEUR</t>
         </is>
       </c>
       <c r="C29" s="31" t="n"/>
       <c r="D29" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G6, B1, HAMAMI</t>
+          <t>SM2, TD/ G6, S1, HAMAMI</t>
         </is>
       </c>
       <c r="E29" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G7, B1, HAMAMI</t>
+          <t>SM2, TD/ G7, S1, HAMAMI</t>
         </is>
       </c>
       <c r="F29" s="31" t="n"/>
       <c r="G29" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G7, B2, Mme Kaisserli</t>
+          <t>IPSD, TD/ G7, S8, Mme Kaisserli</t>
         </is>
       </c>
       <c r="H29" s="27" t="n"/>
@@ -1202,32 +1202,32 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>TIC, COUR/ section 1, Amphi1, HENNI K.</t>
+          <t>TIC, COUR/ section 1, Amphi4, HENNI K.</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>OPM, COUR/ section 1, Amphi1, Mlle Ali Merina.H</t>
+          <t>OPM, COUR/ section 1, Amphi4, Mlle Ali Merina.H</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G2, A1, Mlle Lakeb Ouda</t>
+          <t>OPM, TP/ G2, M3, Mlle Lakeb Ouda</t>
         </is>
       </c>
       <c r="E35" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G4, B1, Mekemmeche</t>
+          <t>PHY2, TD/ G4, S1, Mekemmeche</t>
         </is>
       </c>
       <c r="F35" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G5, B1, Mekemmeche</t>
+          <t>PHY2, TD/ G5, S1, Mekemmeche</t>
         </is>
       </c>
       <c r="G35" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G7, B1, Labdelli</t>
+          <t>PHY2, TD/ G7, S1, Labdelli</t>
         </is>
       </c>
       <c r="H35" s="17" t="n"/>
@@ -1238,17 +1238,17 @@
       <c r="C36" s="31" t="n"/>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G3, B1, Mekemmeche</t>
+          <t>PHY2, TD/ G3, S1, Mekemmeche</t>
         </is>
       </c>
       <c r="E36" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G7, A1, Mlle Hamou Maamar.M</t>
+          <t>OPM, TP/ G7, M3, Mlle Hamou Maamar.M</t>
         </is>
       </c>
       <c r="F36" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G6, B2, Labdelli</t>
+          <t>PHY2, TD/ G6, S8, Labdelli</t>
         </is>
       </c>
       <c r="G36" s="27" t="n"/>
@@ -1260,7 +1260,7 @@
       <c r="C37" s="31" t="n"/>
       <c r="D37" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G5, A2, Mlle Bouzid</t>
+          <t>OPM, TP/ G5, M2, Mlle Bouzid</t>
         </is>
       </c>
       <c r="E37" s="27" t="n"/>
@@ -1274,7 +1274,7 @@
       <c r="C38" s="31" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G6, A3, Mlle Hamou Maamar.M</t>
+          <t>OPM, TP/ G6, M1, Mlle Hamou Maamar.M</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>PHY2, COUR/ section 1, Amphi1, M. Benchehida</t>
+          <t>PHY2, COUR/ section 1, Amphi4, M. Benchehida</t>
         </is>
       </c>
       <c r="C44" s="17" t="n"/>
@@ -2543,28 +2543,28 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>Mod2, COUR/ section 1, C1, Mlle Bouzid Leila</t>
+          <t>Mod2, COUR/ section 1, S7, Mlle Bouzid Leila</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>OAF 2, COUR/ section 1, S12, Mr S. M. Bahri</t>
+          <t>OAF 2, COUR/ section 1, S6, Mr S. M. Bahri</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>Mod2, TD/ G1, S1, Mlle Bouzid Leila</t>
+          <t>Mod2, TD/ G1, B1, Mlle Bouzid Leila</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>OAF 2, TD/ G1, S16, Mr S. M. Bahri</t>
+          <t>OAF 2, TD/ G1, B4, Mr S. M. Bahri</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>TCONTROL, TD/ G1, S2, Mr. BOUAGADA</t>
+          <t>TCONTROL, TD/ G1, B3, Mr. BOUAGADA</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -2657,28 +2657,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>OAF 2, COUR/ section 1, B3, Mr S. M. Bahri</t>
+          <t>OAF 2, COUR/ section 1, S10, Mr S. M. Bahri</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>TCONTROL, COUR/ section 1, S12, Mr. BOUAGADA</t>
+          <t>TCONTROL, COUR/ section 1, S6, Mr. BOUAGADA</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>CFRAC, TD/ G1, S8, M. Zoubir DAHMANI</t>
+          <t>CFRAC, TD/ G1, C1, M. Zoubir DAHMANI</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>TG, TD/ G1, S11, Mr Ablaoui H.</t>
+          <t>TG, TD/ G1, S13, Mr Ablaoui H.</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>PROGQUAD, TD/ G1, S7, M. AMIR A.</t>
+          <t>PROGQUAD, TD/ G1, S14, M. AMIR A.</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -2771,23 +2771,23 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>CFRAC, COUR/ section 1, C2, M. Zoubir DAHMANI</t>
+          <t>CFRAC, COUR/ section 1, S7, M. Zoubir DAHMANI</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>TG, COUR/ section 1, B4, Mr Ablaoui H.</t>
+          <t>TG, COUR/ section 1, S10, Mr Ablaoui H.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>TG, TP/ G1, M3, Mr Ablaoui H.</t>
+          <t>TG, TP/ G1, A1, Mr Ablaoui H.</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>PROGQUAD, TP/ G1, M2, M. AMIR A.</t>
+          <t>PROGQUAD, TP/ G1, A2, M. AMIR A.</t>
         </is>
       </c>
       <c r="G26" s="17" t="n"/>
@@ -2881,12 +2881,12 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>PROGQUAD, COUR/ section 1, B3, M. AMIR A.</t>
+          <t>PROGQUAD, COUR/ section 1, S10, M. AMIR A.</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>Latex, COUR/ section 1, B3, Mme Bouabdelli</t>
+          <t>Latex, COUR/ section 1, S10, Mme Bouabdelli</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>Anglais, COUR/ section 1, B1, M. Dahmani Z.</t>
+          <t>Anglais, COUR/ section 1, S8, M. Dahmani Z.</t>
         </is>
       </c>
       <c r="C44" s="17" t="n"/>
@@ -4186,28 +4186,28 @@
       </c>
       <c r="B8" s="17" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G1, C2, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G1, S6, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="C8" s="17" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G1, S14, Hamiani</t>
+          <t>Chim2, TD/ G1, S4, Hamiani</t>
         </is>
       </c>
       <c r="D8" s="29" t="inlineStr">
         <is>
-          <t>Maths2, COUR/ section 1, Amphi2, Mme.Bechaoui</t>
+          <t>Maths2, COUR/ section 1, Amphi3, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="E8" s="29" t="inlineStr">
         <is>
-          <t>Chim2, COUR/ section 1, Amphi1, Belhachemi</t>
+          <t>Chim2, COUR/ section 1, Amphi4, Belhachemi</t>
         </is>
       </c>
       <c r="F8" s="17" t="n"/>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G1, Amphi3, Benguettat</t>
+          <t>Phys2, TD/ G1, Amphi4, Benguettat</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -4216,12 +4216,12 @@
       <c r="A9" s="30" t="n"/>
       <c r="B9" s="27" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G2, S12, Belhachemi</t>
+          <t>Chim2, TD/ G2, S5, Belhachemi</t>
         </is>
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G2, S13, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G2, S5, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="D9" s="31" t="n"/>
@@ -4229,7 +4229,7 @@
       <c r="F9" s="27" t="n"/>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>Info2, TP/ G2, M1, Adda</t>
+          <t>Info2, TP/ G2, A3, Adda</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -4238,12 +4238,12 @@
       <c r="A10" s="30" t="n"/>
       <c r="B10" s="27" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G3, S13, Benguettat</t>
+          <t>Phys2, TD/ G3, S4, Benguettat</t>
         </is>
       </c>
       <c r="C10" s="27" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G3, S15, Belhachemi</t>
+          <t>Chim2, TD/ G3, S16, Belhachemi</t>
         </is>
       </c>
       <c r="D10" s="31" t="n"/>
@@ -4251,7 +4251,7 @@
       <c r="F10" s="27" t="n"/>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G3, S3, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G3, B2, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="H10" s="27" t="n"/>
@@ -4260,12 +4260,12 @@
       <c r="A11" s="30" t="n"/>
       <c r="B11" s="27" t="inlineStr">
         <is>
-          <t>Info2, TP/ G4, A3, Adda</t>
+          <t>Info2, TP/ G4, M1, Adda</t>
         </is>
       </c>
       <c r="C11" s="27" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G4, S4, Benguettat</t>
+          <t>Phys2, TD/ G4, S15, Benguettat</t>
         </is>
       </c>
       <c r="D11" s="31" t="n"/>
@@ -4273,7 +4273,7 @@
       <c r="F11" s="27" t="n"/>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G4, S1, Belhachemi</t>
+          <t>Chim2, TD/ G4, B1, Belhachemi</t>
         </is>
       </c>
       <c r="H11" s="27" t="n"/>
@@ -4336,28 +4336,28 @@
       </c>
       <c r="B17" s="17" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G1, B4, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G1, S11, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="C17" s="17" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G1, S14, Hamiani</t>
+          <t>Chim2, TD/ G1, S4, Hamiani</t>
         </is>
       </c>
       <c r="D17" s="29" t="inlineStr">
         <is>
-          <t>Maths2, COUR/ section 1, Amphi3, Mme.Bechaoui</t>
+          <t>Maths2, COUR/ section 1, Amphi2, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="E17" s="29" t="inlineStr">
         <is>
-          <t>Chim2, COUR/ section 1, Amphi1, Belhachemi</t>
+          <t>Chim2, COUR/ section 1, Amphi4, Belhachemi</t>
         </is>
       </c>
       <c r="F17" s="17" t="n"/>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G1, S9, Benguettat</t>
+          <t>Phys2, TD/ G1, C2, Benguettat</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -4366,12 +4366,12 @@
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="27" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G2, C1, Belhachemi</t>
+          <t>Chim2, TD/ G2, S7, Belhachemi</t>
         </is>
       </c>
       <c r="C18" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G2, S13, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G2, S5, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="D18" s="31" t="n"/>
@@ -4379,7 +4379,7 @@
       <c r="F18" s="27" t="n"/>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G3, S11, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G3, S13, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -4388,12 +4388,12 @@
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="27" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G3, C2, Benguettat</t>
+          <t>Phys2, TD/ G3, S6, Benguettat</t>
         </is>
       </c>
       <c r="C19" s="27" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G3, S15, Belhachemi</t>
+          <t>Chim2, TD/ G3, S16, Belhachemi</t>
         </is>
       </c>
       <c r="D19" s="31" t="n"/>
@@ -4401,7 +4401,7 @@
       <c r="F19" s="27" t="n"/>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>Chim2, TD/ G4, S10, Belhachemi</t>
+          <t>Chim2, TD/ G4, S12, Belhachemi</t>
         </is>
       </c>
       <c r="H19" s="27" t="n"/>
@@ -4411,7 +4411,7 @@
       <c r="B20" s="27" t="n"/>
       <c r="C20" s="27" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G4, S4, Benguettat</t>
+          <t>Phys2, TD/ G4, S15, Benguettat</t>
         </is>
       </c>
       <c r="D20" s="31" t="n"/>
@@ -4478,22 +4478,22 @@
       </c>
       <c r="B26" s="17" t="inlineStr">
         <is>
-          <t>Info2, TP/ G1, A2, Adda</t>
+          <t>Info2, TP/ G1, M2, Adda</t>
         </is>
       </c>
       <c r="C26" s="17" t="inlineStr">
         <is>
-          <t>Info2, TP/ G3, A3, Adda</t>
+          <t>Info2, TP/ G3, M1, Adda</t>
         </is>
       </c>
       <c r="D26" s="29" t="inlineStr">
         <is>
-          <t>Phys2, COUR/ section 1, Amphi1, Mr.Senouci</t>
+          <t>Phys2, COUR/ section 1, Amphi4, Mr.Senouci</t>
         </is>
       </c>
       <c r="E26" s="29" t="inlineStr">
         <is>
-          <t>Info2, COUR/ section 1, Amphi1, Adda</t>
+          <t>Info2, COUR/ section 1, Amphi4, Adda</t>
         </is>
       </c>
       <c r="F26" s="17" t="n"/>
@@ -4504,7 +4504,7 @@
       <c r="A27" s="30" t="n"/>
       <c r="B27" s="27" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G2, S13, Benguettat</t>
+          <t>Phys2, TD/ G2, S5, Benguettat</t>
         </is>
       </c>
       <c r="C27" s="27" t="n"/>
@@ -4518,7 +4518,7 @@
       <c r="A28" s="30" t="n"/>
       <c r="B28" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G4, S12, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G4, S6, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="C28" s="27" t="n"/>
@@ -4596,17 +4596,17 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>Phys2, COUR/ section 1, Amphi4, Mr.Senouci</t>
+          <t>Phys2, COUR/ section 1, Amphi1, Mr.Senouci</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>HisSci, COUR/ section 1, Amphi4, Benguettat</t>
+          <t>HisSci, COUR/ section 1, Amphi1, Benguettat</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>Phys2, TD/ G2, C1, Benguettat</t>
+          <t>Phys2, TD/ G2, S11, Benguettat</t>
         </is>
       </c>
       <c r="E35" s="17" t="n"/>
@@ -4620,7 +4620,7 @@
       <c r="C36" s="31" t="n"/>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>Maths2, TD/ G4, B4, Mme.Bechaoui</t>
+          <t>Maths2, TD/ G4, S10, Mme.Bechaoui</t>
         </is>
       </c>
       <c r="E36" s="27" t="n"/>
@@ -5904,28 +5904,28 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>Thdyna, COUR/ section 1, S14, Hentit H</t>
+          <t>Thdyna, COUR/ section 1, S2, Hentit H</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>FVC, COUR/ section 1, S5, Latreuch</t>
-        </is>
-      </c>
-      <c r="D8" s="17" t="inlineStr">
-        <is>
-          <t>Thdyna, TD/ G1, Amphi3, Hentit H</t>
-        </is>
-      </c>
-      <c r="E8" s="17" t="n"/>
+          <t>FVC, COUR/ section 1, S14, Latreuch</t>
+        </is>
+      </c>
+      <c r="D8" s="17" t="n"/>
+      <c r="E8" s="17" t="inlineStr">
+        <is>
+          <t>Thdyna, TD/ G1, S14, Hentit H</t>
+        </is>
+      </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>FVC, TD/ G1, S2, Latreuch</t>
+          <t>FVC, TD/ G1, B3, Latreuch</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>MQ, TD/ G1, Amphi4, Meghoufel</t>
+          <t>MQ, TD/ G1, Amphi3, Meghoufel</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -6018,28 +6018,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>Thdyna, COUR/ section 1, S12, Hentit H</t>
+          <t>Thdyna, COUR/ section 1, S5, Hentit H</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>FVC, COUR/ section 1, S5, Latreuch</t>
+          <t>FVC, COUR/ section 1, S14, Latreuch</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>Thdyna, TD/ G1, S16, Hentit H</t>
+          <t>Thdyna, TD/ G1, B4, Hentit H</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>FVC, TD/ G1, S10, Latreuch</t>
+          <t>FVC, TD/ G1, S12, Latreuch</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>MQ, TD/ G1, S8, Meghoufel</t>
+          <t>MQ, TD/ G1, C1, Meghoufel</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -6132,17 +6132,17 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>MQ, COUR/ section 1, S14, Meghoufel</t>
+          <t>MQ, COUR/ section 1, S4, Meghoufel</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>elecmag, COUR/ section 1, C1, Abbes</t>
+          <t>elecmag, COUR/ section 1, S11, Abbes</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>elecmag, TD/ G1, S11, Abbes</t>
+          <t>elecmag, TD/ G1, S13, Abbes</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
@@ -6238,17 +6238,17 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>MQ, COUR/ section 1, B4, Meghoufel</t>
+          <t>MQ, COUR/ section 1, S11, Meghoufel</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>elecmag, COUR/ section 1, B4, Abbes</t>
+          <t>elecmag, COUR/ section 1, S11, Abbes</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>elecmag, TD/ G1, C2, Abbes</t>
+          <t>elecmag, TD/ G1, S7, Abbes</t>
         </is>
       </c>
       <c r="E35" s="17" t="n"/>
@@ -6344,12 +6344,12 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>elecgen, COUR/ section 1, B2, Melati</t>
+          <t>elecgen, COUR/ section 1, S9, Melati</t>
         </is>
       </c>
       <c r="C44" s="29" t="inlineStr">
         <is>
-          <t>elecgen, COUR/ section 1, B1, Melati</t>
+          <t>elecgen, COUR/ section 1, S1, Melati</t>
         </is>
       </c>
       <c r="D44" s="17" t="n"/>
@@ -7552,23 +7552,23 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>PhysSol, COUR/ section 1, S15, Bouattou</t>
+          <t>PhysSol, COUR/ section 1, S16, Bouattou</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>PhysNuc, COUR/ section 1, S6, Abbassa</t>
-        </is>
-      </c>
-      <c r="D8" s="17" t="inlineStr">
-        <is>
-          <t>PhysSol, TD/ G1, Amphi4, Bouattou</t>
-        </is>
-      </c>
-      <c r="E8" s="17" t="n"/>
+          <t>PhysNuc, COUR/ section 1, S13, Abbassa</t>
+        </is>
+      </c>
+      <c r="D8" s="17" t="n"/>
+      <c r="E8" s="17" t="inlineStr">
+        <is>
+          <t>PhysSol, TD/ G1, S13, Bouattou</t>
+        </is>
+      </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>PhysNuc, TD/ G1, S3, Abbassa</t>
+          <t>PhysNuc, TD/ G1, B2, Abbassa</t>
         </is>
       </c>
       <c r="G8" s="17" t="n"/>
@@ -7662,28 +7662,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>PhysSol, COUR/ section 1, S13, Bouattou</t>
+          <t>PhysSol, COUR/ section 1, S4, Bouattou</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>PhysNuc, COUR/ section 1, S6, Abbassa</t>
+          <t>PhysNuc, COUR/ section 1, S13, Abbassa</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>PhysSol, TD/ G1, S2, Bouattou</t>
+          <t>PhysSol, TD/ G1, B3, Bouattou</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>PhysNuc, TD/ G1, S9, Abbassa</t>
+          <t>PhysNuc, TD/ G1, C2, Abbassa</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>TransCha, TD/ G1, S16, Boukra</t>
+          <t>TransCha, TD/ G1, B4, Boukra</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -7776,23 +7776,23 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>TransCha, COUR/ section 1, S15, Boukra</t>
+          <t>TransCha, COUR/ section 1, S16, Boukra</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>PhysAto, COUR/ section 1, C2, Beghdad</t>
+          <t>PhysAto, COUR/ section 1, S7, Beghdad</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>TransCha, TD/ G1, S10, Boukra</t>
+          <t>TransCha, TD/ G1, S12, Boukra</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>PhysAto, TD/ G1, S12, Beghdad</t>
+          <t>PhysAto, TD/ G1, S6, Beghdad</t>
         </is>
       </c>
       <c r="G26" s="17" t="n"/>
@@ -7886,17 +7886,17 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>TransCha, COUR/ section 1, C1, Boukra</t>
+          <t>TransCha, COUR/ section 1, S7, Boukra</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>PhysAto, COUR/ section 1, C1, Beghdad</t>
+          <t>PhysAto, COUR/ section 1, S7, Beghdad</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>PhysAto, TD/ G1, S12, Beghdad</t>
+          <t>PhysAto, TD/ G1, S6, Beghdad</t>
         </is>
       </c>
       <c r="E35" s="17" t="n"/>
@@ -9188,114 +9188,114 @@
           <t>Dimanche</t>
         </is>
       </c>
-      <c r="B8" s="29" t="inlineStr">
-        <is>
-          <t>ChiOrg2, COUR/ section 1, S3, Kadi</t>
-        </is>
-      </c>
-      <c r="C8" s="29" t="inlineStr">
-        <is>
-          <t>ThermoCin, COUR/ section 1, S3, Belayachi</t>
-        </is>
-      </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>ChiOrg2, TD/ G1, S7, Kadi</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="inlineStr">
-        <is>
-          <t>ThermoCin, TD/ G1, Amphi3, Belayachi</t>
-        </is>
-      </c>
+      <c r="B8" s="17" t="inlineStr">
+        <is>
+          <t>ChiOrg2, TD/ G1, S15, Kadi</t>
+        </is>
+      </c>
+      <c r="C8" s="17" t="inlineStr">
+        <is>
+          <t>ThermoCin, TD/ G1, C2, Belayachi</t>
+        </is>
+      </c>
+      <c r="D8" s="29" t="inlineStr">
+        <is>
+          <t>ChiOrg2, COUR/ section 1, Amphi2, Kadi</t>
+        </is>
+      </c>
+      <c r="E8" s="29" t="inlineStr">
+        <is>
+          <t>ThermoCin, COUR/ section 1, Amphi3, Belayachi</t>
+        </is>
+      </c>
+      <c r="F8" s="17" t="n"/>
       <c r="G8" s="17" t="n"/>
       <c r="H8" s="17" t="n"/>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
-      <c r="B9" s="31" t="n"/>
-      <c r="C9" s="31" t="n"/>
-      <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>ThermoCin, TD/ G2, S11, Belayachi</t>
-        </is>
-      </c>
-      <c r="F9" s="27" t="inlineStr">
-        <is>
-          <t>ChiOrg2, TD/ G2, S1, Kadi</t>
-        </is>
-      </c>
+      <c r="B9" s="27" t="inlineStr">
+        <is>
+          <t>ThermoCin, TD/ G2, S14, Belayachi</t>
+        </is>
+      </c>
+      <c r="C9" s="27" t="inlineStr">
+        <is>
+          <t>ChiOrg2, TD/ G2, S12, Kadi</t>
+        </is>
+      </c>
+      <c r="D9" s="31" t="n"/>
+      <c r="E9" s="31" t="n"/>
+      <c r="F9" s="27" t="n"/>
       <c r="G9" s="27" t="n"/>
       <c r="H9" s="27" t="n"/>
     </row>
     <row r="10" ht="21.75" customHeight="1" s="24">
       <c r="A10" s="30" t="n"/>
-      <c r="B10" s="31" t="n"/>
-      <c r="C10" s="31" t="n"/>
-      <c r="D10" s="27" t="n"/>
-      <c r="E10" s="27" t="n"/>
+      <c r="B10" s="27" t="n"/>
+      <c r="C10" s="27" t="n"/>
+      <c r="D10" s="31" t="n"/>
+      <c r="E10" s="31" t="n"/>
       <c r="F10" s="27" t="n"/>
       <c r="G10" s="27" t="n"/>
       <c r="H10" s="27" t="n"/>
     </row>
     <row r="11" ht="21.75" customHeight="1" s="24">
       <c r="A11" s="30" t="n"/>
-      <c r="B11" s="31" t="n"/>
-      <c r="C11" s="31" t="n"/>
-      <c r="D11" s="27" t="n"/>
-      <c r="E11" s="27" t="n"/>
+      <c r="B11" s="27" t="n"/>
+      <c r="C11" s="27" t="n"/>
+      <c r="D11" s="31" t="n"/>
+      <c r="E11" s="31" t="n"/>
       <c r="F11" s="27" t="n"/>
       <c r="G11" s="27" t="n"/>
       <c r="H11" s="27" t="n"/>
     </row>
     <row r="12" ht="21.75" customHeight="1" s="24">
       <c r="A12" s="30" t="n"/>
-      <c r="B12" s="31" t="n"/>
-      <c r="C12" s="31" t="n"/>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
+      <c r="B12" s="27" t="n"/>
+      <c r="C12" s="27" t="n"/>
+      <c r="D12" s="31" t="n"/>
+      <c r="E12" s="31" t="n"/>
       <c r="F12" s="27" t="n"/>
       <c r="G12" s="27" t="n"/>
       <c r="H12" s="27" t="n"/>
     </row>
     <row r="13" ht="21.75" customHeight="1" s="24">
       <c r="A13" s="30" t="n"/>
-      <c r="B13" s="31" t="n"/>
-      <c r="C13" s="31" t="n"/>
-      <c r="D13" s="27" t="n"/>
-      <c r="E13" s="27" t="n"/>
+      <c r="B13" s="27" t="n"/>
+      <c r="C13" s="27" t="n"/>
+      <c r="D13" s="31" t="n"/>
+      <c r="E13" s="31" t="n"/>
       <c r="F13" s="27" t="n"/>
       <c r="G13" s="27" t="n"/>
       <c r="H13" s="27" t="n"/>
     </row>
     <row r="14" ht="21.75" customHeight="1" s="24">
       <c r="A14" s="30" t="n"/>
-      <c r="B14" s="31" t="n"/>
-      <c r="C14" s="31" t="n"/>
-      <c r="D14" s="27" t="n"/>
-      <c r="E14" s="27" t="n"/>
+      <c r="B14" s="27" t="n"/>
+      <c r="C14" s="27" t="n"/>
+      <c r="D14" s="31" t="n"/>
+      <c r="E14" s="31" t="n"/>
       <c r="F14" s="27" t="n"/>
       <c r="G14" s="27" t="n"/>
       <c r="H14" s="27" t="n"/>
     </row>
     <row r="15" ht="21.75" customHeight="1" s="24">
       <c r="A15" s="30" t="n"/>
-      <c r="B15" s="31" t="n"/>
-      <c r="C15" s="31" t="n"/>
-      <c r="D15" s="27" t="n"/>
-      <c r="E15" s="27" t="n"/>
+      <c r="B15" s="27" t="n"/>
+      <c r="C15" s="27" t="n"/>
+      <c r="D15" s="31" t="n"/>
+      <c r="E15" s="31" t="n"/>
       <c r="F15" s="27" t="n"/>
       <c r="G15" s="27" t="n"/>
       <c r="H15" s="27" t="n"/>
     </row>
     <row r="16" ht="21.75" customHeight="1" s="24">
       <c r="A16" s="32" t="n"/>
-      <c r="B16" s="33" t="n"/>
-      <c r="C16" s="33" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
+      <c r="B16" s="16" t="n"/>
+      <c r="C16" s="16" t="n"/>
+      <c r="D16" s="33" t="n"/>
+      <c r="E16" s="33" t="n"/>
       <c r="F16" s="16" t="n"/>
       <c r="G16" s="16" t="n"/>
       <c r="H16" s="16" t="n"/>
@@ -9308,28 +9308,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ChiOrg2, COUR/ section 1, S3, Kadi</t>
-        </is>
-      </c>
-      <c r="C17" s="29" t="inlineStr">
-        <is>
-          <t>ThermoCin, COUR/ section 1, S3, Belayachi</t>
-        </is>
-      </c>
-      <c r="D17" s="17" t="inlineStr">
-        <is>
-          <t>ChimAna, TD/ G1, S3, Bourada</t>
+          <t>ChiOrg2, COUR/ section 1, S2, Kadi</t>
+        </is>
+      </c>
+      <c r="C17" s="17" t="inlineStr">
+        <is>
+          <t>ChimAna, TD/ G1, S12, Bourada</t>
+        </is>
+      </c>
+      <c r="D17" s="29" t="inlineStr">
+        <is>
+          <t>ThermoCin, COUR/ section 1, Amphi1, Belayachi</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>ChiQuan, TD/ G1, S16, Boulenouar</t>
+          <t>ChiQuan, TD/ G1, B4, Boulenouar</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>ChimInorg, TD/ G1, S2, Messaoudi</t>
+          <t>ChimInorg, TD/ G1, B3, Messaoudi</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -9337,16 +9337,16 @@
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="31" t="n"/>
-      <c r="C18" s="31" t="n"/>
-      <c r="D18" s="27" t="inlineStr">
-        <is>
-          <t>ChiQuan, TD/ G2, S1, Boulenouar</t>
-        </is>
-      </c>
+      <c r="C18" s="27" t="inlineStr">
+        <is>
+          <t>ChiQuan, TD/ G2, C2, Boulenouar</t>
+        </is>
+      </c>
+      <c r="D18" s="31" t="n"/>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>ChimAna, TD/ G2, S8, Bourada</t>
+          <t>ChimAna, TD/ G2, C1, Bourada</t>
         </is>
       </c>
       <c r="G18" s="27" t="n"/>
@@ -9355,8 +9355,8 @@
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="31" t="n"/>
-      <c r="C19" s="31" t="n"/>
-      <c r="D19" s="27" t="n"/>
+      <c r="C19" s="27" t="n"/>
+      <c r="D19" s="31" t="n"/>
       <c r="E19" s="27" t="n"/>
       <c r="F19" s="27" t="n"/>
       <c r="G19" s="27" t="n"/>
@@ -9365,8 +9365,8 @@
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
       <c r="B20" s="31" t="n"/>
-      <c r="C20" s="31" t="n"/>
-      <c r="D20" s="27" t="n"/>
+      <c r="C20" s="27" t="n"/>
+      <c r="D20" s="31" t="n"/>
       <c r="E20" s="27" t="n"/>
       <c r="F20" s="27" t="n"/>
       <c r="G20" s="27" t="n"/>
@@ -9375,8 +9375,8 @@
     <row r="21" ht="21.75" customHeight="1" s="24">
       <c r="A21" s="30" t="n"/>
       <c r="B21" s="31" t="n"/>
-      <c r="C21" s="31" t="n"/>
-      <c r="D21" s="27" t="n"/>
+      <c r="C21" s="27" t="n"/>
+      <c r="D21" s="31" t="n"/>
       <c r="E21" s="27" t="n"/>
       <c r="F21" s="27" t="n"/>
       <c r="G21" s="27" t="n"/>
@@ -9385,8 +9385,8 @@
     <row r="22" ht="21.75" customHeight="1" s="24">
       <c r="A22" s="30" t="n"/>
       <c r="B22" s="31" t="n"/>
-      <c r="C22" s="31" t="n"/>
-      <c r="D22" s="27" t="n"/>
+      <c r="C22" s="27" t="n"/>
+      <c r="D22" s="31" t="n"/>
       <c r="E22" s="27" t="n"/>
       <c r="F22" s="27" t="n"/>
       <c r="G22" s="27" t="n"/>
@@ -9395,8 +9395,8 @@
     <row r="23" ht="21.75" customHeight="1" s="24">
       <c r="A23" s="30" t="n"/>
       <c r="B23" s="31" t="n"/>
-      <c r="C23" s="31" t="n"/>
-      <c r="D23" s="27" t="n"/>
+      <c r="C23" s="27" t="n"/>
+      <c r="D23" s="31" t="n"/>
       <c r="E23" s="27" t="n"/>
       <c r="F23" s="27" t="n"/>
       <c r="G23" s="27" t="n"/>
@@ -9405,8 +9405,8 @@
     <row r="24" ht="21.75" customHeight="1" s="24">
       <c r="A24" s="30" t="n"/>
       <c r="B24" s="31" t="n"/>
-      <c r="C24" s="31" t="n"/>
-      <c r="D24" s="27" t="n"/>
+      <c r="C24" s="27" t="n"/>
+      <c r="D24" s="31" t="n"/>
       <c r="E24" s="27" t="n"/>
       <c r="F24" s="27" t="n"/>
       <c r="G24" s="27" t="n"/>
@@ -9415,8 +9415,8 @@
     <row r="25" ht="21.75" customHeight="1" s="24">
       <c r="A25" s="32" t="n"/>
       <c r="B25" s="33" t="n"/>
-      <c r="C25" s="33" t="n"/>
-      <c r="D25" s="16" t="n"/>
+      <c r="C25" s="16" t="n"/>
+      <c r="D25" s="33" t="n"/>
       <c r="E25" s="16" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="16" t="n"/>
@@ -9428,19 +9428,19 @@
           <t>Mardi</t>
         </is>
       </c>
-      <c r="B26" s="29" t="inlineStr">
-        <is>
-          <t>ChimAna, COUR/ section 1, S3, Bourada</t>
+      <c r="B26" s="17" t="inlineStr">
+        <is>
+          <t>ChimInorg, TD/ G2, S15, Messaoudi</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>ChiQuan, COUR/ section 1, S3, Benmalti</t>
-        </is>
-      </c>
-      <c r="D26" s="17" t="inlineStr">
-        <is>
-          <t>ChimInorg, TD/ G2, S9, Messaoudi</t>
+          <t>ChimAna, COUR/ section 1, S16, Bourada</t>
+        </is>
+      </c>
+      <c r="D26" s="29" t="inlineStr">
+        <is>
+          <t>ChiQuan, COUR/ section 1, Amphi3, Benmalti</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
@@ -9450,9 +9450,9 @@
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
-      <c r="B27" s="31" t="n"/>
+      <c r="B27" s="27" t="n"/>
       <c r="C27" s="31" t="n"/>
-      <c r="D27" s="27" t="n"/>
+      <c r="D27" s="31" t="n"/>
       <c r="E27" s="27" t="n"/>
       <c r="F27" s="27" t="n"/>
       <c r="G27" s="27" t="n"/>
@@ -9460,9 +9460,9 @@
     </row>
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
-      <c r="B28" s="31" t="n"/>
+      <c r="B28" s="27" t="n"/>
       <c r="C28" s="31" t="n"/>
-      <c r="D28" s="27" t="n"/>
+      <c r="D28" s="31" t="n"/>
       <c r="E28" s="27" t="n"/>
       <c r="F28" s="27" t="n"/>
       <c r="G28" s="27" t="n"/>
@@ -9470,9 +9470,9 @@
     </row>
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
-      <c r="B29" s="31" t="n"/>
+      <c r="B29" s="27" t="n"/>
       <c r="C29" s="31" t="n"/>
-      <c r="D29" s="27" t="n"/>
+      <c r="D29" s="31" t="n"/>
       <c r="E29" s="27" t="n"/>
       <c r="F29" s="27" t="n"/>
       <c r="G29" s="27" t="n"/>
@@ -9480,9 +9480,9 @@
     </row>
     <row r="30" ht="21.75" customHeight="1" s="24">
       <c r="A30" s="30" t="n"/>
-      <c r="B30" s="31" t="n"/>
+      <c r="B30" s="27" t="n"/>
       <c r="C30" s="31" t="n"/>
-      <c r="D30" s="27" t="n"/>
+      <c r="D30" s="31" t="n"/>
       <c r="E30" s="27" t="n"/>
       <c r="F30" s="27" t="n"/>
       <c r="G30" s="27" t="n"/>
@@ -9490,9 +9490,9 @@
     </row>
     <row r="31" ht="21.75" customHeight="1" s="24">
       <c r="A31" s="30" t="n"/>
-      <c r="B31" s="31" t="n"/>
+      <c r="B31" s="27" t="n"/>
       <c r="C31" s="31" t="n"/>
-      <c r="D31" s="27" t="n"/>
+      <c r="D31" s="31" t="n"/>
       <c r="E31" s="27" t="n"/>
       <c r="F31" s="27" t="n"/>
       <c r="G31" s="27" t="n"/>
@@ -9500,9 +9500,9 @@
     </row>
     <row r="32" ht="21.75" customHeight="1" s="24">
       <c r="A32" s="30" t="n"/>
-      <c r="B32" s="31" t="n"/>
+      <c r="B32" s="27" t="n"/>
       <c r="C32" s="31" t="n"/>
-      <c r="D32" s="27" t="n"/>
+      <c r="D32" s="31" t="n"/>
       <c r="E32" s="27" t="n"/>
       <c r="F32" s="27" t="n"/>
       <c r="G32" s="27" t="n"/>
@@ -9510,9 +9510,9 @@
     </row>
     <row r="33" ht="21.75" customHeight="1" s="24">
       <c r="A33" s="30" t="n"/>
-      <c r="B33" s="31" t="n"/>
+      <c r="B33" s="27" t="n"/>
       <c r="C33" s="31" t="n"/>
-      <c r="D33" s="27" t="n"/>
+      <c r="D33" s="31" t="n"/>
       <c r="E33" s="27" t="n"/>
       <c r="F33" s="27" t="n"/>
       <c r="G33" s="27" t="n"/>
@@ -9520,9 +9520,9 @@
     </row>
     <row r="34" ht="21.75" customHeight="1" s="24">
       <c r="A34" s="32" t="n"/>
-      <c r="B34" s="33" t="n"/>
+      <c r="B34" s="16" t="n"/>
       <c r="C34" s="33" t="n"/>
-      <c r="D34" s="16" t="n"/>
+      <c r="D34" s="33" t="n"/>
       <c r="E34" s="16" t="n"/>
       <c r="F34" s="16" t="n"/>
       <c r="G34" s="16" t="n"/>
@@ -9536,12 +9536,12 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>ChimInorg, COUR/ section 1, S3, Messaoudi</t>
+          <t>ChimInorg, COUR/ section 1, S2, Messaoudi</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>Anglais 4, COUR/ section 1, S3, harrats</t>
+          <t>Anglais 4, COUR/ section 1, S2, harrats</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -9638,7 +9638,7 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>TAPC2, COUR/ section 1, S3, belhalfaoui</t>
+          <t>TAPC2, COUR/ section 1, S2, belhalfaoui</t>
         </is>
       </c>
       <c r="C44" s="17" t="n"/>
@@ -10708,12 +10708,12 @@
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B8:B16"/>
-    <mergeCell ref="C8:C16"/>
+    <mergeCell ref="D8:D16"/>
+    <mergeCell ref="E8:E16"/>
     <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C17:C25"/>
-    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="D17:D25"/>
     <mergeCell ref="C26:C34"/>
+    <mergeCell ref="D26:D34"/>
     <mergeCell ref="B35:B43"/>
     <mergeCell ref="C35:C43"/>
     <mergeCell ref="B44:B52"/>
@@ -10839,110 +10839,114 @@
           <t>Dimanche</t>
         </is>
       </c>
-      <c r="B8" s="29" t="inlineStr">
-        <is>
-          <t>TS, COUR/ section 1, S1, Belhakem</t>
-        </is>
-      </c>
-      <c r="C8" s="29" t="inlineStr">
-        <is>
-          <t>SpecMol, COUR/ section 1, S1, Belouatek</t>
-        </is>
-      </c>
-      <c r="D8" s="17" t="n"/>
-      <c r="E8" s="17" t="inlineStr">
-        <is>
-          <t>TS, TD/ G1, S10, Belhakem</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="inlineStr">
-        <is>
-          <t>TS, TD/ G2, Amphi4, Belhakem</t>
-        </is>
-      </c>
+      <c r="B8" s="17" t="inlineStr">
+        <is>
+          <t>TS, TD/ G1, S13, Belhakem</t>
+        </is>
+      </c>
+      <c r="C8" s="17" t="inlineStr">
+        <is>
+          <t>SpecMol, TD/ G1, B4, Belouatek</t>
+        </is>
+      </c>
+      <c r="D8" s="29" t="inlineStr">
+        <is>
+          <t>TS, COUR/ section 1, Amphi1, Belhakem</t>
+        </is>
+      </c>
+      <c r="E8" s="29" t="inlineStr">
+        <is>
+          <t>SpecMol, COUR/ section 1, Amphi2, Belouatek</t>
+        </is>
+      </c>
+      <c r="F8" s="17" t="n"/>
       <c r="G8" s="17" t="n"/>
       <c r="H8" s="17" t="n"/>
     </row>
     <row r="9" ht="21.75" customHeight="1" s="24">
       <c r="A9" s="30" t="n"/>
-      <c r="B9" s="31" t="n"/>
-      <c r="C9" s="31" t="n"/>
-      <c r="D9" s="27" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
-        <is>
-          <t>SpecMol, TD/ G2, S9, Belouatek</t>
-        </is>
-      </c>
+      <c r="B9" s="27" t="inlineStr">
+        <is>
+          <t>SpecMol, TD/ G2, S12, Belouatek</t>
+        </is>
+      </c>
+      <c r="C9" s="27" t="inlineStr">
+        <is>
+          <t>TS, TD/ G2, C1, Belhakem</t>
+        </is>
+      </c>
+      <c r="D9" s="31" t="n"/>
+      <c r="E9" s="31" t="n"/>
       <c r="F9" s="27" t="n"/>
       <c r="G9" s="27" t="n"/>
       <c r="H9" s="27" t="n"/>
     </row>
     <row r="10" ht="21.75" customHeight="1" s="24">
       <c r="A10" s="30" t="n"/>
-      <c r="B10" s="31" t="n"/>
-      <c r="C10" s="31" t="n"/>
-      <c r="D10" s="27" t="n"/>
-      <c r="E10" s="27" t="n"/>
+      <c r="B10" s="27" t="n"/>
+      <c r="C10" s="27" t="n"/>
+      <c r="D10" s="31" t="n"/>
+      <c r="E10" s="31" t="n"/>
       <c r="F10" s="27" t="n"/>
       <c r="G10" s="27" t="n"/>
       <c r="H10" s="27" t="n"/>
     </row>
     <row r="11" ht="21.75" customHeight="1" s="24">
       <c r="A11" s="30" t="n"/>
-      <c r="B11" s="31" t="n"/>
-      <c r="C11" s="31" t="n"/>
-      <c r="D11" s="27" t="n"/>
-      <c r="E11" s="27" t="n"/>
+      <c r="B11" s="27" t="n"/>
+      <c r="C11" s="27" t="n"/>
+      <c r="D11" s="31" t="n"/>
+      <c r="E11" s="31" t="n"/>
       <c r="F11" s="27" t="n"/>
       <c r="G11" s="27" t="n"/>
       <c r="H11" s="27" t="n"/>
     </row>
     <row r="12" ht="21.75" customHeight="1" s="24">
       <c r="A12" s="30" t="n"/>
-      <c r="B12" s="31" t="n"/>
-      <c r="C12" s="31" t="n"/>
-      <c r="D12" s="27" t="n"/>
-      <c r="E12" s="27" t="n"/>
+      <c r="B12" s="27" t="n"/>
+      <c r="C12" s="27" t="n"/>
+      <c r="D12" s="31" t="n"/>
+      <c r="E12" s="31" t="n"/>
       <c r="F12" s="27" t="n"/>
       <c r="G12" s="27" t="n"/>
       <c r="H12" s="27" t="n"/>
     </row>
     <row r="13" ht="21.75" customHeight="1" s="24">
       <c r="A13" s="30" t="n"/>
-      <c r="B13" s="31" t="n"/>
-      <c r="C13" s="31" t="n"/>
-      <c r="D13" s="27" t="n"/>
-      <c r="E13" s="27" t="n"/>
+      <c r="B13" s="27" t="n"/>
+      <c r="C13" s="27" t="n"/>
+      <c r="D13" s="31" t="n"/>
+      <c r="E13" s="31" t="n"/>
       <c r="F13" s="27" t="n"/>
       <c r="G13" s="27" t="n"/>
       <c r="H13" s="27" t="n"/>
     </row>
     <row r="14" ht="21.75" customHeight="1" s="24">
       <c r="A14" s="30" t="n"/>
-      <c r="B14" s="31" t="n"/>
-      <c r="C14" s="31" t="n"/>
-      <c r="D14" s="27" t="n"/>
-      <c r="E14" s="27" t="n"/>
+      <c r="B14" s="27" t="n"/>
+      <c r="C14" s="27" t="n"/>
+      <c r="D14" s="31" t="n"/>
+      <c r="E14" s="31" t="n"/>
       <c r="F14" s="27" t="n"/>
       <c r="G14" s="27" t="n"/>
       <c r="H14" s="27" t="n"/>
     </row>
     <row r="15" ht="21.75" customHeight="1" s="24">
       <c r="A15" s="30" t="n"/>
-      <c r="B15" s="31" t="n"/>
-      <c r="C15" s="31" t="n"/>
-      <c r="D15" s="27" t="n"/>
-      <c r="E15" s="27" t="n"/>
+      <c r="B15" s="27" t="n"/>
+      <c r="C15" s="27" t="n"/>
+      <c r="D15" s="31" t="n"/>
+      <c r="E15" s="31" t="n"/>
       <c r="F15" s="27" t="n"/>
       <c r="G15" s="27" t="n"/>
       <c r="H15" s="27" t="n"/>
     </row>
     <row r="16" ht="21.75" customHeight="1" s="24">
       <c r="A16" s="32" t="n"/>
-      <c r="B16" s="33" t="n"/>
-      <c r="C16" s="33" t="n"/>
-      <c r="D16" s="16" t="n"/>
-      <c r="E16" s="16" t="n"/>
+      <c r="B16" s="16" t="n"/>
+      <c r="C16" s="16" t="n"/>
+      <c r="D16" s="33" t="n"/>
+      <c r="E16" s="33" t="n"/>
       <c r="F16" s="16" t="n"/>
       <c r="G16" s="16" t="n"/>
       <c r="H16" s="16" t="n"/>
@@ -10955,32 +10959,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>TS, COUR/ section 1, S1, Belhakem</t>
-        </is>
-      </c>
-      <c r="C17" s="29" t="inlineStr">
-        <is>
-          <t>SpecMol, COUR/ section 1, S1, Belouatek</t>
+          <t>TS, COUR/ section 1, S16, Belhakem</t>
+        </is>
+      </c>
+      <c r="C17" s="17" t="inlineStr">
+        <is>
+          <t>ElecChemi, TD/ G1, C1, Belayachi</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>ElecChemi, TD/ G1, Amphi4, Belayachi</t>
-        </is>
-      </c>
-      <c r="E17" s="17" t="inlineStr">
-        <is>
-          <t>ElecChemi, TD/ G2, S4, Belayachi</t>
-        </is>
-      </c>
-      <c r="F17" s="17" t="inlineStr">
-        <is>
-          <t>SpecMol, TD/ G1, S2, Belouatek</t>
-        </is>
-      </c>
+          <t>CSC, TD/ G1, B2, Bourahla</t>
+        </is>
+      </c>
+      <c r="E17" s="29" t="inlineStr">
+        <is>
+          <t>ElecChemi, COUR/ section 1, S2, Belayachi</t>
+        </is>
+      </c>
+      <c r="F17" s="17" t="n"/>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>CSC, TD/ G1, S3, Bourahla</t>
+          <t>ElecChemi, TD/ G2, B2, Belayachi</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -10988,23 +10988,23 @@
     <row r="18" ht="21.75" customHeight="1" s="24">
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="31" t="n"/>
-      <c r="C18" s="31" t="n"/>
+      <c r="C18" s="27" t="inlineStr">
+        <is>
+          <t>CSC, TD/ G2, B4, Bourahla</t>
+        </is>
+      </c>
       <c r="D18" s="27" t="n"/>
-      <c r="E18" s="27" t="n"/>
-      <c r="F18" s="27" t="inlineStr">
-        <is>
-          <t>CSC, TD/ G2, S3, Bourahla</t>
-        </is>
-      </c>
+      <c r="E18" s="31" t="n"/>
+      <c r="F18" s="27" t="n"/>
       <c r="G18" s="27" t="n"/>
       <c r="H18" s="27" t="n"/>
     </row>
     <row r="19" ht="21.75" customHeight="1" s="24">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="31" t="n"/>
-      <c r="C19" s="31" t="n"/>
+      <c r="C19" s="27" t="n"/>
       <c r="D19" s="27" t="n"/>
-      <c r="E19" s="27" t="n"/>
+      <c r="E19" s="31" t="n"/>
       <c r="F19" s="27" t="n"/>
       <c r="G19" s="27" t="n"/>
       <c r="H19" s="27" t="n"/>
@@ -11012,9 +11012,9 @@
     <row r="20" ht="21.75" customHeight="1" s="24">
       <c r="A20" s="30" t="n"/>
       <c r="B20" s="31" t="n"/>
-      <c r="C20" s="31" t="n"/>
+      <c r="C20" s="27" t="n"/>
       <c r="D20" s="27" t="n"/>
-      <c r="E20" s="27" t="n"/>
+      <c r="E20" s="31" t="n"/>
       <c r="F20" s="27" t="n"/>
       <c r="G20" s="27" t="n"/>
       <c r="H20" s="27" t="n"/>
@@ -11022,9 +11022,9 @@
     <row r="21" ht="21.75" customHeight="1" s="24">
       <c r="A21" s="30" t="n"/>
       <c r="B21" s="31" t="n"/>
-      <c r="C21" s="31" t="n"/>
+      <c r="C21" s="27" t="n"/>
       <c r="D21" s="27" t="n"/>
-      <c r="E21" s="27" t="n"/>
+      <c r="E21" s="31" t="n"/>
       <c r="F21" s="27" t="n"/>
       <c r="G21" s="27" t="n"/>
       <c r="H21" s="27" t="n"/>
@@ -11032,9 +11032,9 @@
     <row r="22" ht="21.75" customHeight="1" s="24">
       <c r="A22" s="30" t="n"/>
       <c r="B22" s="31" t="n"/>
-      <c r="C22" s="31" t="n"/>
+      <c r="C22" s="27" t="n"/>
       <c r="D22" s="27" t="n"/>
-      <c r="E22" s="27" t="n"/>
+      <c r="E22" s="31" t="n"/>
       <c r="F22" s="27" t="n"/>
       <c r="G22" s="27" t="n"/>
       <c r="H22" s="27" t="n"/>
@@ -11042,9 +11042,9 @@
     <row r="23" ht="21.75" customHeight="1" s="24">
       <c r="A23" s="30" t="n"/>
       <c r="B23" s="31" t="n"/>
-      <c r="C23" s="31" t="n"/>
+      <c r="C23" s="27" t="n"/>
       <c r="D23" s="27" t="n"/>
-      <c r="E23" s="27" t="n"/>
+      <c r="E23" s="31" t="n"/>
       <c r="F23" s="27" t="n"/>
       <c r="G23" s="27" t="n"/>
       <c r="H23" s="27" t="n"/>
@@ -11052,9 +11052,9 @@
     <row r="24" ht="21.75" customHeight="1" s="24">
       <c r="A24" s="30" t="n"/>
       <c r="B24" s="31" t="n"/>
-      <c r="C24" s="31" t="n"/>
+      <c r="C24" s="27" t="n"/>
       <c r="D24" s="27" t="n"/>
-      <c r="E24" s="27" t="n"/>
+      <c r="E24" s="31" t="n"/>
       <c r="F24" s="27" t="n"/>
       <c r="G24" s="27" t="n"/>
       <c r="H24" s="27" t="n"/>
@@ -11062,9 +11062,9 @@
     <row r="25" ht="21.75" customHeight="1" s="24">
       <c r="A25" s="32" t="n"/>
       <c r="B25" s="33" t="n"/>
-      <c r="C25" s="33" t="n"/>
+      <c r="C25" s="16" t="n"/>
       <c r="D25" s="16" t="n"/>
-      <c r="E25" s="16" t="n"/>
+      <c r="E25" s="33" t="n"/>
       <c r="F25" s="16" t="n"/>
       <c r="G25" s="16" t="n"/>
       <c r="H25" s="16" t="n"/>
@@ -11075,98 +11075,98 @@
           <t>Mardi</t>
         </is>
       </c>
-      <c r="B26" s="29" t="inlineStr">
-        <is>
-          <t>ElecChemi, COUR/ section 1, S1, Belayachi</t>
-        </is>
-      </c>
-      <c r="C26" s="29" t="inlineStr">
-        <is>
-          <t>CSC, COUR/ section 1, S1, Bourahla</t>
-        </is>
-      </c>
-      <c r="D26" s="17" t="n"/>
-      <c r="E26" s="17" t="n"/>
+      <c r="B26" s="17" t="n"/>
+      <c r="C26" s="17" t="n"/>
+      <c r="D26" s="29" t="inlineStr">
+        <is>
+          <t>ElecChemi, COUR/ section 1, Amphi2, Belayachi</t>
+        </is>
+      </c>
+      <c r="E26" s="29" t="inlineStr">
+        <is>
+          <t>SpecMol, COUR/ section 1, S3, Belouatek</t>
+        </is>
+      </c>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="17" t="n"/>
       <c r="H26" s="17" t="n"/>
     </row>
     <row r="27" ht="21.75" customHeight="1" s="24">
       <c r="A27" s="30" t="n"/>
-      <c r="B27" s="31" t="n"/>
-      <c r="C27" s="31" t="n"/>
-      <c r="D27" s="27" t="n"/>
-      <c r="E27" s="27" t="n"/>
+      <c r="B27" s="27" t="n"/>
+      <c r="C27" s="27" t="n"/>
+      <c r="D27" s="31" t="n"/>
+      <c r="E27" s="31" t="n"/>
       <c r="F27" s="27" t="n"/>
       <c r="G27" s="27" t="n"/>
       <c r="H27" s="27" t="n"/>
     </row>
     <row r="28" ht="21.75" customHeight="1" s="24">
       <c r="A28" s="30" t="n"/>
-      <c r="B28" s="31" t="n"/>
-      <c r="C28" s="31" t="n"/>
-      <c r="D28" s="27" t="n"/>
-      <c r="E28" s="27" t="n"/>
+      <c r="B28" s="27" t="n"/>
+      <c r="C28" s="27" t="n"/>
+      <c r="D28" s="31" t="n"/>
+      <c r="E28" s="31" t="n"/>
       <c r="F28" s="27" t="n"/>
       <c r="G28" s="27" t="n"/>
       <c r="H28" s="27" t="n"/>
     </row>
     <row r="29" ht="21.75" customHeight="1" s="24">
       <c r="A29" s="30" t="n"/>
-      <c r="B29" s="31" t="n"/>
-      <c r="C29" s="31" t="n"/>
-      <c r="D29" s="27" t="n"/>
-      <c r="E29" s="27" t="n"/>
+      <c r="B29" s="27" t="n"/>
+      <c r="C29" s="27" t="n"/>
+      <c r="D29" s="31" t="n"/>
+      <c r="E29" s="31" t="n"/>
       <c r="F29" s="27" t="n"/>
       <c r="G29" s="27" t="n"/>
       <c r="H29" s="27" t="n"/>
     </row>
     <row r="30" ht="21.75" customHeight="1" s="24">
       <c r="A30" s="30" t="n"/>
-      <c r="B30" s="31" t="n"/>
-      <c r="C30" s="31" t="n"/>
-      <c r="D30" s="27" t="n"/>
-      <c r="E30" s="27" t="n"/>
+      <c r="B30" s="27" t="n"/>
+      <c r="C30" s="27" t="n"/>
+      <c r="D30" s="31" t="n"/>
+      <c r="E30" s="31" t="n"/>
       <c r="F30" s="27" t="n"/>
       <c r="G30" s="27" t="n"/>
       <c r="H30" s="27" t="n"/>
     </row>
     <row r="31" ht="21.75" customHeight="1" s="24">
       <c r="A31" s="30" t="n"/>
-      <c r="B31" s="31" t="n"/>
-      <c r="C31" s="31" t="n"/>
-      <c r="D31" s="27" t="n"/>
-      <c r="E31" s="27" t="n"/>
+      <c r="B31" s="27" t="n"/>
+      <c r="C31" s="27" t="n"/>
+      <c r="D31" s="31" t="n"/>
+      <c r="E31" s="31" t="n"/>
       <c r="F31" s="27" t="n"/>
       <c r="G31" s="27" t="n"/>
       <c r="H31" s="27" t="n"/>
     </row>
     <row r="32" ht="21.75" customHeight="1" s="24">
       <c r="A32" s="30" t="n"/>
-      <c r="B32" s="31" t="n"/>
-      <c r="C32" s="31" t="n"/>
-      <c r="D32" s="27" t="n"/>
-      <c r="E32" s="27" t="n"/>
+      <c r="B32" s="27" t="n"/>
+      <c r="C32" s="27" t="n"/>
+      <c r="D32" s="31" t="n"/>
+      <c r="E32" s="31" t="n"/>
       <c r="F32" s="27" t="n"/>
       <c r="G32" s="27" t="n"/>
       <c r="H32" s="27" t="n"/>
     </row>
     <row r="33" ht="21.75" customHeight="1" s="24">
       <c r="A33" s="30" t="n"/>
-      <c r="B33" s="31" t="n"/>
-      <c r="C33" s="31" t="n"/>
-      <c r="D33" s="27" t="n"/>
-      <c r="E33" s="27" t="n"/>
+      <c r="B33" s="27" t="n"/>
+      <c r="C33" s="27" t="n"/>
+      <c r="D33" s="31" t="n"/>
+      <c r="E33" s="31" t="n"/>
       <c r="F33" s="27" t="n"/>
       <c r="G33" s="27" t="n"/>
       <c r="H33" s="27" t="n"/>
     </row>
     <row r="34" ht="21.75" customHeight="1" s="24">
       <c r="A34" s="32" t="n"/>
-      <c r="B34" s="33" t="n"/>
-      <c r="C34" s="33" t="n"/>
-      <c r="D34" s="16" t="n"/>
-      <c r="E34" s="16" t="n"/>
+      <c r="B34" s="16" t="n"/>
+      <c r="C34" s="16" t="n"/>
+      <c r="D34" s="33" t="n"/>
+      <c r="E34" s="33" t="n"/>
       <c r="F34" s="16" t="n"/>
       <c r="G34" s="16" t="n"/>
       <c r="H34" s="16" t="n"/>
@@ -11179,12 +11179,12 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>ElecChemi, COUR/ section 1, S1, Belayachi</t>
+          <t>CSC, COUR/ section 1, S16, Bourahla</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>CSC, COUR/ section 1, S1, Bourahla</t>
+          <t>Ethique, COUR/ section 1, S16, Hamiani</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -11281,12 +11281,12 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>Ethique, COUR/ section 1, S1, Hamiani</t>
+          <t>CSC, COUR/ section 1, S16, Bourahla</t>
         </is>
       </c>
       <c r="C44" s="29" t="inlineStr">
         <is>
-          <t>Anglais, COUR/ section 1, S16, harrats</t>
+          <t>Anglais, COUR/ section 1, S3, harrats</t>
         </is>
       </c>
       <c r="D44" s="17" t="n"/>
@@ -12355,12 +12355,12 @@
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B8:B16"/>
-    <mergeCell ref="C8:C16"/>
+    <mergeCell ref="D8:D16"/>
+    <mergeCell ref="E8:E16"/>
     <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C17:C25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="C26:C34"/>
+    <mergeCell ref="E17:E25"/>
+    <mergeCell ref="D26:D34"/>
+    <mergeCell ref="E26:E34"/>
     <mergeCell ref="B35:B43"/>
     <mergeCell ref="C35:C43"/>
     <mergeCell ref="B44:B52"/>
@@ -12489,21 +12489,25 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>PhysSemiC, COUR/ section 1, S4, Bencherif</t>
+          <t>PhysSemiC, COUR/ section 1, C2, Bencherif</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>PhysicStat2, COUR/ section 1, S7, Benotsmane</t>
+          <t>PhysicStat2, COUR/ section 1, B3, Benotsmane</t>
         </is>
       </c>
       <c r="D8" s="17" t="n"/>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>PhysSemiC, TD/ G1, S8, Bencherif</t>
-        </is>
-      </c>
-      <c r="F8" s="17" t="n"/>
+          <t>PhysSemiC, TD/ G1, S12, Bencherif</t>
+        </is>
+      </c>
+      <c r="F8" s="17" t="inlineStr">
+        <is>
+          <t>PhysicStat2, TD/ G1, B1, Benotsmane</t>
+        </is>
+      </c>
       <c r="G8" s="17" t="n"/>
       <c r="H8" s="17" t="n"/>
     </row>
@@ -12595,30 +12599,26 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>PhysSemiC, COUR/ section 1, S14, Bencherif</t>
+          <t>PhysSemiC, COUR/ section 1, S15, Bencherif</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>PhysicStat2, COUR/ section 1, S7, Benotsmane</t>
-        </is>
-      </c>
-      <c r="D17" s="17" t="n"/>
-      <c r="E17" s="17" t="inlineStr">
-        <is>
-          <t>PhysicStat2, TD/ G1, S5, Benotsmane</t>
-        </is>
-      </c>
+          <t>PhysicStat2, COUR/ section 1, B3, Benotsmane</t>
+        </is>
+      </c>
+      <c r="D17" s="17" t="inlineStr">
+        <is>
+          <t>MNS, TD/ G1, B1, Belhouari</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>MNS, TD/ G1, S1, Belhouari</t>
-        </is>
-      </c>
-      <c r="G17" s="17" t="inlineStr">
-        <is>
-          <t>SAM, TD/ G1, S1, Terki</t>
-        </is>
-      </c>
+          <t>SAM, TD/ G1, B3, Terki</t>
+        </is>
+      </c>
+      <c r="G17" s="17" t="n"/>
       <c r="H17" s="17" t="n"/>
     </row>
     <row r="18" ht="21.75" customHeight="1" s="24">
@@ -12709,12 +12709,12 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>MNS, COUR/ section 1, S4, Belhouari</t>
+          <t>MNS, COUR/ section 1, S14, Belhouari</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>SAM, COUR/ section 1, S12, Terki</t>
+          <t>SAM, COUR/ section 1, S6, Terki</t>
         </is>
       </c>
       <c r="D26" s="17" t="n"/>
@@ -12811,12 +12811,12 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>SAM, COUR/ section 1, C2, Terki</t>
+          <t>SAM, COUR/ section 1, S6, Terki</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>Anglais, COUR/ section 1, C2, Hentit N</t>
+          <t>Anglais, COUR/ section 1, S6, Hentit N</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -14111,32 +14111,32 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>ANA2, COUR/ section 2, Amphi2, Mme Ablaoui</t>
+          <t>ANA2, COUR/ section 2, Amphi3, Mme Ablaoui</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>ALG2, COUR/ section 2, Amphi1, M. Medeghri Ahmed</t>
+          <t>ALG2, COUR/ section 2, Amphi4, M. Medeghri Ahmed</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G1, S13, Mme SAIDANI</t>
+          <t>ALG2, TD/ G1, S5, Mme SAIDANI</t>
         </is>
       </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G3, C1, Mme Bendehmane H</t>
+          <t>ANA2, TD/ G3, S11, Mme Bendehmane H</t>
         </is>
       </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G1, B3, BENSALLOUA</t>
+          <t>ASD2, TD/ G1, S9, BENSALLOUA</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G1, C1, M. Kaid</t>
+          <t>ANA2, TD/ G1, S11, M. Kaid</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -14147,22 +14147,22 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G2, C1, Mme Bendehmane H</t>
+          <t>ANA2, TD/ G2, S11, Mme Bendehmane H</t>
         </is>
       </c>
       <c r="E9" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G5, C2, Mme Ablaoui</t>
+          <t>ANA2, TD/ G5, S7, Mme Ablaoui</t>
         </is>
       </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G2, B1, Mme SAIDANI</t>
+          <t>ALG2, TD/ G2, S1, Mme SAIDANI</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G2, S12, BENSALLOUA</t>
+          <t>ASD2, TD/ G2, S6, BENSALLOUA</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -14173,22 +14173,22 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G4, C2, Mme Ablaoui</t>
+          <t>ANA2, TD/ G4, S7, Mme Ablaoui</t>
         </is>
       </c>
       <c r="E10" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G7, S12, M. Ould Ali M</t>
+          <t>ANA2, TD/ G7, S6, M. Ould Ali M</t>
         </is>
       </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G3, B2, Mme TABHARIT</t>
+          <t>ALG2, TD/ G3, S8, Mme TABHARIT</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G4, C2, Mme TABHARIT</t>
+          <t>ALG2, TD/ G4, S7, Mme TABHARIT</t>
         </is>
       </c>
       <c r="H10" s="27" t="n"/>
@@ -14199,18 +14199,18 @@
       <c r="C11" s="31" t="n"/>
       <c r="D11" s="27" t="inlineStr">
         <is>
-          <t>ANA2, TD/ G6, S12, M. Ould Ali M</t>
+          <t>ANA2, TD/ G6, S6, M. Ould Ali M</t>
         </is>
       </c>
       <c r="E11" s="27" t="n"/>
       <c r="F11" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G4, B4, KAID SLIMANE</t>
+          <t>ASD2, TD/ G4, S10, KAID SLIMANE</t>
         </is>
       </c>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G5, S13, KAID SLIMANE</t>
+          <t>ASD2, TD/ G5, S5, KAID SLIMANE</t>
         </is>
       </c>
       <c r="H11" s="27" t="n"/>
@@ -14273,32 +14273,32 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ANA2, COUR/ section 2, Amphi2, Mme Ablaoui</t>
+          <t>ANA2, COUR/ section 2, Amphi3, Mme Ablaoui</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>ASD2, COUR/ section 2, Amphi1, HENNI F</t>
+          <t>ASD2, COUR/ section 2, Amphi4, HENNI F</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G1, B4, HAMAMI</t>
+          <t>SM2, TD/ G1, S10, HAMAMI</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G2, B3, HAMAMI</t>
+          <t>SM2, TD/ G2, S9, HAMAMI</t>
         </is>
       </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>SM2, TD/ G3, B4, HAMAMI</t>
+          <t>SM2, TD/ G3, S10, HAMAMI</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G1, C1, Mme Kaisserli</t>
+          <t>IPSD, TD/ G1, S11, Mme Kaisserli</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -14309,22 +14309,22 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G3, B2, BENSALLOUA</t>
+          <t>ASD2, TD/ G3, S8, BENSALLOUA</t>
         </is>
       </c>
       <c r="E18" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G4, B4, Mme Kaisserli</t>
+          <t>IPSD, TD/ G4, S10, Mme Kaisserli</t>
         </is>
       </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G5, C1, HASSAINE</t>
+          <t>SM2, TD/ G5, S11, HASSAINE</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G5, C2, M. Benyatou Kamel</t>
+          <t>IPSD, TD/ G5, S7, M. Benyatou Kamel</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -14335,22 +14335,22 @@
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G5, B1, Mme TABHARIT</t>
+          <t>ALG2, TD/ G5, S1, Mme TABHARIT</t>
         </is>
       </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G7, B2, Mme TABHARIT</t>
+          <t>ALG2, TD/ G7, S8, Mme TABHARIT</t>
         </is>
       </c>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>ALG2, TD/ G6, B2, Mme TABHARIT</t>
+          <t>ALG2, TD/ G6, S8, Mme TABHARIT</t>
         </is>
       </c>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G6, B4, HASSAINE</t>
+          <t>SM2, TD/ G6, S10, HASSAINE</t>
         </is>
       </c>
       <c r="H19" s="27" t="n"/>
@@ -14361,18 +14361,18 @@
       <c r="C20" s="31" t="n"/>
       <c r="D20" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G6, B3, KAID SLIMANE</t>
+          <t>ASD2, TD/ G6, S9, KAID SLIMANE</t>
         </is>
       </c>
       <c r="E20" s="27" t="n"/>
       <c r="F20" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TD/ G7, B3, HENNI F</t>
+          <t>ASD2, TD/ G7, S9, HENNI F</t>
         </is>
       </c>
       <c r="G20" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G7, S12, Mlle Dj. BENSIKADDOUR</t>
+          <t>IPSD, TD/ G7, S6, Mlle Dj. BENSIKADDOUR</t>
         </is>
       </c>
       <c r="H20" s="27" t="n"/>
@@ -14435,32 +14435,32 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>SM2, COUR/ section 2, Amphi1, HASSAINE</t>
+          <t>SM2, COUR/ section 2, Amphi4, HASSAINE</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>IPSD, COUR/ section 2, Amphi2, Mlle Dj. BENSIKADDOUR</t>
+          <t>IPSD, COUR/ section 2, Amphi3, Mlle Dj. BENSIKADDOUR</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G1, S13, Labdelli</t>
+          <t>PHY2, TD/ G1, S5, Labdelli</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G3, B3, Mme Kaisserli</t>
+          <t>IPSD, TD/ G3, S9, Mme Kaisserli</t>
         </is>
       </c>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G1, A1, BENSALLOUA</t>
+          <t>ASD2, TP/ G1, M3, BENSALLOUA</t>
         </is>
       </c>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G2, A2, BENSALLOUA</t>
+          <t>ASD2, TP/ G2, M2, BENSALLOUA</t>
         </is>
       </c>
       <c r="H26" s="17" t="n"/>
@@ -14471,22 +14471,22 @@
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G2, C2, Mme Kaisserli</t>
+          <t>IPSD, TD/ G2, S7, Mme Kaisserli</t>
         </is>
       </c>
       <c r="E27" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G4, B4, M. Benchehida</t>
+          <t>PHY2, TD/ G4, S10, M. Benchehida</t>
         </is>
       </c>
       <c r="F27" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G2, B2, Labdelli</t>
+          <t>PHY2, TD/ G2, S8, Labdelli</t>
         </is>
       </c>
       <c r="G27" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G3, B4, Labdelli</t>
+          <t>PHY2, TD/ G3, S10, Labdelli</t>
         </is>
       </c>
       <c r="H27" s="27" t="n"/>
@@ -14497,22 +14497,22 @@
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="27" t="inlineStr">
         <is>
-          <t>IPSD, TD/ G6, S12, M. Benyatou Kamel</t>
+          <t>IPSD, TD/ G6, S6, M. Benyatou Kamel</t>
         </is>
       </c>
       <c r="E28" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G5, A3, KAID SLIMANE</t>
+          <t>ASD2, TP/ G5, M1, KAID SLIMANE</t>
         </is>
       </c>
       <c r="F28" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G4, B1, HAMAMI</t>
+          <t>SM2, TD/ G4, S1, HAMAMI</t>
         </is>
       </c>
       <c r="G28" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G4, A3, KAID SLIMANE</t>
+          <t>ASD2, TP/ G4, M1, KAID SLIMANE</t>
         </is>
       </c>
       <c r="H28" s="27" t="n"/>
@@ -14523,18 +14523,18 @@
       <c r="C29" s="31" t="n"/>
       <c r="D29" s="27" t="inlineStr">
         <is>
-          <t>SM2, TD/ G7, C1, HASSAINE</t>
+          <t>SM2, TD/ G7, S11, HASSAINE</t>
         </is>
       </c>
       <c r="E29" s="27" t="n"/>
       <c r="F29" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G5, B3, M. Benchehida</t>
+          <t>PHY2, TD/ G5, S9, M. Benchehida</t>
         </is>
       </c>
       <c r="G29" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G6, C1, M. Benchehida</t>
+          <t>PHY2, TD/ G6, S11, M. Benchehida</t>
         </is>
       </c>
       <c r="H29" s="27" t="n"/>
@@ -14597,28 +14597,28 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>OPM, COUR/ section 2, Amphi2, Mlle Ali Merina.H</t>
+          <t>OPM, COUR/ section 2, Amphi3, Mlle Ali Merina.H</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>TIC, COUR/ section 2, Amphi2, HENNI K.</t>
+          <t>TIC, COUR/ section 2, Amphi3, HENNI K.</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G3, A4, BENSALLOUA</t>
+          <t>ASD2, TP/ G3, C4, BENSALLOUA</t>
         </is>
       </c>
       <c r="E35" s="17" t="n"/>
       <c r="F35" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G1, A2, Mlle Hamou Maamar.M</t>
+          <t>OPM, TP/ G1, M2, Mlle Hamou Maamar.M</t>
         </is>
       </c>
       <c r="G35" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G6, A1, Mlle Ali Merina.H</t>
+          <t>OPM, TP/ G6, M3, Mlle Ali Merina.H</t>
         </is>
       </c>
       <c r="H35" s="17" t="n"/>
@@ -14629,13 +14629,13 @@
       <c r="C36" s="31" t="n"/>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G4, C4, Mlle Ali Merina.H</t>
+          <t>OPM, TP/ G4, A4, Mlle Ali Merina.H</t>
         </is>
       </c>
       <c r="E36" s="27" t="n"/>
       <c r="F36" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G5, A3, Mlle Ali Merina.H</t>
+          <t>OPM, TP/ G5, M1, Mlle Ali Merina.H</t>
         </is>
       </c>
       <c r="G36" s="27" t="n"/>
@@ -14653,7 +14653,7 @@
       <c r="E37" s="27" t="n"/>
       <c r="F37" s="27" t="inlineStr">
         <is>
-          <t>ASD2, TP/ G7, A1, HENNI F</t>
+          <t>ASD2, TP/ G7, M3, HENNI F</t>
         </is>
       </c>
       <c r="G37" s="27" t="n"/>
@@ -14665,7 +14665,7 @@
       <c r="C38" s="31" t="n"/>
       <c r="D38" s="27" t="inlineStr">
         <is>
-          <t>PHY2, TD/ G7, B2, M. Benchehida</t>
+          <t>PHY2, TD/ G7, S8, M. Benchehida</t>
         </is>
       </c>
       <c r="E38" s="27" t="n"/>
@@ -14731,17 +14731,17 @@
       </c>
       <c r="B44" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G2, A1, Mlle Hamou Maamar.M</t>
+          <t>OPM, TP/ G2, M3, Mlle Hamou Maamar.M</t>
         </is>
       </c>
       <c r="C44" s="29" t="inlineStr">
         <is>
-          <t>PHY2, COUR/ section 2, Amphi1, M. Benchehida</t>
+          <t>PHY2, COUR/ section 2, Amphi4, M. Benchehida</t>
         </is>
       </c>
       <c r="D44" s="17" t="inlineStr">
         <is>
-          <t>OPM, TP/ G3, A1, Mlle Hamou Maamar.M</t>
+          <t>OPM, TP/ G3, M3, Mlle Hamou Maamar.M</t>
         </is>
       </c>
       <c r="E44" s="17" t="n"/>
@@ -14753,7 +14753,7 @@
       <c r="A45" s="30" t="n"/>
       <c r="B45" s="27" t="inlineStr">
         <is>
-          <t>OPM, TP/ G7, A2, Mlle Ali Merina.H</t>
+          <t>OPM, TP/ G7, M2, Mlle Ali Merina.H</t>
         </is>
       </c>
       <c r="C45" s="31" t="n"/>
@@ -15946,32 +15946,32 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>TL, COUR/ section 1, Amphi3, BESSAOUD K.</t>
+          <t>TL, COUR/ section 1, Amphi2, BESSAOUD K.</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>SE1, COUR/ section 1, Amphi2, KENNICHE A.</t>
+          <t>SE1, COUR/ section 1, Amphi3, KENNICHE A.</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>TL, TD/ G1, S14, MIDOUN M.</t>
+          <t>TL, TD/ G1, S4, MIDOUN M.</t>
         </is>
       </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>TL, TD/ G5, S13, BESNASSI</t>
+          <t>TL, TD/ G5, S5, BESNASSI</t>
         </is>
       </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>SE1, TD/ G1, S13, BOUZEBIBA</t>
+          <t>SE1, TD/ G1, S5, BOUZEBIBA</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>BDD, TD/ G1, S5, MIROUD</t>
+          <t>BDD, TD/ G1, S16, MIROUD</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -15982,22 +15982,22 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G2, S5, BOUZEBIBA</t>
+          <t>SE1, TD/ G2, S16, BOUZEBIBA</t>
         </is>
       </c>
       <c r="E9" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G6, S15, KHIAT</t>
+          <t>SE1, TD/ G6, S3, KHIAT</t>
         </is>
       </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G2, C1, MIDOUN M.</t>
+          <t>TL, TD/ G2, S11, MIDOUN M.</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G2, S6, MENAD</t>
+          <t>BDD, TD/ G2, S15, MENAD</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -16008,22 +16008,22 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G3, S6, DJAHAFI</t>
+          <t>SE1, TD/ G3, S15, DJAHAFI</t>
         </is>
       </c>
       <c r="E10" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G8, S14, BESSAOUD K.</t>
+          <t>TL, TD/ G8, S4, BESSAOUD K.</t>
         </is>
       </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G4, S14, DJAHAFI</t>
+          <t>SE1, TD/ G4, S4, DJAHAFI</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G3, S14, MIDOUN M.</t>
+          <t>TL, TD/ G3, S4, MIDOUN M.</t>
         </is>
       </c>
       <c r="H10" s="27" t="n"/>
@@ -16034,22 +16034,22 @@
       <c r="C11" s="31" t="n"/>
       <c r="D11" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G4, S15, BESNASSI</t>
+          <t>TL, TD/ G4, S3, BESNASSI</t>
         </is>
       </c>
       <c r="E11" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G9, S4, KENNICHE A.</t>
+          <t>SE1, TD/ G9, S2, KENNICHE A.</t>
         </is>
       </c>
       <c r="F11" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G6, C2, BESNASSI</t>
+          <t>TL, TD/ G6, S7, BESNASSI</t>
         </is>
       </c>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G5, S15, KHIAT</t>
+          <t>SE1, TD/ G5, S3, KHIAT</t>
         </is>
       </c>
       <c r="H11" s="27" t="n"/>
@@ -16060,18 +16060,18 @@
       <c r="C12" s="31" t="n"/>
       <c r="D12" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G7, S4, BESSAOUD K.</t>
+          <t>TL, TD/ G7, S2, BESSAOUD K.</t>
         </is>
       </c>
       <c r="E12" s="27" t="n"/>
       <c r="F12" s="27" t="inlineStr">
         <is>
-          <t>TL, TD/ G9, S12, BESSAOUD K.</t>
+          <t>TL, TD/ G9, S6, BESSAOUD K.</t>
         </is>
       </c>
       <c r="G12" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G7, S4, KENNICHE A.</t>
+          <t>SE1, TD/ G7, S2, KENNICHE A.</t>
         </is>
       </c>
       <c r="H12" s="27" t="n"/>
@@ -16124,27 +16124,27 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>BDD, COUR/ section 1, Amphi3, MAGHNI SANDID Z.</t>
+          <t>BDD, COUR/ section 1, Amphi2, MAGHNI SANDID Z.</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>RÉS, COUR/ section 1, Amphi2, LAREDJ A. M</t>
+          <t>RÉS, COUR/ section 1, Amphi3, LAREDJ A. M</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G1, S13, BOUZEBIBA</t>
+          <t>RÉS, TD/ G1, S5, BOUZEBIBA</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G2, S12, BOUZEBIBA</t>
+          <t>RÉS, TD/ G2, S6, BOUZEBIBA</t>
         </is>
       </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>TL, TP/ G1, A4, MIDOUN M.</t>
+          <t>TL, TP/ G1, C4, MIDOUN M.</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
@@ -16160,22 +16160,22 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G3, C2, MENAD</t>
+          <t>BDD, TD/ G3, S7, MENAD</t>
         </is>
       </c>
       <c r="E18" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G4, C1, MENAD</t>
+          <t>BDD, TD/ G4, S11, MENAD</t>
         </is>
       </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G3, S12, BOUZEBIBA</t>
+          <t>RÉS, TD/ G3, S6, BOUZEBIBA</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G2, A2, MIDOUN M.</t>
+          <t>TL, TP/ G2, M2, MIDOUN M.</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -16186,12 +16186,12 @@
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G5, S12, MAGHNI SANDID Z.</t>
+          <t>BDD, TD/ G5, S6, MAGHNI SANDID Z.</t>
         </is>
       </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G6, C2, MAGHNI SANDID Z.</t>
+          <t>BDD, TD/ G6, S7, MAGHNI SANDID Z.</t>
         </is>
       </c>
       <c r="F19" s="27" t="inlineStr">
@@ -16201,7 +16201,7 @@
       </c>
       <c r="G19" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G5, A3, BESNASSI</t>
+          <t>TL, TP/ G5, M1, BESNASSI</t>
         </is>
       </c>
       <c r="H19" s="27" t="n"/>
@@ -16212,22 +16212,22 @@
       <c r="C20" s="31" t="n"/>
       <c r="D20" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G7, S14, LAREDJ A. M</t>
+          <t>RÉS, TD/ G7, S4, LAREDJ A. M</t>
         </is>
       </c>
       <c r="E20" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G9, S13, LAREDJ A. M</t>
+          <t>RÉS, TD/ G9, S5, LAREDJ A. M</t>
         </is>
       </c>
       <c r="F20" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G7, C2, MAGHNI SANDID Z.</t>
+          <t>BDD, TD/ G7, S7, MAGHNI SANDID Z.</t>
         </is>
       </c>
       <c r="G20" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G7, A4, BESSAOUD K.</t>
+          <t>TL, TP/ G7, C4, BESSAOUD K.</t>
         </is>
       </c>
       <c r="H20" s="27" t="n"/>
@@ -16238,18 +16238,18 @@
       <c r="C21" s="31" t="n"/>
       <c r="D21" s="27" t="inlineStr">
         <is>
-          <t>SE1, TD/ G8, C1, KENNICHE A.</t>
+          <t>SE1, TD/ G8, S11, KENNICHE A.</t>
         </is>
       </c>
       <c r="E21" s="27" t="n"/>
       <c r="F21" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G8, C4, BESSAOUD K.</t>
+          <t>TL, TP/ G8, A4, BESSAOUD K.</t>
         </is>
       </c>
       <c r="G21" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G8, S13, LAREDJ A. M</t>
+          <t>RÉS, TD/ G8, S5, LAREDJ A. M</t>
         </is>
       </c>
       <c r="H21" s="27" t="n"/>
@@ -16302,32 +16302,32 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>POO, COUR/ section 1, Amphi2, ABID M.</t>
+          <t>POO, COUR/ section 1, Amphi3, ABID M.</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>DAW, COUR/ section 1, Amphi3, SEHABA K.</t>
+          <t>DAW, COUR/ section 1, Amphi2, SEHABA K.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>TL, TP/ G3, A1, MIDOUN M.</t>
+          <t>TL, TP/ G3, M3, MIDOUN M.</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>BDD, TP/ G1, C4, MEROUFEL B.</t>
+          <t>BDD, TP/ G1, A4, MEROUFEL B.</t>
         </is>
       </c>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>SE1, TP/ G3, A2, HENNI K</t>
+          <t>SE1, TP/ G3, M2, HENNI K</t>
         </is>
       </c>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>BDD, TP/ G2, C4, MEROUFEL B.</t>
+          <t>BDD, TP/ G2, A4, MEROUFEL B.</t>
         </is>
       </c>
       <c r="H26" s="17" t="n"/>
@@ -16338,22 +16338,22 @@
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G4, S15, BOUZEBIBA</t>
+          <t>RÉS, TD/ G4, S3, BOUZEBIBA</t>
         </is>
       </c>
       <c r="E27" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G2, A4, HENNI K</t>
+          <t>SE1, TP/ G2, C4, HENNI K</t>
         </is>
       </c>
       <c r="F27" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G4, A3, DJAHAFI</t>
+          <t>SE1, TP/ G4, M1, DJAHAFI</t>
         </is>
       </c>
       <c r="G27" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G3, M1, BETOUATI</t>
+          <t>BDD, TP/ G3, A3, BETOUATI</t>
         </is>
       </c>
       <c r="H27" s="27" t="n"/>
@@ -16364,22 +16364,22 @@
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G6, A2, BESNASSI</t>
+          <t>TL, TP/ G6, M2, BESNASSI</t>
         </is>
       </c>
       <c r="E28" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G5, C1, BOUZEBIBA</t>
+          <t>RÉS, TD/ G5, S11, BOUZEBIBA</t>
         </is>
       </c>
       <c r="F28" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TD/ G6, C1, BOUZEBIBA</t>
+          <t>RÉS, TD/ G6, S11, BOUZEBIBA</t>
         </is>
       </c>
       <c r="G28" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G5, A4, DJAHAFI</t>
+          <t>SE1, TP/ G5, C4, DJAHAFI</t>
         </is>
       </c>
       <c r="H28" s="27" t="n"/>
@@ -16390,7 +16390,7 @@
       <c r="C29" s="31" t="n"/>
       <c r="D29" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G8, S14, MAGHNI SANDID Z.</t>
+          <t>BDD, TD/ G8, S4, MAGHNI SANDID Z.</t>
         </is>
       </c>
       <c r="E29" s="27" t="inlineStr">
@@ -16400,12 +16400,12 @@
       </c>
       <c r="F29" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G8, A4, KENNICHE A.</t>
+          <t>SE1, TP/ G8, C4, KENNICHE A.</t>
         </is>
       </c>
       <c r="G29" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G7, M2, MIROUD</t>
+          <t>BDD, TP/ G7, A2, MIROUD</t>
         </is>
       </c>
       <c r="H29" s="27" t="n"/>
@@ -16416,13 +16416,13 @@
       <c r="C30" s="31" t="n"/>
       <c r="D30" s="27" t="inlineStr">
         <is>
-          <t>TL, TP/ G9, A3, BESSAOUD K.</t>
+          <t>TL, TP/ G9, M1, BESSAOUD K.</t>
         </is>
       </c>
       <c r="E30" s="27" t="n"/>
       <c r="F30" s="27" t="inlineStr">
         <is>
-          <t>BDD, TD/ G9, B4, MAGHNI SANDID Z.</t>
+          <t>BDD, TD/ G9, S10, MAGHNI SANDID Z.</t>
         </is>
       </c>
       <c r="G30" s="27" t="inlineStr">
@@ -16480,22 +16480,22 @@
       </c>
       <c r="B35" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G1, A4,  MOUSSA M.</t>
+          <t>RÉS, TP/ G1, C4,  MOUSSA M.</t>
         </is>
       </c>
       <c r="C35" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G2, A3,  MOUSSA M.</t>
+          <t>RÉS, TP/ G2, M1,  MOUSSA M.</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>POO, TP/ G4, M3, ABID M.</t>
+          <t>POO, TP/ G4, A1, ABID M.</t>
         </is>
       </c>
       <c r="E35" s="17" t="inlineStr">
         <is>
-          <t>DAW, TP/ G1, A3, HENNI K</t>
+          <t>DAW, TP/ G1, M1, HENNI K</t>
         </is>
       </c>
       <c r="F35" s="17" t="inlineStr">
@@ -16505,7 +16505,7 @@
       </c>
       <c r="G35" s="17" t="inlineStr">
         <is>
-          <t>POO, TP/ G2, A3, BETOUATI</t>
+          <t>POO, TP/ G2, M1, BETOUATI</t>
         </is>
       </c>
       <c r="H35" s="17" t="n"/>
@@ -16519,22 +16519,22 @@
       </c>
       <c r="C36" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G4, A4, BENHAMED</t>
+          <t>RÉS, TP/ G4, C4, BENHAMED</t>
         </is>
       </c>
       <c r="D36" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G5, M2, BENHAMED</t>
+          <t>RÉS, TP/ G5, A2, BENHAMED</t>
         </is>
       </c>
       <c r="E36" s="27" t="inlineStr">
         <is>
-          <t>POO, TP/ G5, A2, ABID M.</t>
+          <t>POO, TP/ G5, M2, ABID M.</t>
         </is>
       </c>
       <c r="F36" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G2, C4, HENNI K</t>
+          <t>DAW, TP/ G2, A4, HENNI K</t>
         </is>
       </c>
       <c r="G36" s="27" t="inlineStr">
@@ -16548,32 +16548,32 @@
       <c r="A37" s="30" t="n"/>
       <c r="B37" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G4, A2, BETOUATI</t>
+          <t>BDD, TP/ G4, M2, BETOUATI</t>
         </is>
       </c>
       <c r="C37" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G5, A1, BETOUATI</t>
+          <t>BDD, TP/ G5, M3, BETOUATI</t>
         </is>
       </c>
       <c r="D37" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G6, M1, BETOUATI</t>
+          <t>BDD, TP/ G6, A3, BETOUATI</t>
         </is>
       </c>
       <c r="E37" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G7, A4, SEHABA K.</t>
+          <t>DAW, TP/ G7, C4, SEHABA K.</t>
         </is>
       </c>
       <c r="F37" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G6, A4, BENHAMED</t>
+          <t>RÉS, TP/ G6, C4, BENHAMED</t>
         </is>
       </c>
       <c r="G37" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G5, C4, SEHABA K.</t>
+          <t>DAW, TP/ G5, A4, SEHABA K.</t>
         </is>
       </c>
       <c r="H37" s="27" t="n"/>
@@ -16582,7 +16582,7 @@
       <c r="A38" s="30" t="n"/>
       <c r="B38" s="27" t="inlineStr">
         <is>
-          <t>SE1, TP/ G6, A1, DJAHAFI</t>
+          <t>SE1, TP/ G6, M3, DJAHAFI</t>
         </is>
       </c>
       <c r="C38" s="27" t="inlineStr">
@@ -16594,12 +16594,12 @@
       <c r="E38" s="27" t="n"/>
       <c r="F38" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G8, M1, SEHABA K.</t>
+          <t>DAW, TP/ G8, A3, SEHABA K.</t>
         </is>
       </c>
       <c r="G38" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G7, A2, BENHAMED</t>
+          <t>RÉS, TP/ G7, M2, BENHAMED</t>
         </is>
       </c>
       <c r="H38" s="27" t="n"/>
@@ -16608,12 +16608,12 @@
       <c r="A39" s="30" t="n"/>
       <c r="B39" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G8, A3, MIROUD</t>
+          <t>BDD, TP/ G8, M1, MIROUD</t>
         </is>
       </c>
       <c r="C39" s="27" t="inlineStr">
         <is>
-          <t>BDD, TP/ G9, A2, MIROUD</t>
+          <t>BDD, TP/ G9, M2, MIROUD</t>
         </is>
       </c>
       <c r="D39" s="27" t="n"/>
@@ -16621,7 +16621,7 @@
       <c r="F39" s="27" t="n"/>
       <c r="G39" s="27" t="inlineStr">
         <is>
-          <t>POO, TP/ G8, A4, ABID M.</t>
+          <t>POO, TP/ G8, C4, ABID M.</t>
         </is>
       </c>
       <c r="H39" s="27" t="n"/>
@@ -16674,22 +16674,22 @@
       </c>
       <c r="B44" s="17" t="inlineStr">
         <is>
-          <t>POO, TP/ G3, A4, BETOUATI</t>
+          <t>POO, TP/ G3, C4, BETOUATI</t>
         </is>
       </c>
       <c r="C44" s="17" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G9, A1, BENHAMED</t>
+          <t>RÉS, TP/ G9, M3, BENHAMED</t>
         </is>
       </c>
       <c r="D44" s="17" t="inlineStr">
         <is>
-          <t>POO, TP/ G9, A2, ABID M.</t>
+          <t>POO, TP/ G9, M2, ABID M.</t>
         </is>
       </c>
       <c r="E44" s="17" t="inlineStr">
         <is>
-          <t>DAW, TP/ G9, A1, SEHABA K.</t>
+          <t>DAW, TP/ G9, M3, SEHABA K.</t>
         </is>
       </c>
       <c r="F44" s="17" t="n"/>
@@ -16700,7 +16700,7 @@
       <c r="A45" s="30" t="n"/>
       <c r="B45" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G4, C4, HENNI K</t>
+          <t>DAW, TP/ G4, A4, HENNI K</t>
         </is>
       </c>
       <c r="C45" s="27" t="n"/>
@@ -16714,7 +16714,7 @@
       <c r="A46" s="30" t="n"/>
       <c r="B46" s="27" t="inlineStr">
         <is>
-          <t>DAW, TP/ G6, M1, SEHABA K.</t>
+          <t>DAW, TP/ G6, A3, SEHABA K.</t>
         </is>
       </c>
       <c r="C46" s="27" t="n"/>
@@ -16742,7 +16742,7 @@
       <c r="A48" s="30" t="n"/>
       <c r="B48" s="27" t="inlineStr">
         <is>
-          <t>RÉS, TP/ G8, A3, BENHAMED</t>
+          <t>RÉS, TP/ G8, M1, BENHAMED</t>
         </is>
       </c>
       <c r="C48" s="27" t="n"/>
@@ -17902,32 +17902,32 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>AP, COUR/ section 1, Amphi4, MECHAOUI M. D.G</t>
+          <t>AP, COUR/ section 1, Amphi1, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>SI, COUR/ section 1, Amphi3, BENIDRIS F.Z</t>
+          <t>SI, COUR/ section 1, Amphi2, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>SI, TD/ G1, S7, BENIDRIS F.Z</t>
+          <t>SI, TD/ G1, S14, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="E8" s="17" t="inlineStr">
         <is>
-          <t>SI, TD/ G5, S5, BENIDRIS F.Z</t>
+          <t>SI, TD/ G5, S16, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G1, S15, HOCINE N.</t>
+          <t>RS, TD/ G1, S3, HOCINE N.</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G1, A1, DELALI A.</t>
+          <t>DSS, TP/ G1, M3, DELALI A.</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -17938,22 +17938,22 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>RS, TD/ G2, S11, HOCINE N.</t>
+          <t>RS, TD/ G2, S13, HOCINE N.</t>
         </is>
       </c>
       <c r="E9" s="27" t="inlineStr">
         <is>
-          <t>RS, TD/ G6, S6, HOCINE N.</t>
+          <t>RS, TD/ G6, S15, HOCINE N.</t>
         </is>
       </c>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G2, A1, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G2, M3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G2, S7, BENIDRIS F.Z</t>
+          <t>SI, TD/ G2, S14, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -17964,17 +17964,17 @@
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G3, A1, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G3, M3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="E10" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G7, A1, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G7, M3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>DSS, TP/ G3, A2, DELALI A.</t>
+          <t>DSS, TP/ G3, M2, DELALI A.</t>
         </is>
       </c>
       <c r="G10" s="27" t="n"/>
@@ -17986,7 +17986,7 @@
       <c r="C11" s="31" t="n"/>
       <c r="D11" s="27" t="inlineStr">
         <is>
-          <t>DSS, TP/ G4, A2, DELALI A.</t>
+          <t>DSS, TP/ G4, M2, DELALI A.</t>
         </is>
       </c>
       <c r="E11" s="27" t="n"/>
@@ -18052,32 +18052,32 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>IA, COUR/ section 1, Amphi4, HOCINE N.</t>
+          <t>IA, COUR/ section 1, Amphi1, HOCINE N.</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>DSS, COUR/ section 1, Amphi3, DELALI A.</t>
+          <t>DSS, COUR/ section 1, Amphi2, DELALI A.</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>AP, TP/ G1, A1, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G1, M3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="E17" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G5, S15, HOCINE N.</t>
+          <t>RS, TD/ G5, S3, HOCINE N.</t>
         </is>
       </c>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>RS, TD/ G3, S14, HOCINE N.</t>
+          <t>RS, TD/ G3, S4, HOCINE N.</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>AP, TP/ G4, C4, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G4, A4, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -18088,22 +18088,22 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>DSS, TP/ G2, A2, DELALI A.</t>
+          <t>DSS, TP/ G2, M2, DELALI A.</t>
         </is>
       </c>
       <c r="E18" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G6, S14, BENIDRIS F.Z</t>
+          <t>SI, TD/ G6, S4, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G4, S13, BENIDRIS F.Z</t>
+          <t>SI, TD/ G4, S5, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>DSS, TP/ G5, M1, DELALI A.</t>
+          <t>DSS, TP/ G5, A3, DELALI A.</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -18114,17 +18114,17 @@
       <c r="C19" s="31" t="n"/>
       <c r="D19" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G3, S15, BENIDRIS F.Z</t>
+          <t>SI, TD/ G3, S3, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="E19" s="27" t="inlineStr">
         <is>
-          <t>DSS, TP/ G7, A3, DELALI A.</t>
+          <t>DSS, TP/ G7, M1, DELALI A.</t>
         </is>
       </c>
       <c r="F19" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G5, M1, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G5, A3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="G19" s="27" t="n"/>
@@ -18136,7 +18136,7 @@
       <c r="C20" s="31" t="n"/>
       <c r="D20" s="27" t="inlineStr">
         <is>
-          <t>RS, TD/ G4, S4, HOCINE N.</t>
+          <t>RS, TD/ G4, S2, HOCINE N.</t>
         </is>
       </c>
       <c r="E20" s="27" t="n"/>
@@ -18202,28 +18202,28 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>CDS, COUR/ section 1, Amphi3, MIDOUN M.</t>
+          <t>CDS, COUR/ section 1, Amphi2, MIDOUN M.</t>
         </is>
       </c>
       <c r="C26" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G1, A2, HOCINE N.</t>
+          <t>IA, TP/ G1, M2, HOCINE N.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>DSS, TP/ G6, A4, DELALI A.</t>
+          <t>DSS, TP/ G6, C4, DELALI A.</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G2, M1, HOCINE N.</t>
+          <t>IA, TP/ G2, A3, HOCINE N.</t>
         </is>
       </c>
       <c r="F26" s="17" t="n"/>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G3, M3, HOCINE N.</t>
+          <t>IA, TP/ G3, A1, HOCINE N.</t>
         </is>
       </c>
       <c r="H26" s="17" t="n"/>
@@ -18233,12 +18233,12 @@
       <c r="B27" s="31" t="n"/>
       <c r="C27" s="27" t="inlineStr">
         <is>
-          <t>AP, TP/ G6, A1, MECHAOUI M. D.G</t>
+          <t>AP, TP/ G6, M3, MECHAOUI M. D.G</t>
         </is>
       </c>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>RS, TD/ G7, S4, HOCINE N.</t>
+          <t>RS, TD/ G7, S2, HOCINE N.</t>
         </is>
       </c>
       <c r="E27" s="27" t="n"/>
@@ -18251,7 +18251,7 @@
       <c r="B28" s="31" t="n"/>
       <c r="C28" s="27" t="inlineStr">
         <is>
-          <t>SI, TD/ G7, B1, BENIDRIS F.Z</t>
+          <t>SI, TD/ G7, S1, BENIDRIS F.Z</t>
         </is>
       </c>
       <c r="D28" s="27" t="n"/>
@@ -18328,12 +18328,12 @@
       </c>
       <c r="B35" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G4, C4, HOCINE N.</t>
+          <t>IA, TP/ G4, A4, HOCINE N.</t>
         </is>
       </c>
       <c r="C35" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G5, C4, HOCINE N.</t>
+          <t>IA, TP/ G5, A4, HOCINE N.</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -18344,7 +18344,7 @@
       </c>
       <c r="F35" s="17" t="inlineStr">
         <is>
-          <t>IA, TP/ G7, M2, HOCINE N.</t>
+          <t>IA, TP/ G7, A2, HOCINE N.</t>
         </is>
       </c>
       <c r="G35" s="17" t="n"/>
@@ -19633,28 +19633,28 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>ANA4, COUR/ section 1, S16, Mme Limam</t>
+          <t>ANA4, COUR/ section 1, S1, Mme Limam</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>ALG4, COUR/ section 1, S16, M.Ould ali</t>
+          <t>ALG4, COUR/ section 1, S3, M.Ould ali</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G1, S10, Mme Limam</t>
+          <t>ANA4, TD/ G1, S12, Mme Limam</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ALG4, TD/ G1, S5, M.Ould ali</t>
+          <t>ALG4, TD/ G1, S16, M.Ould ali</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>AC, TD/ G1, S11, Mlle Amina FERRAOUN</t>
+          <t>AC, TD/ G1, S13, Mlle Amina FERRAOUN</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -19665,18 +19665,18 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>ALG4, TD/ G2, S9, M.Ould ali</t>
+          <t>ALG4, TD/ G2, C2, M.Ould ali</t>
         </is>
       </c>
       <c r="E9" s="27" t="n"/>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G2, S4, Mme Limam</t>
+          <t>ANA4, TD/ G2, S2, Mme Limam</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>ANUM2, TD/ G2, S10, M. Belhamiti Omar</t>
+          <t>ANUM2, TD/ G2, S12, M. Belhamiti Omar</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -19759,28 +19759,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ANA4, COUR/ section 1, S16, Mme Limam</t>
+          <t>ANA4, COUR/ section 1, S1, Mme Limam</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>AC, COUR/ section 1, S16, Mlle Amina FERRAOUN</t>
+          <t>AC, COUR/ section 1, S3, Mlle Amina FERRAOUN</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G1, S5, Mme Limam</t>
+          <t>ANA4, TD/ G1, S16, Mme Limam</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>ANUM2, TD/ G1, S4, M. Belhamiti Omar</t>
+          <t>ANUM2, TD/ G1, S2, M. Belhamiti Omar</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>PROBA, TD/ G1, S14, M. Mohammedi Mustapha</t>
+          <t>PROBA, TD/ G1, S4, M. Mohammedi Mustapha</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -19791,18 +19791,18 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>AC, TD/ G2, S6, Mlle Amina FERRAOUN</t>
+          <t>AC, TD/ G2, S15, Mlle Amina FERRAOUN</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>ANA4, TD/ G2, S15, Mme Limam</t>
+          <t>ANA4, TD/ G2, S3, Mme Limam</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>GÉOMÉ, TD/ G2, S15, Mme Bendahmane Hafida</t>
+          <t>GÉOMÉ, TD/ G2, S3, Mme Bendahmane Hafida</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -19885,17 +19885,17 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>AC, COUR/ section 1, S16, Mlle Amina FERRAOUN</t>
+          <t>AC, COUR/ section 1, S3, Mlle Amina FERRAOUN</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>ANUM2, COUR/ section 1, S16, M. Belhamiti Omar</t>
+          <t>ANUM2, COUR/ section 1, S3, M. Belhamiti Omar</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>GÉOMÉ, TD/ G1, S6, Mme Bendahmane Hafida</t>
+          <t>GÉOMÉ, TD/ G1, S15, Mme Bendahmane Hafida</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
@@ -19909,7 +19909,7 @@
       <c r="C27" s="31" t="n"/>
       <c r="D27" s="27" t="inlineStr">
         <is>
-          <t>PROBA, TD/ G2, S5, M. Mohammedi Mustapha</t>
+          <t>PROBA, TD/ G2, S16, M. Mohammedi Mustapha</t>
         </is>
       </c>
       <c r="E27" s="27" t="n"/>
@@ -19995,12 +19995,12 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>PROBA, COUR/ section 1, S16, M. Mohammedi Mustapha</t>
+          <t>PROBA, COUR/ section 1, S1, M. Mohammedi Mustapha</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>GÉOMÉ, COUR/ section 1, S16, Mme Bendahmane Hafida</t>
+          <t>GÉOMÉ, COUR/ section 1, S1, Mme Bendahmane Hafida</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -20097,7 +20097,7 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>APsciences, COUR/ section 1, S16, M. Ghezzar Med</t>
+          <t>APsciences, COUR/ section 1, S1, M. Ghezzar Med</t>
         </is>
       </c>
       <c r="C44" s="17" t="n"/>
@@ -21300,7 +21300,7 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>TOL, COUR/ section 1, S2, M. Menad Abdallah</t>
+          <t>TOL, COUR/ section 1, S3, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
@@ -21310,18 +21310,18 @@
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>TOL, TD/ G1, S8, M. Menad Abdallah</t>
+          <t>TOL, TD/ G1, C1, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>EDP, TD/ G1, S7, Mme Belmouhoub-Ould ali</t>
+          <t>EDP, TD/ G1, S14, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>TRAL, TD/ G1, S9, M. Andasmas M</t>
+          <t>TRAL, TD/ G1, C2, M. Andasmas M</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -21332,18 +21332,18 @@
       <c r="C9" s="31" t="n"/>
       <c r="D9" s="27" t="inlineStr">
         <is>
-          <t>EDP, TD/ G2, S16, Mme Belmouhoub-Ould ali</t>
+          <t>EDP, TD/ G2, B4, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
       <c r="E9" s="27" t="n"/>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>TOL, TD/ G2, S6, M. Menad Abdallah</t>
+          <t>TOL, TD/ G2, S15, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
         <is>
-          <t>Géo. Diff, TD/ G2, S8, M. Fettouch Houari</t>
+          <t>Géo. Diff, TD/ G2, C1, M. Fettouch Houari</t>
         </is>
       </c>
       <c r="H9" s="27" t="n"/>
@@ -21426,7 +21426,7 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>TOL, COUR/ section 1, S2, M. Menad Abdallah</t>
+          <t>TOL, COUR/ section 1, S3, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
@@ -21436,18 +21436,18 @@
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>TOL, TD/ G1, S7, M. Menad Abdallah</t>
+          <t>TOL, TD/ G1, S14, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>EDP, TD/ G1, S6, Mme Belmouhoub-Ould ali</t>
+          <t>EDP, TD/ G1, S15, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>Géo. Diff, TD/ G1, S5, M. Fettouch Houari</t>
+          <t>Géo. Diff, TD/ G1, S16, M. Fettouch Houari</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -21458,18 +21458,18 @@
       <c r="C18" s="31" t="n"/>
       <c r="D18" s="27" t="inlineStr">
         <is>
-          <t>EDP, TD/ G2, S11, Mme Belmouhoub-Ould ali</t>
+          <t>EDP, TD/ G2, S13, Mme Belmouhoub-Ould ali</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>TOL, TD/ G2, S5, M. Menad Abdallah</t>
+          <t>TOL, TD/ G2, S16, M. Menad Abdallah</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>TRAL, TD/ G2, S4, M. Andasmas M</t>
+          <t>TRAL, TD/ G2, S2, M. Andasmas M</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -21654,12 +21654,12 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>TRAL, COUR/ section 1, S2, Mme Limam</t>
+          <t>TRAL, COUR/ section 1, S3, Mme Limam</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>Géo. Diff, COUR/ section 1, S2, M. BELARBI Lakehal</t>
+          <t>Géo. Diff, COUR/ section 1, S3, M. BELARBI Lakehal</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
@@ -21756,7 +21756,7 @@
       </c>
       <c r="B44" s="29" t="inlineStr">
         <is>
-          <t>ETHrecherche, COUR/ section 1, S2, M. Kaid Med</t>
+          <t>ETHrecherche, COUR/ section 1, S3, M. Kaid Med</t>
         </is>
       </c>
       <c r="C44" s="17" t="n"/>
@@ -22959,28 +22959,28 @@
       </c>
       <c r="B8" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G1, B1, KHIAT</t>
+          <t>AOSI, TD/ G1, S8, KHIAT</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>AOSI, COUR/ section 1, Amphi4, KHELIFA N.</t>
+          <t>AOSI, COUR/ section 1, Amphi1, KHELIFA N.</t>
         </is>
       </c>
       <c r="D8" s="29" t="inlineStr">
         <is>
-          <t>ALOS, COUR/ section 1, Amphi1, MOUSSA M.</t>
+          <t>ALOS, COUR/ section 1, Amphi4, MOUSSA M.</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G1, A3, MOUSSA M.</t>
+          <t>ALOS, TP/ G1, M1, MOUSSA M.</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>SSI, TP/ G1, A4, BENTAOUZA C</t>
+          <t>SSI, TP/ G1, C4, BENTAOUZA C</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -22989,7 +22989,7 @@
       <c r="A9" s="30" t="n"/>
       <c r="B9" s="27" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G2, A1, MOUSSA M.</t>
+          <t>ALOS, TP/ G2, M3, MOUSSA M.</t>
         </is>
       </c>
       <c r="C9" s="31" t="n"/>
@@ -22997,7 +22997,7 @@
       <c r="E9" s="27" t="n"/>
       <c r="F9" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G2, S11, KHIAT</t>
+          <t>AOSI, TD/ G2, S13, KHIAT</t>
         </is>
       </c>
       <c r="G9" s="27" t="inlineStr">
@@ -23011,7 +23011,7 @@
       <c r="A10" s="30" t="n"/>
       <c r="B10" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G3, B2, KHELIFA N.</t>
+          <t>AOSI, TD/ G3, S9, KHELIFA N.</t>
         </is>
       </c>
       <c r="C10" s="31" t="n"/>
@@ -23019,12 +23019,12 @@
       <c r="E10" s="27" t="n"/>
       <c r="F10" s="27" t="inlineStr">
         <is>
-          <t>SSI, TP/ G3, A4, BENTAOUZA C</t>
+          <t>SSI, TP/ G3, C4, BENTAOUZA C</t>
         </is>
       </c>
       <c r="G10" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G3, A2, KHELIFA N.</t>
+          <t>AOSI, TP/ G3, M2, KHELIFA N.</t>
         </is>
       </c>
       <c r="H10" s="27" t="n"/>
@@ -23033,7 +23033,7 @@
       <c r="A11" s="30" t="n"/>
       <c r="B11" s="27" t="inlineStr">
         <is>
-          <t>SSI, TP/ G4, A2, BENTAOUZA C</t>
+          <t>SSI, TP/ G4, M2, BENTAOUZA C</t>
         </is>
       </c>
       <c r="C11" s="31" t="n"/>
@@ -23041,12 +23041,12 @@
       <c r="E11" s="27" t="n"/>
       <c r="F11" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G4, S10, KHELIFA N.</t>
+          <t>AOSI, TD/ G4, S12, KHELIFA N.</t>
         </is>
       </c>
       <c r="G11" s="27" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G4, A3, MOUSSA M.</t>
+          <t>ALOS, TP/ G4, M1, MOUSSA M.</t>
         </is>
       </c>
       <c r="H11" s="27" t="n"/>
@@ -23109,28 +23109,28 @@
       </c>
       <c r="B17" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G1, A1, KHIAT</t>
+          <t>AOSI, TP/ G1, M3, KHIAT</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>SSI, COUR/ section 1, Amphi4, BENTAOUZA C</t>
+          <t>SSI, COUR/ section 1, Amphi1, BENTAOUZA C</t>
         </is>
       </c>
       <c r="D17" s="29" t="inlineStr">
         <is>
-          <t>OWS, COUR/ section 1, Amphi2, DJEBBARA R.</t>
+          <t>OWS, COUR/ section 1, Amphi3, DJEBBARA R.</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>RO, TP/ G1, M3,  MIROUD</t>
+          <t>RO, TP/ G1, A1,  MIROUD</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>FDD, TP/ G1, M2, HABIB ZAHMANI M</t>
+          <t>FDD, TP/ G1, A2, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -23139,7 +23139,7 @@
       <c r="A18" s="30" t="n"/>
       <c r="B18" s="27" t="inlineStr">
         <is>
-          <t>SSI, TP/ G2, A4, BENTAOUZA C</t>
+          <t>SSI, TP/ G2, C4, BENTAOUZA C</t>
         </is>
       </c>
       <c r="C18" s="31" t="n"/>
@@ -23147,12 +23147,12 @@
       <c r="E18" s="27" t="n"/>
       <c r="F18" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G2, M2, KHIAT</t>
+          <t>AOSI, TP/ G2, A2, KHIAT</t>
         </is>
       </c>
       <c r="G18" s="27" t="inlineStr">
         <is>
-          <t>RO, TP/ G3, M3, BAHNES N.</t>
+          <t>RO, TP/ G3, A1, BAHNES N.</t>
         </is>
       </c>
       <c r="H18" s="27" t="n"/>
@@ -23161,7 +23161,7 @@
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="27" t="inlineStr">
         <is>
-          <t>ALOS, TP/ G3, A3, MOUSSA M.</t>
+          <t>ALOS, TP/ G3, M1, MOUSSA M.</t>
         </is>
       </c>
       <c r="C19" s="31" t="n"/>
@@ -23175,7 +23175,7 @@
       <c r="A20" s="30" t="n"/>
       <c r="B20" s="27" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G4, A2, KHELIFA N.</t>
+          <t>AOSI, TP/ G4, M2, KHELIFA N.</t>
         </is>
       </c>
       <c r="C20" s="31" t="n"/>
@@ -23243,27 +23243,27 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>FDD, COUR/ section 1, Amphi4, MOUMEN M.</t>
+          <t>FDD, COUR/ section 1, Amphi1, MOUMEN M.</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>RO, COUR/ section 1, Amphi4, BAHNES N.</t>
+          <t>RO, COUR/ section 1, Amphi1, BAHNES N.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G1, M1, MEROUFEL B.</t>
+          <t>SMA, TP/ G1, A3, MEROUFEL B.</t>
         </is>
       </c>
       <c r="E26" s="17" t="inlineStr">
         <is>
-          <t>FDD, TP/ G3, M2, HABIB ZAHMANI M</t>
+          <t>FDD, TP/ G3, A2, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G2, C4, MEROUFEL B.</t>
+          <t>SMA, TP/ G2, A4, MEROUFEL B.</t>
         </is>
       </c>
       <c r="G26" s="17" t="n"/>
@@ -23293,7 +23293,7 @@
       <c r="C28" s="31" t="n"/>
       <c r="D28" s="27" t="inlineStr">
         <is>
-          <t>RO, TP/ G4, C4, BAHNES N.</t>
+          <t>RO, TP/ G4, A4, BAHNES N.</t>
         </is>
       </c>
       <c r="E28" s="27" t="n"/>
@@ -23369,23 +23369,23 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>GP, COUR/ section 1, Amphi3, DELALI A.</t>
+          <t>GP, COUR/ section 1, Amphi2, DELALI A.</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>SMA, COUR/ section 1, Amphi3, MEROUFEL B.</t>
+          <t>SMA, COUR/ section 1, Amphi2, MEROUFEL B.</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
       <c r="E35" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G3, C4, MEROUFEL B.</t>
+          <t>SMA, TP/ G3, A4, MEROUFEL B.</t>
         </is>
       </c>
       <c r="F35" s="17" t="inlineStr">
         <is>
-          <t>SMA, TP/ G4, M3, MEROUFEL B.</t>
+          <t>SMA, TP/ G4, A1, MEROUFEL B.</t>
         </is>
       </c>
       <c r="G35" s="17" t="n"/>
@@ -24677,28 +24677,28 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>GSR, COUR/ section 1, B3, LAREDJ A.</t>
+          <t>GSR, COUR/ section 1, S10, LAREDJ A.</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>VS, COUR/ section 1, C1, FILALI F.</t>
+          <t>VS, COUR/ section 1, S11, FILALI F.</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>GSR, TD/ G1, S2, LAREDJ A.</t>
+          <t>GSR, TD/ G1, B3, LAREDJ A.</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>RO, TD/ G1, S9, BAHNES N.</t>
+          <t>RO, TD/ G1, C2, BAHNES N.</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>GSR, TP/ G1, C4, LAREDJ A.</t>
+          <t>GSR, TP/ G1, A4, LAREDJ A.</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -24791,17 +24791,17 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>ASBDA, COUR/ section 1, B1, HABIB ZAHMANI M</t>
+          <t>ASBDA, COUR/ section 1, S8, HABIB ZAHMANI M</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>PR, COUR/ section 1, C1, HOCINE N.</t>
+          <t>PR, COUR/ section 1, S11, HOCINE N.</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TD/ G1, S10, KHIAT</t>
+          <t>AOSI, TD/ G1, S12, KHIAT</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
@@ -24897,23 +24897,23 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>SRI, COUR/ section 1, B4, BENTAOUZA C</t>
+          <t>SRI, COUR/ section 1, S10, BENTAOUZA C</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>AOSI, COUR/ section 1, B2, KHELIFA N.</t>
+          <t>AOSI, COUR/ section 1, S8, KHELIFA N.</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>VS, TP/ G1, M2, FILALI F.</t>
+          <t>VS, TP/ G1, A2, FILALI F.</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>SRI, TP/ G1, M1, BENTAOUZA C</t>
+          <t>SRI, TP/ G1, A3, BENTAOUZA C</t>
         </is>
       </c>
       <c r="G26" s="17" t="n"/>
@@ -25007,24 +25007,24 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>RO, COUR/ section 1, B1, BAHNES N.</t>
+          <t>RO, COUR/ section 1, S8, BAHNES N.</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>GP, COUR/ section 1, B1, DELALI A.</t>
+          <t>GP, COUR/ section 1, S8, DELALI A.</t>
         </is>
       </c>
       <c r="D35" s="17" t="n"/>
       <c r="E35" s="17" t="inlineStr">
         <is>
-          <t>AOSI, TP/ G1, M1, KHIAT</t>
+          <t>AOSI, TP/ G1, A3, KHIAT</t>
         </is>
       </c>
       <c r="F35" s="17" t="n"/>
       <c r="G35" s="17" t="inlineStr">
         <is>
-          <t>PR, TP/ G1, M1, HOCINE N.</t>
+          <t>PR, TP/ G1, A3, HOCINE N.</t>
         </is>
       </c>
       <c r="H35" s="17" t="n"/>
@@ -26315,28 +26315,28 @@
       </c>
       <c r="B8" s="29" t="inlineStr">
         <is>
-          <t>AC2, COUR/ section 1, B4, M. BELAIDI Benharrat</t>
+          <t>AC2, COUR/ section 1, S11, M. BELAIDI Benharrat</t>
         </is>
       </c>
       <c r="C8" s="29" t="inlineStr">
         <is>
-          <t>TO2, COUR/ section 1, C2, M. B. BENDOUKHA</t>
+          <t>TO2, COUR/ section 1, S7, M. B. BENDOUKHA</t>
         </is>
       </c>
       <c r="D8" s="17" t="inlineStr">
         <is>
-          <t>AC2, TD/ G1, S3, M. BELAIDI Benharrat</t>
+          <t>AC2, TD/ G1, B2, M. BELAIDI Benharrat</t>
         </is>
       </c>
       <c r="E8" s="17" t="n"/>
       <c r="F8" s="17" t="inlineStr">
         <is>
-          <t>TO2, TD/ G1, S8, M. B. BENDOUKHA</t>
+          <t>TO2, TD/ G1, C1, M. B. BENDOUKHA</t>
         </is>
       </c>
       <c r="G8" s="17" t="inlineStr">
         <is>
-          <t>GéoDiff2, TD/ G1, S16, M. BELARBI Lakehal</t>
+          <t>GéoDiff2, TD/ G1, B4, M. BELARBI Lakehal</t>
         </is>
       </c>
       <c r="H8" s="17" t="n"/>
@@ -26429,28 +26429,28 @@
       </c>
       <c r="B17" s="29" t="inlineStr">
         <is>
-          <t>GéoDiff2, COUR/ section 1, B2, M. BELARBI Lakehal</t>
+          <t>GéoDiff2, COUR/ section 1, S9, M. BELARBI Lakehal</t>
         </is>
       </c>
       <c r="C17" s="29" t="inlineStr">
         <is>
-          <t>Dis2, COUR/ section 1, C2, M. BOUZIT Hamid</t>
+          <t>Dis2, COUR/ section 1, S7, M. BOUZIT Hamid</t>
         </is>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>AC2, TD/ G1, S9, M. BELAIDI Benharrat</t>
+          <t>AC2, TD/ G1, C2, M. BELAIDI Benharrat</t>
         </is>
       </c>
       <c r="E17" s="17" t="n"/>
       <c r="F17" s="17" t="inlineStr">
         <is>
-          <t>GéoDiff2, TD/ G1, S7, M. BELARBI Lakehal</t>
+          <t>GéoDiff2, TD/ G1, S14, M. BELARBI Lakehal</t>
         </is>
       </c>
       <c r="G17" s="17" t="inlineStr">
         <is>
-          <t>Dis2, TD/ G1, S6, M. BOUZIT Hamid</t>
+          <t>Dis2, TD/ G1, S15, M. BOUZIT Hamid</t>
         </is>
       </c>
       <c r="H17" s="17" t="n"/>
@@ -26543,28 +26543,28 @@
       </c>
       <c r="B26" s="29" t="inlineStr">
         <is>
-          <t>EDP2, COUR/ section 1, C1, M. Andasmas M</t>
+          <t>EDP2, COUR/ section 1, S11, M. Andasmas M</t>
         </is>
       </c>
       <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>STAT2, COUR/ section 1, B3, Mlle Dj.BENSIKADDOUR</t>
+          <t>STAT2, COUR/ section 1, S9, Mlle Dj.BENSIKADDOUR</t>
         </is>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>EDP2, TD/ G1, S7, M. Andasmas M</t>
+          <t>EDP2, TD/ G1, S14, M. Andasmas M</t>
         </is>
       </c>
       <c r="E26" s="17" t="n"/>
       <c r="F26" s="17" t="inlineStr">
         <is>
-          <t>STAT2, TD/ G1, C2, Mlle Dj.BENSIKADDOUR</t>
+          <t>STAT2, TD/ G1, S7, Mlle Dj.BENSIKADDOUR</t>
         </is>
       </c>
       <c r="G26" s="17" t="inlineStr">
         <is>
-          <t>SEMIGROUP, TD/ G1, C2, Mlle Medeghri Ahmed</t>
+          <t>SEMIGROUP, TD/ G1, S7, Mlle Medeghri Ahmed</t>
         </is>
       </c>
       <c r="H26" s="17" t="n"/>
@@ -26657,17 +26657,17 @@
       </c>
       <c r="B35" s="29" t="inlineStr">
         <is>
-          <t>SEMIGROUP, COUR/ section 1, B2, Mlle Medeghri Ahmed</t>
+          <t>SEMIGROUP, COUR/ section 1, S9, Mlle Medeghri Ahmed</t>
         </is>
       </c>
       <c r="C35" s="29" t="inlineStr">
         <is>
-          <t>Anglais2, COUR/ section 1, B2, M. Dahmani Z.</t>
+          <t>Anglais2, COUR/ section 1, S9, M. Dahmani Z.</t>
         </is>
       </c>
       <c r="D35" s="17" t="inlineStr">
         <is>
-          <t>EDP2, TD/ G1, B3, M. Andasmas M</t>
+          <t>EDP2, TD/ G1, S9, M. Andasmas M</t>
         </is>
       </c>
       <c r="E35" s="17" t="n"/>

</xml_diff>